<commit_message>
Adding data to calibrate CIN2/CIN3 to HPV16
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="67">
   <si>
     <t>N</t>
   </si>
@@ -201,6 +201,30 @@
   </si>
   <si>
     <t>McDonald 2014</t>
+  </si>
+  <si>
+    <t>CIN2/CIN3 Prevalence HPV16 (HIV+)</t>
+  </si>
+  <si>
+    <t>CIN2/CIN3 Prevalence HPV16 (HIV-)</t>
+  </si>
+  <si>
+    <t>HPV Prevalence in HIV+ Women HPV16</t>
+  </si>
+  <si>
+    <t>HPV Prevalence in HIV- Women HPV16</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Proportion of HPV infections that were HPV16 among women with WNL/CIN1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Proportion of HPV infections that were HPV16 among women with CIN2/CIN3</t>
   </si>
 </sst>
 </file>
@@ -236,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -247,19 +271,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -275,20 +302,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I161" totalsRowShown="0">
-  <autoFilter ref="A1:I161"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K199" totalsRowShown="0">
+  <autoFilter ref="A1:K199"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="Criteria"/>
     <tableColumn id="9" name="Source"/>
     <tableColumn id="2" name="Group"/>
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="2">
-      <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
+    <tableColumn id="4" name="Mean" dataDxfId="0">
+      <calculatedColumnFormula>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="1"/>
-    <tableColumn id="6" name="UB" dataDxfId="0"/>
+    <tableColumn id="5" name="LB" dataDxfId="2"/>
+    <tableColumn id="6" name="UB" dataDxfId="1"/>
+    <tableColumn id="8" name="Column1"/>
+    <tableColumn id="11" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -557,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:K199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="J201" sqref="J201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -569,9 +598,11 @@
     <col min="2" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="5" width="11.81640625" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" customWidth="1"/>
+    <col min="11" max="11" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -599,8 +630,14 @@
       <c r="I1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -620,11 +657,11 @@
         <v>48</v>
       </c>
       <c r="G2">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -644,11 +681,11 @@
         <v>221</v>
       </c>
       <c r="G3">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4298642533936653E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -668,11 +705,11 @@
         <v>243</v>
       </c>
       <c r="G4">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.12757201646090535</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -692,11 +729,11 @@
         <v>175</v>
       </c>
       <c r="G5">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.15428571428571428</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -716,11 +753,11 @@
         <v>407</v>
       </c>
       <c r="G6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>8.1081081081081086E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -740,11 +777,11 @@
         <v>147</v>
       </c>
       <c r="G7">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4421768707482991E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -764,11 +801,11 @@
         <v>76</v>
       </c>
       <c r="G8">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.8947368421052627E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -788,11 +825,11 @@
         <v>28</v>
       </c>
       <c r="G9">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -813,11 +850,11 @@
         <v>13</v>
       </c>
       <c r="G10">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -838,11 +875,11 @@
         <v>13</v>
       </c>
       <c r="G11">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -862,11 +899,11 @@
         <v>191</v>
       </c>
       <c r="G12">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.5706806282722512E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -886,11 +923,11 @@
         <v>693</v>
       </c>
       <c r="G13">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.7417027417027416E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -910,11 +947,11 @@
         <v>662</v>
       </c>
       <c r="G14">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1148036253776436E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -934,11 +971,11 @@
         <v>666</v>
       </c>
       <c r="G15">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.6036036036036036E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -958,8 +995,8 @@
         <v>2272</v>
       </c>
       <c r="G16">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.8609154929577465E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -982,8 +1019,8 @@
         <v>1400</v>
       </c>
       <c r="G17">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.1428571428571431E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1006,8 +1043,8 @@
         <v>982</v>
       </c>
       <c r="G18">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.0549898167006109E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1030,8 +1067,8 @@
         <v>617</v>
       </c>
       <c r="G19">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1069692058346839E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1055,8 +1092,8 @@
         <v>283.5</v>
       </c>
       <c r="G20">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1080,8 +1117,8 @@
         <v>283.5</v>
       </c>
       <c r="G21">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1104,8 +1141,8 @@
         <v>239</v>
       </c>
       <c r="G22">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.16317991631799164</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1128,8 +1165,8 @@
         <v>914</v>
       </c>
       <c r="G23">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.20787746170678337</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1152,8 +1189,8 @@
         <v>905</v>
       </c>
       <c r="G24">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.21878453038674034</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1176,8 +1213,8 @@
         <v>841</v>
       </c>
       <c r="G25">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.14744351961950058</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1200,8 +1237,8 @@
         <v>2679</v>
       </c>
       <c r="G26">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.11534154535274356</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1224,8 +1261,8 @@
         <v>1547</v>
       </c>
       <c r="G27">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>6.1409179056237877E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1248,8 +1285,8 @@
         <v>1058</v>
       </c>
       <c r="G28">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.780718336483932E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1272,8 +1309,8 @@
         <v>645</v>
       </c>
       <c r="G29">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.0155038759689922E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1296,8 +1333,8 @@
         <v>296.5</v>
       </c>
       <c r="G30">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.6981450252951095E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1320,8 +1357,8 @@
         <v>296.5</v>
       </c>
       <c r="G31">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.6981450252951095E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1344,8 +1381,8 @@
         <v>239</v>
       </c>
       <c r="G32">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.16317991631799164</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1368,8 +1405,8 @@
         <v>914</v>
       </c>
       <c r="G33">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.20787746170678337</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1392,8 +1429,8 @@
         <v>905</v>
       </c>
       <c r="G34">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.21878453038674034</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1416,8 +1453,8 @@
         <v>841</v>
       </c>
       <c r="G35">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.14744351961950058</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1440,8 +1477,8 @@
         <v>2679</v>
       </c>
       <c r="G36">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.11534154535274356</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1464,8 +1501,8 @@
         <v>1547</v>
       </c>
       <c r="G37">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>6.1409179056237877E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1488,8 +1525,8 @@
         <v>1058</v>
       </c>
       <c r="G38">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.780718336483932E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1512,8 +1549,8 @@
         <v>645</v>
       </c>
       <c r="G39">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.0155038759689922E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1536,8 +1573,8 @@
         <v>296.5</v>
       </c>
       <c r="G40">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.6981450252951095E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1560,8 +1597,8 @@
         <v>296.5</v>
       </c>
       <c r="G41">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.6981450252951095E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1584,8 +1621,8 @@
         <v>191</v>
       </c>
       <c r="G42">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.58638743455497377</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1608,8 +1645,8 @@
         <v>693</v>
       </c>
       <c r="G43">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.34920634920634919</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1632,8 +1669,8 @@
         <v>662</v>
       </c>
       <c r="G44">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.2175226586102719</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1656,8 +1693,8 @@
         <v>666</v>
       </c>
       <c r="G45">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.16666666666666666</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1680,8 +1717,8 @@
         <v>2272</v>
       </c>
       <c r="G46">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.16461267605633803</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1704,8 +1741,8 @@
         <v>1400</v>
       </c>
       <c r="G47">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.14499999999999999</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1728,8 +1765,8 @@
         <v>982</v>
       </c>
       <c r="G48">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.10183299389002037</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -1752,8 +1789,8 @@
         <v>617</v>
       </c>
       <c r="G49" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.14424635332252836</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1778,8 +1815,8 @@
         <v>283.5</v>
       </c>
       <c r="G50" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.13227513227513227</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1804,8 +1841,8 @@
         <v>283.5</v>
       </c>
       <c r="G51" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.13227513227513227</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -1828,8 +1865,8 @@
         <v>8</v>
       </c>
       <c r="G52" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.75</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H52" s="1">
         <v>0.44993750650906073</v>
@@ -1856,8 +1893,8 @@
         <v>63</v>
       </c>
       <c r="G53" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.61904761904761907</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H53" s="1">
         <v>0.49912995181888981</v>
@@ -1884,8 +1921,8 @@
         <v>66</v>
       </c>
       <c r="G54" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.5</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H54" s="1">
         <v>0.37937033884025395</v>
@@ -1912,8 +1949,8 @@
         <v>21</v>
       </c>
       <c r="G55" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.2857142857142857</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H55" s="1">
         <v>9.2495929098426521E-2</v>
@@ -1940,8 +1977,8 @@
         <v>35</v>
       </c>
       <c r="G56" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.42857142857142855</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H56" s="1">
         <v>0.26462021631607502</v>
@@ -1968,8 +2005,8 @@
         <v>93</v>
       </c>
       <c r="G57" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.23655913978494625</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H57" s="1">
         <v>0.15018730143155551</v>
@@ -1996,8 +2033,8 @@
         <v>101</v>
       </c>
       <c r="G58" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.21782178217821782</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H58" s="1">
         <v>0.13732122306748479</v>
@@ -2024,8 +2061,8 @@
         <v>84</v>
       </c>
       <c r="G59" s="1">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.19047619047619047</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H59" s="1">
         <v>0.10650088546422966</v>
@@ -2054,8 +2091,8 @@
         <v>5624</v>
       </c>
       <c r="G60">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.0135135135135136E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -2078,8 +2115,8 @@
         <v>5141</v>
       </c>
       <c r="G61">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>8.8504182065745965E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -2102,8 +2139,8 @@
         <v>3643</v>
       </c>
       <c r="G62">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.28191051331320338</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2126,8 +2163,8 @@
         <v>2773</v>
       </c>
       <c r="G63">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.45185719437432381</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2150,8 +2187,8 @@
         <v>1956</v>
       </c>
       <c r="G64">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3721881390593047</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -2174,8 +2211,8 @@
         <v>1638</v>
       </c>
       <c r="G65">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.26923076923076922</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -2198,8 +2235,8 @@
         <v>1362</v>
       </c>
       <c r="G66">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.22687224669603523</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -2222,8 +2259,8 @@
         <v>5624</v>
       </c>
       <c r="G67">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.3157894736842105E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -2246,8 +2283,8 @@
         <v>5141</v>
       </c>
       <c r="G68">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.10095312196070803</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -2270,8 +2307,8 @@
         <v>3643</v>
       </c>
       <c r="G69">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.33324183365358223</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -2294,8 +2331,8 @@
         <v>2773</v>
       </c>
       <c r="G70" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.44825099170573385</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
@@ -2320,8 +2357,8 @@
         <v>1956</v>
       </c>
       <c r="G71" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3614519427402863</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
@@ -2346,8 +2383,8 @@
         <v>1638</v>
       </c>
       <c r="G72" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.32173382173382176</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
@@ -2372,8 +2409,8 @@
         <v>1362</v>
       </c>
       <c r="G73" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.20851688693098386</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
@@ -2398,8 +2435,8 @@
         <v>5624</v>
       </c>
       <c r="G74" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.2901849217638691E-3</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
@@ -2424,8 +2461,8 @@
         <v>5141</v>
       </c>
       <c r="G75" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>9.0643843610192565E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
@@ -2450,8 +2487,8 @@
         <v>3643</v>
       </c>
       <c r="G76" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.31265440570958003</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
@@ -2476,8 +2513,8 @@
         <v>2773</v>
       </c>
       <c r="G77" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.42372881355932202</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
@@ -2502,8 +2539,8 @@
         <v>1956</v>
       </c>
       <c r="G78" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.41666666666666669</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
@@ -2528,8 +2565,8 @@
         <v>1638</v>
       </c>
       <c r="G79" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.32539682539682541</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
@@ -2554,8 +2591,8 @@
         <v>1362</v>
       </c>
       <c r="G80" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.28928046989721001</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
@@ -2580,8 +2617,8 @@
         <v>5624</v>
       </c>
       <c r="G81" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.0312944523470839E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
@@ -2606,8 +2643,8 @@
         <v>5141</v>
       </c>
       <c r="G82" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.10737210659404785</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
@@ -2632,8 +2669,8 @@
         <v>3643</v>
       </c>
       <c r="G83" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.30359593741421903</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
@@ -2658,8 +2695,8 @@
         <v>2773</v>
       </c>
       <c r="G84" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.40245221781464119</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
@@ -2684,8 +2721,8 @@
         <v>1956</v>
       </c>
       <c r="G85" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.40132924335378323</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
@@ -2710,8 +2747,8 @@
         <v>1638</v>
       </c>
       <c r="G86" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.39560439560439559</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
@@ -2736,8 +2773,8 @@
         <v>1362</v>
       </c>
       <c r="G87" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.28854625550660795</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
@@ -2762,8 +2799,8 @@
         <v>5624</v>
       </c>
       <c r="G88" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.0312944523470839E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
@@ -2788,8 +2825,8 @@
         <v>5141</v>
       </c>
       <c r="G89" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.10834468002334176</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
@@ -2814,8 +2851,8 @@
         <v>3643</v>
       </c>
       <c r="G90" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3085369201207796</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
@@ -2840,8 +2877,8 @@
         <v>2773</v>
       </c>
       <c r="G91" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.38910926794085826</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
@@ -2866,8 +2903,8 @@
         <v>1956</v>
       </c>
       <c r="G92" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.46574642126789367</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
@@ -2892,8 +2929,8 @@
         <v>1638</v>
       </c>
       <c r="G93" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.30525030525030528</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
@@ -2918,8 +2955,8 @@
         <v>1362</v>
       </c>
       <c r="G94" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.27165932452276065</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
@@ -2944,8 +2981,8 @@
         <v>5624</v>
       </c>
       <c r="G95" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>9.2460881934566148E-3</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
@@ -2970,8 +3007,8 @@
         <v>5141</v>
       </c>
       <c r="G96" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.8389418401089289E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
@@ -2996,8 +3033,8 @@
         <v>3643</v>
       </c>
       <c r="G97" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.27724402964589623</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
@@ -3022,8 +3059,8 @@
         <v>2773</v>
       </c>
       <c r="G98" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.45834835917778577</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
@@ -3048,8 +3085,8 @@
         <v>1956</v>
       </c>
       <c r="G99" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.55265848670756645</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
@@ -3074,8 +3111,8 @@
         <v>1638</v>
       </c>
       <c r="G100" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3504273504273504</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
@@ -3100,8 +3137,8 @@
         <v>1362</v>
       </c>
       <c r="G101" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3656387665198238</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
@@ -3126,8 +3163,8 @@
         <v>5622</v>
       </c>
       <c r="G102" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>9.8719316969050161E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
@@ -3152,8 +3189,8 @@
         <v>5489</v>
       </c>
       <c r="G103" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.32738203680087447</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
@@ -3178,8 +3215,8 @@
         <v>3869</v>
       </c>
       <c r="G104" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.50581545619023005</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
@@ -3204,8 +3241,8 @@
         <v>3174</v>
       </c>
       <c r="G105" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.4732199117832388</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
@@ -3230,8 +3267,8 @@
         <v>2404</v>
       </c>
       <c r="G106" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.35108153078202997</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
@@ -3256,8 +3293,8 @@
         <v>2075</v>
       </c>
       <c r="G107" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.26024096385542167</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
@@ -3282,8 +3319,8 @@
         <v>1829</v>
       </c>
       <c r="G108" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.21159103335155824</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
@@ -3308,8 +3345,8 @@
         <v>5622</v>
       </c>
       <c r="G109" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6663109213802913E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
@@ -3334,8 +3371,8 @@
         <v>5489</v>
       </c>
       <c r="G110" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.32683548916013844</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
@@ -3360,8 +3397,8 @@
         <v>3869</v>
       </c>
       <c r="G111" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.50193848539674335</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
@@ -3386,8 +3423,8 @@
         <v>3174</v>
       </c>
       <c r="G112" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.44990548204158792</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
@@ -3412,8 +3449,8 @@
         <v>2404</v>
       </c>
       <c r="G113" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3781198003327787</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
@@ -3438,8 +3475,8 @@
         <v>2075</v>
       </c>
       <c r="G114" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.25156626506024099</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
@@ -3464,8 +3501,8 @@
         <v>1829</v>
       </c>
       <c r="G115" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.20229633679606343</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
@@ -3490,8 +3527,8 @@
         <v>5622</v>
       </c>
       <c r="G116" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>8.6979722518676625E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
@@ -3516,8 +3553,8 @@
         <v>5489</v>
       </c>
       <c r="G117" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.31554017125159411</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
@@ -3542,8 +3579,8 @@
         <v>3869</v>
       </c>
       <c r="G118" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.46627035409666578</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
@@ -3568,8 +3605,8 @@
         <v>3174</v>
       </c>
       <c r="G119" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.47416509136735979</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
@@ -3594,8 +3631,8 @@
         <v>2404</v>
       </c>
       <c r="G120" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3639767054908486</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
@@ -3620,8 +3657,8 @@
         <v>2075</v>
       </c>
       <c r="G121" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.25542168674698795</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
@@ -3646,8 +3683,8 @@
         <v>1829</v>
       </c>
       <c r="G122" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.17495899398578457</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
@@ -3672,8 +3709,8 @@
         <v>5622</v>
       </c>
       <c r="G123" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>9.3738882959800776E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
@@ -3698,8 +3735,8 @@
         <v>5489</v>
       </c>
       <c r="G124" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.32665330661322645</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
@@ -3724,8 +3761,8 @@
         <v>3869</v>
       </c>
       <c r="G125" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.52261566296200568</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
@@ -3750,8 +3787,8 @@
         <v>3174</v>
       </c>
       <c r="G126" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.48109640831758033</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
@@ -3776,8 +3813,8 @@
         <v>2404</v>
       </c>
       <c r="G127" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.37354409317803661</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
@@ -3802,8 +3839,8 @@
         <v>2075</v>
       </c>
       <c r="G128" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.33638554216867472</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
@@ -3828,8 +3865,8 @@
         <v>1829</v>
       </c>
       <c r="G129" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.19737561509021323</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
@@ -3854,8 +3891,8 @@
         <v>5622</v>
       </c>
       <c r="G130" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>9.4450373532550688E-2</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
@@ -3880,8 +3917,8 @@
         <v>5489</v>
       </c>
       <c r="G131" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.30916378210967388</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
@@ -3906,8 +3943,8 @@
         <v>3869</v>
       </c>
       <c r="G132" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.51512018609459809</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
@@ -3932,8 +3969,8 @@
         <v>3174</v>
       </c>
       <c r="G133" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.5</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
@@ -3958,8 +3995,8 @@
         <v>2404</v>
       </c>
       <c r="G134" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.40266222961730447</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
@@ -3984,8 +4021,8 @@
         <v>2075</v>
       </c>
       <c r="G135" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.3378313253012048</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
@@ -4010,8 +4047,8 @@
         <v>1829</v>
       </c>
       <c r="G136" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.26845270639693819</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
@@ -4036,8 +4073,8 @@
         <v>5622</v>
       </c>
       <c r="G137" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.1104589114194237</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
@@ -4062,8 +4099,8 @@
         <v>5489</v>
       </c>
       <c r="G138" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.32683548916013844</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
@@ -4088,8 +4125,8 @@
         <v>3869</v>
       </c>
       <c r="G139" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.49004910829671749</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
@@ -4114,8 +4151,8 @@
         <v>3174</v>
       </c>
       <c r="G140" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.53308128544423439</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
@@ -4140,8 +4177,8 @@
         <v>2404</v>
       </c>
       <c r="G141" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.44550748752079866</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
@@ -4166,8 +4203,8 @@
         <v>2075</v>
       </c>
       <c r="G142" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.37493975903614457</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
@@ -4192,8 +4229,8 @@
         <v>1829</v>
       </c>
       <c r="G143" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.27063969382176051</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
@@ -4218,8 +4255,8 @@
         <v>48</v>
       </c>
       <c r="G144" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.75</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
@@ -4244,8 +4281,8 @@
         <v>221</v>
       </c>
       <c r="G145" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.60633484162895923</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -4270,8 +4307,8 @@
         <v>243</v>
       </c>
       <c r="G146" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.5967078189300411</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
@@ -4296,8 +4333,8 @@
         <v>175</v>
       </c>
       <c r="G147" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.5485714285714286</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
@@ -4322,8 +4359,8 @@
         <v>407</v>
       </c>
       <c r="G148" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.46437346437346438</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
@@ -4348,8 +4385,8 @@
         <v>147</v>
       </c>
       <c r="G149" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.42176870748299322</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
@@ -4374,8 +4411,8 @@
         <v>76</v>
       </c>
       <c r="G150" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.43421052631578949</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
@@ -4400,8 +4437,8 @@
         <v>28</v>
       </c>
       <c r="G151" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.5357142857142857</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
@@ -4426,8 +4463,8 @@
         <v>26</v>
       </c>
       <c r="G152" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.34615384615384615</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
@@ -4452,8 +4489,8 @@
         <v>191</v>
       </c>
       <c r="G153" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.60209424083769636</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
@@ -4478,8 +4515,8 @@
         <v>693</v>
       </c>
       <c r="G154" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.37662337662337664</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
@@ -4504,8 +4541,8 @@
         <v>662</v>
       </c>
       <c r="G155" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.23867069486404835</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
@@ -4530,8 +4567,8 @@
         <v>666</v>
       </c>
       <c r="G156" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.20270270270270271</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
@@ -4556,8 +4593,8 @@
         <v>2272</v>
       </c>
       <c r="G157" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.1932218309859155</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
@@ -4582,8 +4619,8 @@
         <v>1400</v>
       </c>
       <c r="G158" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.17642857142857143</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
@@ -4608,8 +4645,8 @@
         <v>982</v>
       </c>
       <c r="G159" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.13238289205702647</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
@@ -4634,13 +4671,13 @@
         <v>617</v>
       </c>
       <c r="G160" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.16531604538087522</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>57</v>
       </c>
@@ -4660,11 +4697,1123 @@
         <v>567</v>
       </c>
       <c r="G161" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.14638447971781304</v>
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>0</v>
       </c>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
+    </row>
+    <row r="162" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D162" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E162" s="1">
+        <v>6</v>
+      </c>
+      <c r="F162" s="1">
+        <v>48</v>
+      </c>
+      <c r="G162" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.0125000000000001E-2</v>
+      </c>
+      <c r="H162" s="7"/>
+      <c r="I162" s="7"/>
+      <c r="J162">
+        <v>0.161</v>
+      </c>
+      <c r="K162" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A163" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D163" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E163" s="1">
+        <v>12</v>
+      </c>
+      <c r="F163" s="1">
+        <v>221</v>
+      </c>
+      <c r="G163" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>8.742081447963802E-3</v>
+      </c>
+      <c r="H163" s="7"/>
+      <c r="I163" s="7"/>
+      <c r="J163">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D164" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E164" s="1">
+        <v>31</v>
+      </c>
+      <c r="F164" s="1">
+        <v>243</v>
+      </c>
+      <c r="G164" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.0539094650205762E-2</v>
+      </c>
+      <c r="H164" s="7"/>
+      <c r="I164" s="7"/>
+      <c r="J164">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A165" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D165" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E165" s="1">
+        <v>27</v>
+      </c>
+      <c r="F165" s="1">
+        <v>175</v>
+      </c>
+      <c r="G165" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>1.9902857142857142E-2</v>
+      </c>
+      <c r="H165" s="7"/>
+      <c r="I165" s="7"/>
+      <c r="J165">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A166" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D166" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E166" s="1">
+        <v>33</v>
+      </c>
+      <c r="F166" s="1">
+        <v>407</v>
+      </c>
+      <c r="G166" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>1.0459459459459461E-2</v>
+      </c>
+      <c r="H166" s="7"/>
+      <c r="I166" s="7"/>
+      <c r="J166">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D167" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E167" s="1">
+        <v>8</v>
+      </c>
+      <c r="F167" s="1">
+        <v>147</v>
+      </c>
+      <c r="G167" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>1.8122448979591838E-2</v>
+      </c>
+      <c r="H167" s="7"/>
+      <c r="I167" s="7"/>
+      <c r="J167">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D168" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E168" s="1">
+        <v>6</v>
+      </c>
+      <c r="F168" s="1">
+        <v>76</v>
+      </c>
+      <c r="G168" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.6289473684210526E-2</v>
+      </c>
+      <c r="H168" s="7"/>
+      <c r="I168" s="7"/>
+      <c r="J168">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D169" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E169" s="1">
+        <v>2</v>
+      </c>
+      <c r="F169" s="1">
+        <v>28</v>
+      </c>
+      <c r="G169" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.3785714285714285E-2</v>
+      </c>
+      <c r="H169" s="7"/>
+      <c r="I169" s="7"/>
+      <c r="J169">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D170" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E170" s="1">
+        <v>1</v>
+      </c>
+      <c r="F170" s="1">
+        <f>26/2</f>
+        <v>13</v>
+      </c>
+      <c r="G170" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.561538461538462E-2</v>
+      </c>
+      <c r="H170" s="7"/>
+      <c r="I170" s="7"/>
+      <c r="J170">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D171" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E171" s="1">
+        <v>1</v>
+      </c>
+      <c r="F171" s="1">
+        <f>26/2</f>
+        <v>13</v>
+      </c>
+      <c r="G171" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.561538461538462E-2</v>
+      </c>
+      <c r="H171" s="7"/>
+      <c r="I171" s="7"/>
+      <c r="J171">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D172" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E172" s="1">
+        <v>3</v>
+      </c>
+      <c r="F172" s="1">
+        <v>191</v>
+      </c>
+      <c r="G172" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.1361256544502618E-3</v>
+      </c>
+      <c r="H172" s="7"/>
+      <c r="I172" s="7"/>
+      <c r="J172">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A173" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D173" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E173" s="1">
+        <v>19</v>
+      </c>
+      <c r="F173" s="1">
+        <v>693</v>
+      </c>
+      <c r="G173" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>3.7287157287157289E-3</v>
+      </c>
+      <c r="H173" s="7"/>
+      <c r="I173" s="7"/>
+      <c r="J173">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A174" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D174" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E174" s="1">
+        <v>14</v>
+      </c>
+      <c r="F174" s="1">
+        <v>662</v>
+      </c>
+      <c r="G174" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.8761329305135954E-3</v>
+      </c>
+      <c r="H174" s="7"/>
+      <c r="I174" s="7"/>
+      <c r="J174">
+        <v>0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A175" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D175" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E175" s="1">
+        <v>24</v>
+      </c>
+      <c r="F175" s="1">
+        <v>666</v>
+      </c>
+      <c r="G175" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>7.4954954954954949E-3</v>
+      </c>
+      <c r="H175" s="7"/>
+      <c r="I175" s="7"/>
+      <c r="J175">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A176" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D176" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E176" s="1">
+        <v>65</v>
+      </c>
+      <c r="F176" s="4">
+        <v>2272</v>
+      </c>
+      <c r="G176" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>5.9507042253521122E-3</v>
+      </c>
+      <c r="H176" s="7"/>
+      <c r="I176" s="7"/>
+      <c r="J176">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A177" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D177" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E177" s="1">
+        <v>44</v>
+      </c>
+      <c r="F177" s="4">
+        <v>1400</v>
+      </c>
+      <c r="G177" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>9.0828571428571425E-3</v>
+      </c>
+      <c r="H177" s="7"/>
+      <c r="I177" s="7"/>
+      <c r="J177">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A178" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D178" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E178" s="1">
+        <v>30</v>
+      </c>
+      <c r="F178" s="1">
+        <v>982</v>
+      </c>
+      <c r="G178" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>8.8289205702647647E-3</v>
+      </c>
+      <c r="H178" s="7"/>
+      <c r="I178" s="7"/>
+      <c r="J178">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D179" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E179" s="1">
+        <v>13</v>
+      </c>
+      <c r="F179" s="1">
+        <v>617</v>
+      </c>
+      <c r="G179" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>6.0891410048622358E-3</v>
+      </c>
+      <c r="H179" s="7"/>
+      <c r="I179" s="7"/>
+      <c r="J179">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A180" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D180" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E180" s="1">
+        <v>4</v>
+      </c>
+      <c r="F180" s="1">
+        <f>567/2</f>
+        <v>283.5</v>
+      </c>
+      <c r="G180" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>4.0776014109347438E-3</v>
+      </c>
+      <c r="H180" s="7"/>
+      <c r="I180" s="7"/>
+      <c r="J180">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D181" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E181" s="1">
+        <v>4</v>
+      </c>
+      <c r="F181" s="1">
+        <f>567/2</f>
+        <v>283.5</v>
+      </c>
+      <c r="G181" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>4.0776014109347438E-3</v>
+      </c>
+      <c r="H181" s="7"/>
+      <c r="I181" s="7"/>
+      <c r="J181">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>61</v>
+      </c>
+      <c r="B182" t="s">
+        <v>56</v>
+      </c>
+      <c r="C182" t="s">
+        <v>53</v>
+      </c>
+      <c r="D182">
+        <v>2014</v>
+      </c>
+      <c r="E182">
+        <v>36</v>
+      </c>
+      <c r="F182">
+        <v>48</v>
+      </c>
+      <c r="G182" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>7.1250000000000008E-2</v>
+      </c>
+      <c r="H182" s="7"/>
+      <c r="I182" s="7"/>
+      <c r="J182">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K182" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>61</v>
+      </c>
+      <c r="B183" t="s">
+        <v>56</v>
+      </c>
+      <c r="C183" t="s">
+        <v>5</v>
+      </c>
+      <c r="D183">
+        <v>2014</v>
+      </c>
+      <c r="E183">
+        <v>134</v>
+      </c>
+      <c r="F183">
+        <v>221</v>
+      </c>
+      <c r="G183" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>5.7601809954751129E-2</v>
+      </c>
+      <c r="H183" s="7"/>
+      <c r="I183" s="7"/>
+      <c r="J183">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>61</v>
+      </c>
+      <c r="B184" t="s">
+        <v>56</v>
+      </c>
+      <c r="C184" t="s">
+        <v>6</v>
+      </c>
+      <c r="D184">
+        <v>2014</v>
+      </c>
+      <c r="E184">
+        <v>145</v>
+      </c>
+      <c r="F184">
+        <v>243</v>
+      </c>
+      <c r="G184" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>5.6687242798353903E-2</v>
+      </c>
+      <c r="H184" s="7"/>
+      <c r="I184" s="7"/>
+      <c r="J184">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>61</v>
+      </c>
+      <c r="B185" t="s">
+        <v>56</v>
+      </c>
+      <c r="C185" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185">
+        <v>2014</v>
+      </c>
+      <c r="E185">
+        <v>96</v>
+      </c>
+      <c r="F185">
+        <v>175</v>
+      </c>
+      <c r="G185" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>5.5954285714285713E-2</v>
+      </c>
+      <c r="H185" s="7"/>
+      <c r="I185" s="7"/>
+      <c r="J185">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>61</v>
+      </c>
+      <c r="B186" t="s">
+        <v>56</v>
+      </c>
+      <c r="C186" t="s">
+        <v>8</v>
+      </c>
+      <c r="D186">
+        <v>2014</v>
+      </c>
+      <c r="E186">
+        <v>189</v>
+      </c>
+      <c r="F186">
+        <v>407</v>
+      </c>
+      <c r="G186" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>4.7366093366093362E-2</v>
+      </c>
+      <c r="H186" s="7"/>
+      <c r="I186" s="7"/>
+      <c r="J186">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>61</v>
+      </c>
+      <c r="B187" t="s">
+        <v>56</v>
+      </c>
+      <c r="C187" t="s">
+        <v>9</v>
+      </c>
+      <c r="D187">
+        <v>2014</v>
+      </c>
+      <c r="E187">
+        <v>62</v>
+      </c>
+      <c r="F187">
+        <v>147</v>
+      </c>
+      <c r="G187" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>4.5972789115646263E-2</v>
+      </c>
+      <c r="H187" s="7"/>
+      <c r="I187" s="7"/>
+      <c r="J187">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>61</v>
+      </c>
+      <c r="B188" t="s">
+        <v>56</v>
+      </c>
+      <c r="C188" t="s">
+        <v>10</v>
+      </c>
+      <c r="D188">
+        <v>2014</v>
+      </c>
+      <c r="E188">
+        <v>33</v>
+      </c>
+      <c r="F188">
+        <v>76</v>
+      </c>
+      <c r="G188" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>4.7328947368421054E-2</v>
+      </c>
+      <c r="H188" s="7"/>
+      <c r="I188" s="7"/>
+      <c r="J188">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>61</v>
+      </c>
+      <c r="B189" t="s">
+        <v>56</v>
+      </c>
+      <c r="C189" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189">
+        <v>2014</v>
+      </c>
+      <c r="E189">
+        <v>15</v>
+      </c>
+      <c r="F189">
+        <v>28</v>
+      </c>
+      <c r="G189" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>5.8392857142857142E-2</v>
+      </c>
+      <c r="H189" s="7"/>
+      <c r="I189" s="7"/>
+      <c r="J189">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>61</v>
+      </c>
+      <c r="B190" t="s">
+        <v>56</v>
+      </c>
+      <c r="C190" t="s">
+        <v>54</v>
+      </c>
+      <c r="D190">
+        <v>2014</v>
+      </c>
+      <c r="E190">
+        <v>9</v>
+      </c>
+      <c r="F190">
+        <v>26</v>
+      </c>
+      <c r="G190" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>3.7730769230769227E-2</v>
+      </c>
+      <c r="H190" s="7"/>
+      <c r="I190" s="7"/>
+      <c r="J190">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>62</v>
+      </c>
+      <c r="B191" t="s">
+        <v>56</v>
+      </c>
+      <c r="C191" t="s">
+        <v>53</v>
+      </c>
+      <c r="D191">
+        <v>2014</v>
+      </c>
+      <c r="E191">
+        <v>115</v>
+      </c>
+      <c r="F191">
+        <v>191</v>
+      </c>
+      <c r="G191" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>5.7198952879581155E-2</v>
+      </c>
+      <c r="H191" s="7"/>
+      <c r="I191" s="7"/>
+      <c r="J191">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>62</v>
+      </c>
+      <c r="B192" t="s">
+        <v>56</v>
+      </c>
+      <c r="C192" t="s">
+        <v>5</v>
+      </c>
+      <c r="D192">
+        <v>2014</v>
+      </c>
+      <c r="E192">
+        <v>261</v>
+      </c>
+      <c r="F192">
+        <v>693</v>
+      </c>
+      <c r="G192" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>3.5779220779220779E-2</v>
+      </c>
+      <c r="H192" s="7"/>
+      <c r="I192" s="7"/>
+      <c r="J192">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>62</v>
+      </c>
+      <c r="B193" t="s">
+        <v>56</v>
+      </c>
+      <c r="C193" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193">
+        <v>2014</v>
+      </c>
+      <c r="E193">
+        <v>158</v>
+      </c>
+      <c r="F193">
+        <v>662</v>
+      </c>
+      <c r="G193" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.2673716012084594E-2</v>
+      </c>
+      <c r="H193" s="7"/>
+      <c r="I193" s="7"/>
+      <c r="J193">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>62</v>
+      </c>
+      <c r="B194" t="s">
+        <v>56</v>
+      </c>
+      <c r="C194" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194">
+        <v>2014</v>
+      </c>
+      <c r="E194">
+        <v>135</v>
+      </c>
+      <c r="F194">
+        <v>666</v>
+      </c>
+      <c r="G194" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.4527027027027026E-2</v>
+      </c>
+      <c r="H194" s="7"/>
+      <c r="I194" s="7"/>
+      <c r="J194">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>62</v>
+      </c>
+      <c r="B195" t="s">
+        <v>56</v>
+      </c>
+      <c r="C195" t="s">
+        <v>8</v>
+      </c>
+      <c r="D195">
+        <v>2014</v>
+      </c>
+      <c r="E195">
+        <v>439</v>
+      </c>
+      <c r="F195">
+        <v>2272</v>
+      </c>
+      <c r="G195" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.3379841549295774E-2</v>
+      </c>
+      <c r="H195" s="7"/>
+      <c r="I195" s="7"/>
+      <c r="J195">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>62</v>
+      </c>
+      <c r="B196" t="s">
+        <v>56</v>
+      </c>
+      <c r="C196" t="s">
+        <v>9</v>
+      </c>
+      <c r="D196">
+        <v>2014</v>
+      </c>
+      <c r="E196">
+        <v>247</v>
+      </c>
+      <c r="F196">
+        <v>1400</v>
+      </c>
+      <c r="G196" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.8052142857142859E-2</v>
+      </c>
+      <c r="H196" s="7"/>
+      <c r="I196" s="7"/>
+      <c r="J196">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>62</v>
+      </c>
+      <c r="B197" t="s">
+        <v>56</v>
+      </c>
+      <c r="C197" t="s">
+        <v>10</v>
+      </c>
+      <c r="D197">
+        <v>2014</v>
+      </c>
+      <c r="E197">
+        <v>130</v>
+      </c>
+      <c r="F197">
+        <v>982</v>
+      </c>
+      <c r="G197" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.104887983706721E-2</v>
+      </c>
+      <c r="H197" s="7"/>
+      <c r="I197" s="7"/>
+      <c r="J197">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>62</v>
+      </c>
+      <c r="B198" t="s">
+        <v>56</v>
+      </c>
+      <c r="C198" t="s">
+        <v>11</v>
+      </c>
+      <c r="D198">
+        <v>2014</v>
+      </c>
+      <c r="E198">
+        <v>102</v>
+      </c>
+      <c r="F198">
+        <v>617</v>
+      </c>
+      <c r="G198" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.628525121555916E-2</v>
+      </c>
+      <c r="H198" s="7"/>
+      <c r="I198" s="7"/>
+      <c r="J198">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>62</v>
+      </c>
+      <c r="B199" t="s">
+        <v>56</v>
+      </c>
+      <c r="C199" t="s">
+        <v>54</v>
+      </c>
+      <c r="D199">
+        <v>2014</v>
+      </c>
+      <c r="E199">
+        <v>83</v>
+      </c>
+      <c r="F199">
+        <v>567</v>
+      </c>
+      <c r="G199" s="6">
+        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
+        <v>2.3275132275132275E-2</v>
+      </c>
+      <c r="H199" s="7"/>
+      <c r="I199" s="7"/>
+      <c r="J199">
+        <v>0.159</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating calibration functions to most recent
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CISNET\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="64">
   <si>
     <t>N</t>
   </si>
@@ -209,16 +209,7 @@
     <t>CIN2/CIN3 Prevalence HPV16 (HIV-)</t>
   </si>
   <si>
-    <t>HPV Prevalence in HIV+ Women HPV16</t>
-  </si>
-  <si>
-    <t>HPV Prevalence in HIV- Women HPV16</t>
-  </si>
-  <si>
     <t>Column1</t>
-  </si>
-  <si>
-    <t>Proportion of HPV infections that were HPV16 among women with WNL/CIN1</t>
   </si>
   <si>
     <t>Column2</t>
@@ -280,13 +271,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,8 +293,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K199" totalsRowShown="0">
-  <autoFilter ref="A1:K199"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K181" totalsRowShown="0">
+  <autoFilter ref="A1:K181"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Criteria"/>
     <tableColumn id="9" name="Source"/>
@@ -311,11 +302,11 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="0">
+    <tableColumn id="4" name="Mean" dataDxfId="2">
       <calculatedColumnFormula>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="2"/>
-    <tableColumn id="6" name="UB" dataDxfId="1"/>
+    <tableColumn id="5" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" name="UB" dataDxfId="0"/>
     <tableColumn id="8" name="Column1"/>
     <tableColumn id="11" name="Column2"/>
   </tableColumns>
@@ -586,23 +577,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K199"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="J201" sqref="J201"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="M188" sqref="M188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" customWidth="1"/>
-    <col min="11" max="11" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -631,13 +622,13 @@
         <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -661,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -685,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -709,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -733,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -757,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -781,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -805,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -829,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -854,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -879,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -903,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -927,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -951,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -975,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -999,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1023,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1047,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1071,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1096,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1121,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1145,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1169,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1193,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1217,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1265,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1289,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1313,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1385,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1409,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -1433,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -1457,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -1481,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1505,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1529,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -1553,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1577,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -1601,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1625,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1649,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -1673,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -1697,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1721,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -1745,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
@@ -1769,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
@@ -1795,7 +1786,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
@@ -1821,7 +1812,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -1847,7 +1838,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1875,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
@@ -1903,7 +1894,7 @@
         <v>0.73896528627634828</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
@@ -1931,7 +1922,7 @@
         <v>0.62062966115974605</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
@@ -1959,7 +1950,7 @@
         <v>0.47893264233014488</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>36</v>
       </c>
@@ -1987,7 +1978,7 @@
         <v>0.59252264082678208</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>36</v>
       </c>
@@ -2015,7 +2006,7 @@
         <v>0.32293097813833699</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>36</v>
       </c>
@@ -2043,7 +2034,7 @@
         <v>0.29832234128895085</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>36</v>
       </c>
@@ -2071,7 +2062,7 @@
         <v>0.27445149548815129</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
@@ -2095,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>40</v>
       </c>
@@ -2119,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>40</v>
       </c>
@@ -2143,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>40</v>
       </c>
@@ -2167,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -2191,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>40</v>
       </c>
@@ -2215,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
@@ -2239,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>41</v>
       </c>
@@ -2263,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>41</v>
       </c>
@@ -2287,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>41</v>
       </c>
@@ -2311,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>41</v>
       </c>
@@ -2337,7 +2328,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>41</v>
       </c>
@@ -2363,7 +2354,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>41</v>
       </c>
@@ -2389,7 +2380,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>41</v>
       </c>
@@ -2415,7 +2406,7 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -2441,7 +2432,7 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>42</v>
       </c>
@@ -2467,7 +2458,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>42</v>
       </c>
@@ -2493,7 +2484,7 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>42</v>
       </c>
@@ -2519,7 +2510,7 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>42</v>
       </c>
@@ -2545,7 +2536,7 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
@@ -2571,7 +2562,7 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>42</v>
       </c>
@@ -2597,7 +2588,7 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
@@ -2623,7 +2614,7 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2649,7 +2640,7 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>43</v>
       </c>
@@ -2675,7 +2666,7 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>43</v>
       </c>
@@ -2701,7 +2692,7 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>43</v>
       </c>
@@ -2727,7 +2718,7 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>43</v>
       </c>
@@ -2753,7 +2744,7 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>43</v>
       </c>
@@ -2779,7 +2770,7 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>44</v>
       </c>
@@ -2805,7 +2796,7 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>44</v>
       </c>
@@ -2831,7 +2822,7 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>44</v>
       </c>
@@ -2857,7 +2848,7 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>44</v>
       </c>
@@ -2883,7 +2874,7 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>44</v>
       </c>
@@ -2909,7 +2900,7 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>44</v>
       </c>
@@ -2935,7 +2926,7 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>44</v>
       </c>
@@ -2961,7 +2952,7 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>45</v>
       </c>
@@ -2987,7 +2978,7 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>45</v>
       </c>
@@ -3013,7 +3004,7 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>45</v>
       </c>
@@ -3039,7 +3030,7 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>45</v>
       </c>
@@ -3065,7 +3056,7 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>45</v>
       </c>
@@ -3091,7 +3082,7 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>45</v>
       </c>
@@ -3117,7 +3108,7 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>45</v>
       </c>
@@ -3143,7 +3134,7 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>46</v>
       </c>
@@ -3169,7 +3160,7 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>46</v>
       </c>
@@ -3195,7 +3186,7 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>46</v>
       </c>
@@ -3221,7 +3212,7 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>46</v>
       </c>
@@ -3247,7 +3238,7 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>46</v>
       </c>
@@ -3273,7 +3264,7 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>46</v>
       </c>
@@ -3299,7 +3290,7 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>46</v>
       </c>
@@ -3325,7 +3316,7 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>47</v>
       </c>
@@ -3351,7 +3342,7 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -3377,7 +3368,7 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>47</v>
       </c>
@@ -3403,7 +3394,7 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>47</v>
       </c>
@@ -3429,7 +3420,7 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>47</v>
       </c>
@@ -3455,7 +3446,7 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>47</v>
       </c>
@@ -3481,7 +3472,7 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>47</v>
       </c>
@@ -3507,7 +3498,7 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>48</v>
       </c>
@@ -3533,7 +3524,7 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>48</v>
       </c>
@@ -3559,7 +3550,7 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>48</v>
       </c>
@@ -3585,7 +3576,7 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>48</v>
       </c>
@@ -3611,7 +3602,7 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>48</v>
       </c>
@@ -3637,7 +3628,7 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>48</v>
       </c>
@@ -3663,7 +3654,7 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>48</v>
       </c>
@@ -3689,7 +3680,7 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>49</v>
       </c>
@@ -3715,7 +3706,7 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>49</v>
       </c>
@@ -3741,7 +3732,7 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>49</v>
       </c>
@@ -3767,7 +3758,7 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -3793,7 +3784,7 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>49</v>
       </c>
@@ -3819,7 +3810,7 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>49</v>
       </c>
@@ -3845,7 +3836,7 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>49</v>
       </c>
@@ -3871,7 +3862,7 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>50</v>
       </c>
@@ -3897,7 +3888,7 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>50</v>
       </c>
@@ -3923,7 +3914,7 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>50</v>
       </c>
@@ -3949,7 +3940,7 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>50</v>
       </c>
@@ -3975,7 +3966,7 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>50</v>
       </c>
@@ -4001,7 +3992,7 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>50</v>
       </c>
@@ -4027,7 +4018,7 @@
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>50</v>
       </c>
@@ -4053,7 +4044,7 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>51</v>
       </c>
@@ -4079,7 +4070,7 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>51</v>
       </c>
@@ -4105,7 +4096,7 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>51</v>
       </c>
@@ -4131,7 +4122,7 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>51</v>
       </c>
@@ -4157,7 +4148,7 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>51</v>
       </c>
@@ -4183,7 +4174,7 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>51</v>
       </c>
@@ -4209,7 +4200,7 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>51</v>
       </c>
@@ -4235,7 +4226,7 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>55</v>
       </c>
@@ -4261,7 +4252,7 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>55</v>
       </c>
@@ -4287,7 +4278,7 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>55</v>
       </c>
@@ -4313,7 +4304,7 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>55</v>
       </c>
@@ -4339,7 +4330,7 @@
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>55</v>
       </c>
@@ -4365,7 +4356,7 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>55</v>
       </c>
@@ -4391,7 +4382,7 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>55</v>
       </c>
@@ -4417,7 +4408,7 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>55</v>
       </c>
@@ -4443,7 +4434,7 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>55</v>
       </c>
@@ -4469,7 +4460,7 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>57</v>
       </c>
@@ -4495,7 +4486,7 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>57</v>
       </c>
@@ -4521,7 +4512,7 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>57</v>
       </c>
@@ -4547,7 +4538,7 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>57</v>
       </c>
@@ -4573,7 +4564,7 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>57</v>
       </c>
@@ -4599,7 +4590,7 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>57</v>
       </c>
@@ -4625,7 +4616,7 @@
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>57</v>
       </c>
@@ -4651,7 +4642,7 @@
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>57</v>
       </c>
@@ -4677,7 +4668,7 @@
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>57</v>
       </c>
@@ -4703,7 +4694,7 @@
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
     </row>
-    <row r="162" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>59</v>
       </c>
@@ -4732,10 +4723,10 @@
         <v>0.161</v>
       </c>
       <c r="K162" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>59</v>
       </c>
@@ -4764,7 +4755,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>59</v>
       </c>
@@ -4793,7 +4784,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>59</v>
       </c>
@@ -4822,7 +4813,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>59</v>
       </c>
@@ -4851,7 +4842,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>59</v>
       </c>
@@ -4880,7 +4871,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>59</v>
       </c>
@@ -4909,7 +4900,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>59</v>
       </c>
@@ -4938,7 +4929,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>59</v>
       </c>
@@ -4968,7 +4959,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>59</v>
       </c>
@@ -4998,7 +4989,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>60</v>
       </c>
@@ -5027,7 +5018,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>60</v>
       </c>
@@ -5056,7 +5047,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>60</v>
       </c>
@@ -5085,7 +5076,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>60</v>
       </c>
@@ -5114,7 +5105,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>60</v>
       </c>
@@ -5143,7 +5134,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>60</v>
       </c>
@@ -5172,7 +5163,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>60</v>
       </c>
@@ -5201,7 +5192,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>60</v>
       </c>
@@ -5230,7 +5221,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>60</v>
       </c>
@@ -5260,7 +5251,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>60</v>
       </c>
@@ -5290,535 +5281,12 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
-        <v>61</v>
-      </c>
-      <c r="B182" t="s">
-        <v>56</v>
-      </c>
-      <c r="C182" t="s">
-        <v>53</v>
-      </c>
-      <c r="D182">
-        <v>2014</v>
-      </c>
-      <c r="E182">
-        <v>36</v>
-      </c>
-      <c r="F182">
-        <v>48</v>
-      </c>
-      <c r="G182" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>7.1250000000000008E-2</v>
-      </c>
-      <c r="H182" s="7"/>
-      <c r="I182" s="7"/>
-      <c r="J182">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="K182" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
-        <v>61</v>
-      </c>
-      <c r="B183" t="s">
-        <v>56</v>
-      </c>
-      <c r="C183" t="s">
-        <v>5</v>
-      </c>
-      <c r="D183">
-        <v>2014</v>
-      </c>
-      <c r="E183">
-        <v>134</v>
-      </c>
-      <c r="F183">
-        <v>221</v>
-      </c>
-      <c r="G183" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>5.7601809954751129E-2</v>
-      </c>
-      <c r="H183" s="7"/>
-      <c r="I183" s="7"/>
-      <c r="J183">
-        <v>9.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
-        <v>61</v>
-      </c>
-      <c r="B184" t="s">
-        <v>56</v>
-      </c>
-      <c r="C184" t="s">
-        <v>6</v>
-      </c>
-      <c r="D184">
-        <v>2014</v>
-      </c>
-      <c r="E184">
-        <v>145</v>
-      </c>
-      <c r="F184">
-        <v>243</v>
-      </c>
-      <c r="G184" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>5.6687242798353903E-2</v>
-      </c>
-      <c r="H184" s="7"/>
-      <c r="I184" s="7"/>
-      <c r="J184">
-        <v>9.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
-        <v>61</v>
-      </c>
-      <c r="B185" t="s">
-        <v>56</v>
-      </c>
-      <c r="C185" t="s">
-        <v>7</v>
-      </c>
-      <c r="D185">
-        <v>2014</v>
-      </c>
-      <c r="E185">
-        <v>96</v>
-      </c>
-      <c r="F185">
-        <v>175</v>
-      </c>
-      <c r="G185" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>5.5954285714285713E-2</v>
-      </c>
-      <c r="H185" s="7"/>
-      <c r="I185" s="7"/>
-      <c r="J185">
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
-        <v>61</v>
-      </c>
-      <c r="B186" t="s">
-        <v>56</v>
-      </c>
-      <c r="C186" t="s">
-        <v>8</v>
-      </c>
-      <c r="D186">
-        <v>2014</v>
-      </c>
-      <c r="E186">
-        <v>189</v>
-      </c>
-      <c r="F186">
-        <v>407</v>
-      </c>
-      <c r="G186" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>4.7366093366093362E-2</v>
-      </c>
-      <c r="H186" s="7"/>
-      <c r="I186" s="7"/>
-      <c r="J186">
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
-        <v>61</v>
-      </c>
-      <c r="B187" t="s">
-        <v>56</v>
-      </c>
-      <c r="C187" t="s">
-        <v>9</v>
-      </c>
-      <c r="D187">
-        <v>2014</v>
-      </c>
-      <c r="E187">
-        <v>62</v>
-      </c>
-      <c r="F187">
-        <v>147</v>
-      </c>
-      <c r="G187" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>4.5972789115646263E-2</v>
-      </c>
-      <c r="H187" s="7"/>
-      <c r="I187" s="7"/>
-      <c r="J187">
-        <v>0.109</v>
-      </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
-        <v>61</v>
-      </c>
-      <c r="B188" t="s">
-        <v>56</v>
-      </c>
-      <c r="C188" t="s">
-        <v>10</v>
-      </c>
-      <c r="D188">
-        <v>2014</v>
-      </c>
-      <c r="E188">
-        <v>33</v>
-      </c>
-      <c r="F188">
-        <v>76</v>
-      </c>
-      <c r="G188" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>4.7328947368421054E-2</v>
-      </c>
-      <c r="H188" s="7"/>
-      <c r="I188" s="7"/>
-      <c r="J188">
-        <v>0.109</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
-        <v>61</v>
-      </c>
-      <c r="B189" t="s">
-        <v>56</v>
-      </c>
-      <c r="C189" t="s">
-        <v>11</v>
-      </c>
-      <c r="D189">
-        <v>2014</v>
-      </c>
-      <c r="E189">
-        <v>15</v>
-      </c>
-      <c r="F189">
-        <v>28</v>
-      </c>
-      <c r="G189" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>5.8392857142857142E-2</v>
-      </c>
-      <c r="H189" s="7"/>
-      <c r="I189" s="7"/>
-      <c r="J189">
-        <v>0.109</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
-        <v>61</v>
-      </c>
-      <c r="B190" t="s">
-        <v>56</v>
-      </c>
-      <c r="C190" t="s">
-        <v>54</v>
-      </c>
-      <c r="D190">
-        <v>2014</v>
-      </c>
-      <c r="E190">
-        <v>9</v>
-      </c>
-      <c r="F190">
-        <v>26</v>
-      </c>
-      <c r="G190" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>3.7730769230769227E-2</v>
-      </c>
-      <c r="H190" s="7"/>
-      <c r="I190" s="7"/>
-      <c r="J190">
-        <v>0.109</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>62</v>
-      </c>
-      <c r="B191" t="s">
-        <v>56</v>
-      </c>
-      <c r="C191" t="s">
-        <v>53</v>
-      </c>
-      <c r="D191">
-        <v>2014</v>
-      </c>
-      <c r="E191">
-        <v>115</v>
-      </c>
-      <c r="F191">
-        <v>191</v>
-      </c>
-      <c r="G191" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>5.7198952879581155E-2</v>
-      </c>
-      <c r="H191" s="7"/>
-      <c r="I191" s="7"/>
-      <c r="J191">
-        <v>9.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>62</v>
-      </c>
-      <c r="B192" t="s">
-        <v>56</v>
-      </c>
-      <c r="C192" t="s">
-        <v>5</v>
-      </c>
-      <c r="D192">
-        <v>2014</v>
-      </c>
-      <c r="E192">
-        <v>261</v>
-      </c>
-      <c r="F192">
-        <v>693</v>
-      </c>
-      <c r="G192" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>3.5779220779220779E-2</v>
-      </c>
-      <c r="H192" s="7"/>
-      <c r="I192" s="7"/>
-      <c r="J192">
-        <v>9.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
-        <v>62</v>
-      </c>
-      <c r="B193" t="s">
-        <v>56</v>
-      </c>
-      <c r="C193" t="s">
-        <v>6</v>
-      </c>
-      <c r="D193">
-        <v>2014</v>
-      </c>
-      <c r="E193">
-        <v>158</v>
-      </c>
-      <c r="F193">
-        <v>662</v>
-      </c>
-      <c r="G193" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.2673716012084594E-2</v>
-      </c>
-      <c r="H193" s="7"/>
-      <c r="I193" s="7"/>
-      <c r="J193">
-        <v>9.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
-        <v>62</v>
-      </c>
-      <c r="B194" t="s">
-        <v>56</v>
-      </c>
-      <c r="C194" t="s">
-        <v>7</v>
-      </c>
-      <c r="D194">
-        <v>2014</v>
-      </c>
-      <c r="E194">
-        <v>135</v>
-      </c>
-      <c r="F194">
-        <v>666</v>
-      </c>
-      <c r="G194" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.4527027027027026E-2</v>
-      </c>
-      <c r="H194" s="7"/>
-      <c r="I194" s="7"/>
-      <c r="J194">
-        <v>0.121</v>
-      </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
-        <v>62</v>
-      </c>
-      <c r="B195" t="s">
-        <v>56</v>
-      </c>
-      <c r="C195" t="s">
-        <v>8</v>
-      </c>
-      <c r="D195">
-        <v>2014</v>
-      </c>
-      <c r="E195">
-        <v>439</v>
-      </c>
-      <c r="F195">
-        <v>2272</v>
-      </c>
-      <c r="G195" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.3379841549295774E-2</v>
-      </c>
-      <c r="H195" s="7"/>
-      <c r="I195" s="7"/>
-      <c r="J195">
-        <v>0.121</v>
-      </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>62</v>
-      </c>
-      <c r="B196" t="s">
-        <v>56</v>
-      </c>
-      <c r="C196" t="s">
-        <v>9</v>
-      </c>
-      <c r="D196">
-        <v>2014</v>
-      </c>
-      <c r="E196">
-        <v>247</v>
-      </c>
-      <c r="F196">
-        <v>1400</v>
-      </c>
-      <c r="G196" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.8052142857142859E-2</v>
-      </c>
-      <c r="H196" s="7"/>
-      <c r="I196" s="7"/>
-      <c r="J196">
-        <v>0.159</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>62</v>
-      </c>
-      <c r="B197" t="s">
-        <v>56</v>
-      </c>
-      <c r="C197" t="s">
-        <v>10</v>
-      </c>
-      <c r="D197">
-        <v>2014</v>
-      </c>
-      <c r="E197">
-        <v>130</v>
-      </c>
-      <c r="F197">
-        <v>982</v>
-      </c>
-      <c r="G197" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.104887983706721E-2</v>
-      </c>
-      <c r="H197" s="7"/>
-      <c r="I197" s="7"/>
-      <c r="J197">
-        <v>0.159</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>62</v>
-      </c>
-      <c r="B198" t="s">
-        <v>56</v>
-      </c>
-      <c r="C198" t="s">
-        <v>11</v>
-      </c>
-      <c r="D198">
-        <v>2014</v>
-      </c>
-      <c r="E198">
-        <v>102</v>
-      </c>
-      <c r="F198">
-        <v>617</v>
-      </c>
-      <c r="G198" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.628525121555916E-2</v>
-      </c>
-      <c r="H198" s="7"/>
-      <c r="I198" s="7"/>
-      <c r="J198">
-        <v>0.159</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
-        <v>62</v>
-      </c>
-      <c r="B199" t="s">
-        <v>56</v>
-      </c>
-      <c r="C199" t="s">
-        <v>54</v>
-      </c>
-      <c r="D199">
-        <v>2014</v>
-      </c>
-      <c r="E199">
-        <v>83</v>
-      </c>
-      <c r="F199">
-        <v>567</v>
-      </c>
-      <c r="G199" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.3275132275132275E-2</v>
-      </c>
-      <c r="H199" s="7"/>
-      <c r="I199" s="7"/>
-      <c r="J199">
-        <v>0.159</v>
-      </c>
-    </row>
+    <row r="182" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correct in-sheet cell calculation, add description
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -271,13 +271,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,11 +302,11 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="2">
-      <calculatedColumnFormula>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</calculatedColumnFormula>
+    <tableColumn id="4" name="Mean" dataDxfId="0">
+      <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="1"/>
-    <tableColumn id="6" name="UB" dataDxfId="0"/>
+    <tableColumn id="5" name="LB" dataDxfId="2"/>
+    <tableColumn id="6" name="UB" dataDxfId="1"/>
     <tableColumn id="8" name="Column1"/>
     <tableColumn id="11" name="Column2"/>
   </tableColumns>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="M188" sqref="M188"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,8 +648,8 @@
         <v>48</v>
       </c>
       <c r="G2">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -672,8 +672,8 @@
         <v>221</v>
       </c>
       <c r="G3">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>5.4298642533936653E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -696,8 +696,8 @@
         <v>243</v>
       </c>
       <c r="G4">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.12757201646090535</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -720,8 +720,8 @@
         <v>175</v>
       </c>
       <c r="G5">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.15428571428571428</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -744,8 +744,8 @@
         <v>407</v>
       </c>
       <c r="G6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>8.1081081081081086E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -768,8 +768,8 @@
         <v>147</v>
       </c>
       <c r="G7">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>5.4421768707482991E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -792,8 +792,8 @@
         <v>76</v>
       </c>
       <c r="G8">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.8947368421052627E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -816,8 +816,8 @@
         <v>28</v>
       </c>
       <c r="G9">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.1428571428571425E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -841,8 +841,8 @@
         <v>13</v>
       </c>
       <c r="G10">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -866,8 +866,8 @@
         <v>13</v>
       </c>
       <c r="G11">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -890,8 +890,8 @@
         <v>191</v>
       </c>
       <c r="G12">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.5706806282722512E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -914,8 +914,8 @@
         <v>693</v>
       </c>
       <c r="G13">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.7417027417027416E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -938,8 +938,8 @@
         <v>662</v>
       </c>
       <c r="G14">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.1148036253776436E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -962,8 +962,8 @@
         <v>666</v>
       </c>
       <c r="G15">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.6036036036036036E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -986,8 +986,8 @@
         <v>2272</v>
       </c>
       <c r="G16">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.8609154929577465E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1010,8 +1010,8 @@
         <v>1400</v>
       </c>
       <c r="G17">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.1428571428571431E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1034,8 +1034,8 @@
         <v>982</v>
       </c>
       <c r="G18">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.0549898167006109E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,8 +1058,8 @@
         <v>617</v>
       </c>
       <c r="G19">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.1069692058346839E-2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1083,8 +1083,8 @@
         <v>283.5</v>
       </c>
       <c r="G20">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.4109347442680775E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1108,8 +1108,8 @@
         <v>283.5</v>
       </c>
       <c r="G21">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.4109347442680775E-2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1132,8 +1132,8 @@
         <v>239</v>
       </c>
       <c r="G22">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.16317991631799164</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1156,8 +1156,8 @@
         <v>914</v>
       </c>
       <c r="G23">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.20787746170678337</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1180,8 +1180,8 @@
         <v>905</v>
       </c>
       <c r="G24">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.21878453038674034</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1204,8 +1204,8 @@
         <v>841</v>
       </c>
       <c r="G25">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.14744351961950058</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1228,8 +1228,8 @@
         <v>2679</v>
       </c>
       <c r="G26">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.11534154535274356</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1252,8 +1252,8 @@
         <v>1547</v>
       </c>
       <c r="G27">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>6.1409179056237877E-2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1276,8 +1276,8 @@
         <v>1058</v>
       </c>
       <c r="G28">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.780718336483932E-2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,8 +1300,8 @@
         <v>645</v>
       </c>
       <c r="G29">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.0155038759689922E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1324,8 +1324,8 @@
         <v>296.5</v>
       </c>
       <c r="G30">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.6981450252951095E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1348,8 +1348,8 @@
         <v>296.5</v>
       </c>
       <c r="G31">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.6981450252951095E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,8 +1372,8 @@
         <v>239</v>
       </c>
       <c r="G32">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.16317991631799164</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1396,8 +1396,8 @@
         <v>914</v>
       </c>
       <c r="G33">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.20787746170678337</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1420,8 +1420,8 @@
         <v>905</v>
       </c>
       <c r="G34">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.21878453038674034</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,8 +1444,8 @@
         <v>841</v>
       </c>
       <c r="G35">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.14744351961950058</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1468,8 +1468,8 @@
         <v>2679</v>
       </c>
       <c r="G36">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.11534154535274356</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1492,8 +1492,8 @@
         <v>1547</v>
       </c>
       <c r="G37">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>6.1409179056237877E-2</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1516,8 +1516,8 @@
         <v>1058</v>
       </c>
       <c r="G38">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.780718336483932E-2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1540,8 +1540,8 @@
         <v>645</v>
       </c>
       <c r="G39">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.0155038759689922E-2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1564,8 +1564,8 @@
         <v>296.5</v>
       </c>
       <c r="G40">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.6981450252951095E-2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1588,8 +1588,8 @@
         <v>296.5</v>
       </c>
       <c r="G41">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.6981450252951095E-2</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1612,8 +1612,8 @@
         <v>191</v>
       </c>
       <c r="G42">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.58638743455497377</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1636,8 +1636,8 @@
         <v>693</v>
       </c>
       <c r="G43">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.34920634920634919</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1660,8 +1660,8 @@
         <v>662</v>
       </c>
       <c r="G44">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.2175226586102719</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1684,8 +1684,8 @@
         <v>666</v>
       </c>
       <c r="G45">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1708,8 +1708,8 @@
         <v>2272</v>
       </c>
       <c r="G46">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.16461267605633803</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1732,8 +1732,8 @@
         <v>1400</v>
       </c>
       <c r="G47">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.14499999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1756,8 +1756,8 @@
         <v>982</v>
       </c>
       <c r="G48">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.10183299389002037</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1780,8 +1780,8 @@
         <v>617</v>
       </c>
       <c r="G49" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.14424635332252836</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1806,8 +1806,8 @@
         <v>283.5</v>
       </c>
       <c r="G50" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.13227513227513227</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1832,8 +1832,8 @@
         <v>283.5</v>
       </c>
       <c r="G51" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.13227513227513227</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -1856,8 +1856,8 @@
         <v>8</v>
       </c>
       <c r="G52" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.75</v>
       </c>
       <c r="H52" s="1">
         <v>0.44993750650906073</v>
@@ -1884,8 +1884,8 @@
         <v>63</v>
       </c>
       <c r="G53" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.61904761904761907</v>
       </c>
       <c r="H53" s="1">
         <v>0.49912995181888981</v>
@@ -1912,8 +1912,8 @@
         <v>66</v>
       </c>
       <c r="G54" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5</v>
       </c>
       <c r="H54" s="1">
         <v>0.37937033884025395</v>
@@ -1940,8 +1940,8 @@
         <v>21</v>
       </c>
       <c r="G55" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.2857142857142857</v>
       </c>
       <c r="H55" s="1">
         <v>9.2495929098426521E-2</v>
@@ -1968,8 +1968,8 @@
         <v>35</v>
       </c>
       <c r="G56" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.42857142857142855</v>
       </c>
       <c r="H56" s="1">
         <v>0.26462021631607502</v>
@@ -1996,8 +1996,8 @@
         <v>93</v>
       </c>
       <c r="G57" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.23655913978494625</v>
       </c>
       <c r="H57" s="1">
         <v>0.15018730143155551</v>
@@ -2024,8 +2024,8 @@
         <v>101</v>
       </c>
       <c r="G58" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.21782178217821782</v>
       </c>
       <c r="H58" s="1">
         <v>0.13732122306748479</v>
@@ -2052,8 +2052,8 @@
         <v>84</v>
       </c>
       <c r="G59" s="1">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.19047619047619047</v>
       </c>
       <c r="H59" s="1">
         <v>0.10650088546422966</v>
@@ -2082,8 +2082,8 @@
         <v>5624</v>
       </c>
       <c r="G60">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.0135135135135136E-2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2106,8 +2106,8 @@
         <v>5141</v>
       </c>
       <c r="G61">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>8.8504182065745965E-2</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2130,8 +2130,8 @@
         <v>3643</v>
       </c>
       <c r="G62">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.28191051331320338</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2154,8 +2154,8 @@
         <v>2773</v>
       </c>
       <c r="G63">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.45185719437432381</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2178,8 +2178,8 @@
         <v>1956</v>
       </c>
       <c r="G64">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3721881390593047</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2202,8 +2202,8 @@
         <v>1638</v>
       </c>
       <c r="G65">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.26923076923076922</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -2226,8 +2226,8 @@
         <v>1362</v>
       </c>
       <c r="G66">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.22687224669603523</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2250,8 +2250,8 @@
         <v>5624</v>
       </c>
       <c r="G67">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.3157894736842105E-2</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -2274,8 +2274,8 @@
         <v>5141</v>
       </c>
       <c r="G68">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.10095312196070803</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -2298,8 +2298,8 @@
         <v>3643</v>
       </c>
       <c r="G69">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.33324183365358223</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -2322,8 +2322,8 @@
         <v>2773</v>
       </c>
       <c r="G70" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.44825099170573385</v>
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
@@ -2348,8 +2348,8 @@
         <v>1956</v>
       </c>
       <c r="G71" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3614519427402863</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
@@ -2374,8 +2374,8 @@
         <v>1638</v>
       </c>
       <c r="G72" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.32173382173382176</v>
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
@@ -2400,8 +2400,8 @@
         <v>1362</v>
       </c>
       <c r="G73" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.20851688693098386</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
@@ -2426,8 +2426,8 @@
         <v>5624</v>
       </c>
       <c r="G74" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.2901849217638691E-3</v>
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
@@ -2452,8 +2452,8 @@
         <v>5141</v>
       </c>
       <c r="G75" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>9.0643843610192565E-2</v>
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
@@ -2478,8 +2478,8 @@
         <v>3643</v>
       </c>
       <c r="G76" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.31265440570958003</v>
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
@@ -2504,8 +2504,8 @@
         <v>2773</v>
       </c>
       <c r="G77" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.42372881355932202</v>
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
@@ -2530,8 +2530,8 @@
         <v>1956</v>
       </c>
       <c r="G78" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.41666666666666669</v>
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
@@ -2556,8 +2556,8 @@
         <v>1638</v>
       </c>
       <c r="G79" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.32539682539682541</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
@@ -2582,8 +2582,8 @@
         <v>1362</v>
       </c>
       <c r="G80" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.28928046989721001</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
@@ -2608,8 +2608,8 @@
         <v>5624</v>
       </c>
       <c r="G81" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.0312944523470839E-2</v>
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
@@ -2634,8 +2634,8 @@
         <v>5141</v>
       </c>
       <c r="G82" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.10737210659404785</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
@@ -2660,8 +2660,8 @@
         <v>3643</v>
       </c>
       <c r="G83" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.30359593741421903</v>
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
@@ -2686,8 +2686,8 @@
         <v>2773</v>
       </c>
       <c r="G84" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.40245221781464119</v>
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
@@ -2712,8 +2712,8 @@
         <v>1956</v>
       </c>
       <c r="G85" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.40132924335378323</v>
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
@@ -2738,8 +2738,8 @@
         <v>1638</v>
       </c>
       <c r="G86" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.39560439560439559</v>
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
@@ -2764,8 +2764,8 @@
         <v>1362</v>
       </c>
       <c r="G87" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.28854625550660795</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
@@ -2790,8 +2790,8 @@
         <v>5624</v>
       </c>
       <c r="G88" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.0312944523470839E-2</v>
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
@@ -2816,8 +2816,8 @@
         <v>5141</v>
       </c>
       <c r="G89" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.10834468002334176</v>
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
@@ -2842,8 +2842,8 @@
         <v>3643</v>
       </c>
       <c r="G90" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3085369201207796</v>
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
@@ -2868,8 +2868,8 @@
         <v>2773</v>
       </c>
       <c r="G91" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.38910926794085826</v>
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
@@ -2894,8 +2894,8 @@
         <v>1956</v>
       </c>
       <c r="G92" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.46574642126789367</v>
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
@@ -2920,8 +2920,8 @@
         <v>1638</v>
       </c>
       <c r="G93" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.30525030525030528</v>
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
@@ -2946,8 +2946,8 @@
         <v>1362</v>
       </c>
       <c r="G94" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.27165932452276065</v>
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
@@ -2972,8 +2972,8 @@
         <v>5624</v>
       </c>
       <c r="G95" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>9.2460881934566148E-3</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
@@ -2998,8 +2998,8 @@
         <v>5141</v>
       </c>
       <c r="G96" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.8389418401089289E-2</v>
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
@@ -3024,8 +3024,8 @@
         <v>3643</v>
       </c>
       <c r="G97" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.27724402964589623</v>
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
@@ -3050,8 +3050,8 @@
         <v>2773</v>
       </c>
       <c r="G98" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.45834835917778577</v>
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
@@ -3076,8 +3076,8 @@
         <v>1956</v>
       </c>
       <c r="G99" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.55265848670756645</v>
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
@@ -3102,8 +3102,8 @@
         <v>1638</v>
       </c>
       <c r="G100" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3504273504273504</v>
       </c>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
@@ -3128,8 +3128,8 @@
         <v>1362</v>
       </c>
       <c r="G101" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3656387665198238</v>
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
@@ -3154,8 +3154,8 @@
         <v>5622</v>
       </c>
       <c r="G102" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>9.8719316969050161E-2</v>
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
@@ -3180,8 +3180,8 @@
         <v>5489</v>
       </c>
       <c r="G103" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.32738203680087447</v>
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
@@ -3206,8 +3206,8 @@
         <v>3869</v>
       </c>
       <c r="G104" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.50581545619023005</v>
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
@@ -3232,8 +3232,8 @@
         <v>3174</v>
       </c>
       <c r="G105" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.4732199117832388</v>
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
@@ -3258,8 +3258,8 @@
         <v>2404</v>
       </c>
       <c r="G106" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.35108153078202997</v>
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
@@ -3284,8 +3284,8 @@
         <v>2075</v>
       </c>
       <c r="G107" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.26024096385542167</v>
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
@@ -3310,8 +3310,8 @@
         <v>1829</v>
       </c>
       <c r="G108" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.21159103335155824</v>
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
@@ -3336,8 +3336,8 @@
         <v>5622</v>
       </c>
       <c r="G109" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.6663109213802913E-2</v>
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
@@ -3362,8 +3362,8 @@
         <v>5489</v>
       </c>
       <c r="G110" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.32683548916013844</v>
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
@@ -3388,8 +3388,8 @@
         <v>3869</v>
       </c>
       <c r="G111" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.50193848539674335</v>
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
@@ -3414,8 +3414,8 @@
         <v>3174</v>
       </c>
       <c r="G112" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.44990548204158792</v>
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
@@ -3440,8 +3440,8 @@
         <v>2404</v>
       </c>
       <c r="G113" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3781198003327787</v>
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
@@ -3466,8 +3466,8 @@
         <v>2075</v>
       </c>
       <c r="G114" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.25156626506024099</v>
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
@@ -3492,8 +3492,8 @@
         <v>1829</v>
       </c>
       <c r="G115" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.20229633679606343</v>
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
@@ -3518,8 +3518,8 @@
         <v>5622</v>
       </c>
       <c r="G116" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>8.6979722518676625E-2</v>
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
@@ -3544,8 +3544,8 @@
         <v>5489</v>
       </c>
       <c r="G117" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.31554017125159411</v>
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
@@ -3570,8 +3570,8 @@
         <v>3869</v>
       </c>
       <c r="G118" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.46627035409666578</v>
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
@@ -3596,8 +3596,8 @@
         <v>3174</v>
       </c>
       <c r="G119" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.47416509136735979</v>
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
@@ -3622,8 +3622,8 @@
         <v>2404</v>
       </c>
       <c r="G120" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3639767054908486</v>
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
@@ -3648,8 +3648,8 @@
         <v>2075</v>
       </c>
       <c r="G121" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.25542168674698795</v>
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
@@ -3674,8 +3674,8 @@
         <v>1829</v>
       </c>
       <c r="G122" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.17495899398578457</v>
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
@@ -3700,8 +3700,8 @@
         <v>5622</v>
       </c>
       <c r="G123" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>9.3738882959800776E-2</v>
       </c>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
@@ -3726,8 +3726,8 @@
         <v>5489</v>
       </c>
       <c r="G124" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.32665330661322645</v>
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
@@ -3752,8 +3752,8 @@
         <v>3869</v>
       </c>
       <c r="G125" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.52261566296200568</v>
       </c>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
@@ -3778,8 +3778,8 @@
         <v>3174</v>
       </c>
       <c r="G126" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.48109640831758033</v>
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
@@ -3804,8 +3804,8 @@
         <v>2404</v>
       </c>
       <c r="G127" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.37354409317803661</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
@@ -3830,8 +3830,8 @@
         <v>2075</v>
       </c>
       <c r="G128" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.33638554216867472</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
@@ -3856,8 +3856,8 @@
         <v>1829</v>
       </c>
       <c r="G129" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.19737561509021323</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
@@ -3882,8 +3882,8 @@
         <v>5622</v>
       </c>
       <c r="G130" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>9.4450373532550688E-2</v>
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
@@ -3908,8 +3908,8 @@
         <v>5489</v>
       </c>
       <c r="G131" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.30916378210967388</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
@@ -3934,8 +3934,8 @@
         <v>3869</v>
       </c>
       <c r="G132" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.51512018609459809</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
@@ -3960,8 +3960,8 @@
         <v>3174</v>
       </c>
       <c r="G133" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
@@ -3986,8 +3986,8 @@
         <v>2404</v>
       </c>
       <c r="G134" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.40266222961730447</v>
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
@@ -4012,8 +4012,8 @@
         <v>2075</v>
       </c>
       <c r="G135" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.3378313253012048</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
@@ -4038,8 +4038,8 @@
         <v>1829</v>
       </c>
       <c r="G136" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.26845270639693819</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
@@ -4064,8 +4064,8 @@
         <v>5622</v>
       </c>
       <c r="G137" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.1104589114194237</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
@@ -4090,8 +4090,8 @@
         <v>5489</v>
       </c>
       <c r="G138" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.32683548916013844</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
@@ -4116,8 +4116,8 @@
         <v>3869</v>
       </c>
       <c r="G139" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.49004910829671749</v>
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
@@ -4142,8 +4142,8 @@
         <v>3174</v>
       </c>
       <c r="G140" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.53308128544423439</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
@@ -4168,8 +4168,8 @@
         <v>2404</v>
       </c>
       <c r="G141" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.44550748752079866</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
@@ -4194,8 +4194,8 @@
         <v>2075</v>
       </c>
       <c r="G142" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.37493975903614457</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
@@ -4220,8 +4220,8 @@
         <v>1829</v>
       </c>
       <c r="G143" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.27063969382176051</v>
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
@@ -4246,8 +4246,8 @@
         <v>48</v>
       </c>
       <c r="G144" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.75</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
@@ -4272,8 +4272,8 @@
         <v>221</v>
       </c>
       <c r="G145" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.60633484162895923</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -4298,8 +4298,8 @@
         <v>243</v>
       </c>
       <c r="G146" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5967078189300411</v>
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
@@ -4324,8 +4324,8 @@
         <v>175</v>
       </c>
       <c r="G147" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5485714285714286</v>
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
@@ -4350,8 +4350,8 @@
         <v>407</v>
       </c>
       <c r="G148" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.46437346437346438</v>
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
@@ -4376,8 +4376,8 @@
         <v>147</v>
       </c>
       <c r="G149" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.42176870748299322</v>
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
@@ -4402,8 +4402,8 @@
         <v>76</v>
       </c>
       <c r="G150" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.43421052631578949</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
@@ -4428,8 +4428,8 @@
         <v>28</v>
       </c>
       <c r="G151" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5357142857142857</v>
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
@@ -4454,8 +4454,8 @@
         <v>26</v>
       </c>
       <c r="G152" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.34615384615384615</v>
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
@@ -4480,8 +4480,8 @@
         <v>191</v>
       </c>
       <c r="G153" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.60209424083769636</v>
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
@@ -4506,8 +4506,8 @@
         <v>693</v>
       </c>
       <c r="G154" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.37662337662337664</v>
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
@@ -4532,8 +4532,8 @@
         <v>662</v>
       </c>
       <c r="G155" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.23867069486404835</v>
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
@@ -4558,8 +4558,8 @@
         <v>666</v>
       </c>
       <c r="G156" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.20270270270270271</v>
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
@@ -4584,8 +4584,8 @@
         <v>2272</v>
       </c>
       <c r="G157" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.1932218309859155</v>
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
@@ -4610,8 +4610,8 @@
         <v>1400</v>
       </c>
       <c r="G158" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.17642857142857143</v>
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
@@ -4636,8 +4636,8 @@
         <v>982</v>
       </c>
       <c r="G159" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.13238289205702647</v>
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
@@ -4662,8 +4662,8 @@
         <v>617</v>
       </c>
       <c r="G160" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.16531604538087522</v>
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
@@ -4688,8 +4688,8 @@
         <v>567</v>
       </c>
       <c r="G161" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>0</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.14638447971781304</v>
       </c>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
@@ -4714,8 +4714,8 @@
         <v>48</v>
       </c>
       <c r="G162" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.0125000000000001E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.125</v>
       </c>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
@@ -4746,8 +4746,8 @@
         <v>221</v>
       </c>
       <c r="G163" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>8.742081447963802E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>5.4298642533936653E-2</v>
       </c>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
@@ -4775,8 +4775,8 @@
         <v>243</v>
       </c>
       <c r="G164" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.0539094650205762E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.12757201646090535</v>
       </c>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
@@ -4804,8 +4804,8 @@
         <v>175</v>
       </c>
       <c r="G165" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>1.9902857142857142E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.15428571428571428</v>
       </c>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
@@ -4833,8 +4833,8 @@
         <v>407</v>
       </c>
       <c r="G166" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>1.0459459459459461E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>8.1081081081081086E-2</v>
       </c>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
@@ -4862,8 +4862,8 @@
         <v>147</v>
       </c>
       <c r="G167" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>1.8122448979591838E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>5.4421768707482991E-2</v>
       </c>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
@@ -4891,8 +4891,8 @@
         <v>76</v>
       </c>
       <c r="G168" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.6289473684210526E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
@@ -4920,8 +4920,8 @@
         <v>28</v>
       </c>
       <c r="G169" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.3785714285714285E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
@@ -4950,8 +4950,8 @@
         <v>13</v>
       </c>
       <c r="G170" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.561538461538462E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
@@ -4980,8 +4980,8 @@
         <v>13</v>
       </c>
       <c r="G171" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.561538461538462E-2</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
@@ -5009,8 +5009,8 @@
         <v>191</v>
       </c>
       <c r="G172" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.1361256544502618E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.5706806282722512E-2</v>
       </c>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
@@ -5038,8 +5038,8 @@
         <v>693</v>
       </c>
       <c r="G173" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>3.7287157287157289E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.7417027417027416E-2</v>
       </c>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
@@ -5067,8 +5067,8 @@
         <v>662</v>
       </c>
       <c r="G174" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>2.8761329305135954E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.1148036253776436E-2</v>
       </c>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
@@ -5096,8 +5096,8 @@
         <v>666</v>
       </c>
       <c r="G175" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>7.4954954954954949E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.6036036036036036E-2</v>
       </c>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
@@ -5125,8 +5125,8 @@
         <v>2272</v>
       </c>
       <c r="G176" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>5.9507042253521122E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.8609154929577465E-2</v>
       </c>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
@@ -5154,8 +5154,8 @@
         <v>1400</v>
       </c>
       <c r="G177" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>9.0828571428571425E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.1428571428571431E-2</v>
       </c>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
@@ -5183,8 +5183,8 @@
         <v>982</v>
       </c>
       <c r="G178" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>8.8289205702647647E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>3.0549898167006109E-2</v>
       </c>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
@@ -5212,8 +5212,8 @@
         <v>617</v>
       </c>
       <c r="G179" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>6.0891410048622358E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>2.1069692058346839E-2</v>
       </c>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
@@ -5242,8 +5242,8 @@
         <v>283.5</v>
       </c>
       <c r="G180" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>4.0776014109347438E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.4109347442680775E-2</v>
       </c>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
@@ -5272,8 +5272,8 @@
         <v>283.5</v>
       </c>
       <c r="G181" s="6">
-        <f>Table1[Pos]/Table1[N]*Table1[[#This Row],[Column1]]</f>
-        <v>4.0776014109347438E-3</v>
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>1.4109347442680775E-2</v>
       </c>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>

</xml_diff>

<commit_message>
Fixing type in likeFun.m where hpv_hiv_2008 was used instead of hpv_hivNeg_2008. Swapping HIV+ and HIV- data for HPV prevalence in women (no CIN2/3) by HIV status. Adding calibration to HPV prevalence in males by HIV status.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -271,13 +271,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,11 +302,11 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="0">
+    <tableColumn id="4" name="Mean" dataDxfId="2">
       <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="2"/>
-    <tableColumn id="6" name="UB" dataDxfId="1"/>
+    <tableColumn id="5" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" name="UB" dataDxfId="0"/>
     <tableColumn id="8" name="Column1"/>
     <tableColumn id="11" name="Column2"/>
   </tableColumns>
@@ -579,21 +579,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" customWidth="1"/>
+    <col min="11" max="11" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -628,7 +628,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -676,7 +676,7 @@
         <v>5.4298642533936653E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -700,7 +700,7 @@
         <v>0.12757201646090535</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -724,7 +724,7 @@
         <v>0.15428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -748,7 +748,7 @@
         <v>8.1081081081081086E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -772,7 +772,7 @@
         <v>5.4421768707482991E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -796,7 +796,7 @@
         <v>7.8947368421052627E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -820,7 +820,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -845,7 +845,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -870,7 +870,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -894,7 +894,7 @@
         <v>1.5706806282722512E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -918,7 +918,7 @@
         <v>2.7417027417027416E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -942,7 +942,7 @@
         <v>2.1148036253776436E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -966,7 +966,7 @@
         <v>3.6036036036036036E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -990,7 +990,7 @@
         <v>2.8609154929577465E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>3.1428571428571431E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>3.0549898167006109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>2.1069692058346839E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>1.4109347442680775E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>1.4109347442680775E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>0.16317991631799164</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>0.20787746170678337</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>0.21878453038674034</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0.14744351961950058</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0.11534154535274356</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>6.1409179056237877E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>3.780718336483932E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>2.0155038759689922E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1352,9 +1352,9 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
@@ -1376,9 +1376,9 @@
         <v>0.16317991631799164</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
@@ -1400,9 +1400,9 @@
         <v>0.20787746170678337</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>29</v>
@@ -1424,9 +1424,9 @@
         <v>0.21878453038674034</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>29</v>
@@ -1448,9 +1448,9 @@
         <v>0.14744351961950058</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>29</v>
@@ -1472,9 +1472,9 @@
         <v>0.11534154535274356</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>29</v>
@@ -1496,9 +1496,9 @@
         <v>6.1409179056237877E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>29</v>
@@ -1520,9 +1520,9 @@
         <v>3.780718336483932E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>29</v>
@@ -1544,9 +1544,9 @@
         <v>2.0155038759689922E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>29</v>
@@ -1568,9 +1568,9 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>29</v>
@@ -1592,9 +1592,9 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>29</v>
@@ -1616,9 +1616,9 @@
         <v>0.58638743455497377</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>29</v>
@@ -1640,9 +1640,9 @@
         <v>0.34920634920634919</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>29</v>
@@ -1664,9 +1664,9 @@
         <v>0.2175226586102719</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>29</v>
@@ -1688,9 +1688,9 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>29</v>
@@ -1712,9 +1712,9 @@
         <v>0.16461267605633803</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>29</v>
@@ -1736,9 +1736,9 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>29</v>
@@ -1760,9 +1760,9 @@
         <v>0.10183299389002037</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>29</v>
@@ -1786,9 +1786,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
@@ -1812,9 +1812,9 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>29</v>
@@ -1838,7 +1838,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>0.73896528627634828</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>0.62062966115974605</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>0.47893264233014488</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>36</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0.59252264082678208</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>36</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>0.32293097813833699</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>36</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>0.29832234128895085</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>36</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>0.27445149548815129</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>1.0135135135135136E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>40</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>8.8504182065745965E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>40</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0.28191051331320338</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>40</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.45185719437432381</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0.3721881390593047</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>40</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>0.26923076923076922</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>0.22687224669603523</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>41</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0.10095312196070803</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>41</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>0.33324183365358223</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>41</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>41</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>41</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>41</v>
       </c>
@@ -2406,7 +2406,7 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>42</v>
       </c>
@@ -2458,7 +2458,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>42</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>42</v>
       </c>
@@ -2510,7 +2510,7 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>42</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>42</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
@@ -2614,7 +2614,7 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>43</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>43</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>43</v>
       </c>
@@ -2718,7 +2718,7 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>43</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>43</v>
       </c>
@@ -2770,7 +2770,7 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>44</v>
       </c>
@@ -2796,7 +2796,7 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>44</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>44</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>44</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>44</v>
       </c>
@@ -2900,7 +2900,7 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>44</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>44</v>
       </c>
@@ -2952,7 +2952,7 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>45</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>45</v>
       </c>
@@ -3004,7 +3004,7 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>45</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>45</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>45</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>45</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>45</v>
       </c>
@@ -3134,7 +3134,7 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>46</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>46</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>46</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>46</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>46</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>46</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>46</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>47</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>47</v>
       </c>
@@ -3394,7 +3394,7 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>47</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>47</v>
       </c>
@@ -3446,7 +3446,7 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>47</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>47</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>48</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>48</v>
       </c>
@@ -3550,7 +3550,7 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>48</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>48</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>48</v>
       </c>
@@ -3628,7 +3628,7 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>48</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>48</v>
       </c>
@@ -3680,7 +3680,7 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>49</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>49</v>
       </c>
@@ -3732,7 +3732,7 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>49</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -3784,7 +3784,7 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>49</v>
       </c>
@@ -3810,7 +3810,7 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>49</v>
       </c>
@@ -3836,7 +3836,7 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>49</v>
       </c>
@@ -3862,7 +3862,7 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>50</v>
       </c>
@@ -3888,7 +3888,7 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>50</v>
       </c>
@@ -3914,7 +3914,7 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>50</v>
       </c>
@@ -3940,7 +3940,7 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>50</v>
       </c>
@@ -3966,7 +3966,7 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>50</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>50</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>50</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>51</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>51</v>
       </c>
@@ -4096,7 +4096,7 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>51</v>
       </c>
@@ -4122,7 +4122,7 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>51</v>
       </c>
@@ -4148,7 +4148,7 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>51</v>
       </c>
@@ -4174,7 +4174,7 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>51</v>
       </c>
@@ -4200,7 +4200,7 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>51</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>55</v>
       </c>
@@ -4252,7 +4252,7 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>55</v>
       </c>
@@ -4278,7 +4278,7 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>55</v>
       </c>
@@ -4304,7 +4304,7 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>55</v>
       </c>
@@ -4330,7 +4330,7 @@
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>55</v>
       </c>
@@ -4356,7 +4356,7 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>55</v>
       </c>
@@ -4382,7 +4382,7 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>55</v>
       </c>
@@ -4408,7 +4408,7 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>55</v>
       </c>
@@ -4434,7 +4434,7 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>55</v>
       </c>
@@ -4460,7 +4460,7 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>57</v>
       </c>
@@ -4486,7 +4486,7 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>57</v>
       </c>
@@ -4512,7 +4512,7 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>57</v>
       </c>
@@ -4538,7 +4538,7 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>57</v>
       </c>
@@ -4564,7 +4564,7 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>57</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>57</v>
       </c>
@@ -4616,7 +4616,7 @@
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>57</v>
       </c>
@@ -4642,7 +4642,7 @@
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>57</v>
       </c>
@@ -4668,7 +4668,7 @@
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>57</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
     </row>
-    <row r="162" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>59</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>59</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>59</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>59</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>59</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>59</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>59</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>59</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>59</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>59</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>60</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>60</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>60</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>60</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>60</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>60</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>60</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>60</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>60</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>60</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Calibration_targets.xlsx with additional reference info, usage status, and pending questions for use in model calibration.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="68">
   <si>
     <t>N</t>
   </si>
@@ -119,9 +119,6 @@
     <t>HR HPV Prevalence in HIV+ Men</t>
   </si>
   <si>
-    <t>Mbulawa</t>
-  </si>
-  <si>
     <t>18-25</t>
   </si>
   <si>
@@ -194,28 +191,43 @@
     <t>HPV Prevalence in HIV+ Women (all)</t>
   </si>
   <si>
-    <t>McDonald</t>
-  </si>
-  <si>
     <t>HPV Prevalence in HIV- Women (all)</t>
   </si>
   <si>
-    <t>McDonald 2014</t>
-  </si>
-  <si>
-    <t>CIN2/CIN3 Prevalence HPV16 (HIV+)</t>
-  </si>
-  <si>
-    <t>CIN2/CIN3 Prevalence HPV16 (HIV-)</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Proportion of HPV infections that were HPV16 among women with CIN2/CIN3</t>
+    <t>McDonald (2014) Front Oncol. "Distribution of Human Papillomavirus Genotypes among HIV-Positive and HIV-Negative Women in Cape Town, South Africa</t>
+  </si>
+  <si>
+    <t>McDonald (2014) Front Oncol.</t>
+  </si>
+  <si>
+    <t>Usage Status</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Mbulawa (2015) BMC Infect Dis. "Human papillomavirus prevalence in South African women and men according to age and human immunodeficiency virus status</t>
+  </si>
+  <si>
+    <t>Mbulawa (2015) BMC Infect Dis.</t>
+  </si>
+  <si>
+    <t>Africa Centre cohort (now on AHRI) for KZN. Can access the HIV prevalence estimates by putting in a data request ("ACDIS:HIV Surveillance 2010-2016.Release 2016-12").</t>
+  </si>
+  <si>
+    <t>Reference unverified. Reference found does not stratify by HIV status. Looks like the HIV+ and HIV- values were swapped. The following references support that these values were swapped: McDonald et al. 2014; Adebamowo et al. 2017; De Vuyst et al. 2011</t>
+  </si>
+  <si>
+    <t>What year of data in our model should we compare to…2006? Were persons on ART included in this analysis? If so, were they considered HIV+?</t>
+  </si>
+  <si>
+    <t>What year of data in our model should we compare to…2009? Were persons on ART included in this analysis? If so, were they considered HIV+?</t>
+  </si>
+  <si>
+    <t>Check whether these values came from the 2014 or 2012 paper.  What year of data in our model should we compare to…2006? Were persons on ART included in this analysis? If so, were they considered HIV+?</t>
   </si>
 </sst>
 </file>
@@ -251,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,19 +277,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,13 +317,13 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="0">
+    <tableColumn id="4" name="Mean" dataDxfId="2">
       <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="2"/>
-    <tableColumn id="6" name="UB" dataDxfId="1"/>
-    <tableColumn id="8" name="Column1"/>
-    <tableColumn id="11" name="Column2"/>
+    <tableColumn id="5" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" name="UB" dataDxfId="0"/>
+    <tableColumn id="8" name="Usage Status"/>
+    <tableColumn id="11" name="Questions"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,21 +594,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" customWidth="1"/>
+    <col min="11" max="11" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -604,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -616,24 +632,24 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -651,13 +667,19 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -675,13 +697,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>5.4298642533936653E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -699,13 +724,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.12757201646090535</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -723,13 +751,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.15428571428571428</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -747,13 +778,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>8.1081081081081086E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -771,13 +805,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>5.4421768707482991E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -795,13 +832,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.8947368421052627E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -819,13 +859,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.1428571428571425E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -844,13 +887,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.6923076923076927E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
@@ -869,13 +915,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.6923076923076927E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -893,13 +942,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.5706806282722512E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -917,13 +969,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.7417027417027416E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -941,13 +996,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.1148036253776436E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -965,13 +1023,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.6036036036036036E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -989,13 +1050,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.8609154929577465E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1013,13 +1077,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.1428571428571431E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
@@ -1037,13 +1104,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.0549898167006109E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -1061,13 +1131,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.1069692058346839E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
@@ -1086,13 +1159,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.4109347442680775E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
@@ -1111,8 +1187,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.4109347442680775E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1135,8 +1214,14 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16317991631799164</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1159,8 +1244,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.20787746170678337</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1183,8 +1271,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.21878453038674034</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1207,8 +1298,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14744351961950058</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1231,8 +1325,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.11534154535274356</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1255,8 +1352,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>6.1409179056237877E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1279,8 +1379,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.780718336483932E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1303,8 +1406,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.0155038759689922E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1327,8 +1433,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1351,8 +1460,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1375,8 +1487,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16317991631799164</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1399,8 +1514,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.20787746170678337</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -1423,8 +1541,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.21878453038674034</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -1447,8 +1568,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14744351961950058</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -1471,8 +1595,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.11534154535274356</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1495,8 +1622,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>6.1409179056237877E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1519,8 +1649,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.780718336483932E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -1543,8 +1676,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.0155038759689922E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1567,8 +1703,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -1591,8 +1730,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1615,8 +1757,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.58638743455497377</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1639,8 +1784,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.34920634920634919</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -1663,8 +1811,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.2175226586102719</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -1687,8 +1838,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1711,8 +1865,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16461267605633803</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -1735,8 +1892,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14499999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
@@ -1759,8 +1919,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.10183299389002037</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
@@ -1785,8 +1948,11 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
@@ -1811,8 +1977,11 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -1837,16 +2006,19 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="5">
@@ -1865,16 +2037,22 @@
       <c r="I52" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>60</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="5">
@@ -1893,16 +2071,19 @@
       <c r="I53" s="1">
         <v>0.73896528627634828</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="5">
@@ -1921,16 +2102,19 @@
       <c r="I54" s="1">
         <v>0.62062966115974605</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="5">
@@ -1949,16 +2133,19 @@
       <c r="I55" s="1">
         <v>0.47893264233014488</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="5">
@@ -1977,16 +2164,19 @@
       <c r="I56" s="1">
         <v>0.59252264082678208</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="5">
@@ -2005,16 +2195,19 @@
       <c r="I57" s="1">
         <v>0.32293097813833699</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="5">
@@ -2033,16 +2226,19 @@
       <c r="I58" s="1">
         <v>0.29832234128895085</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="5">
@@ -2061,13 +2257,16 @@
       <c r="I59" s="1">
         <v>0.27445149548815129</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -2085,13 +2284,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.0135135135135136E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -2109,13 +2311,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>8.8504182065745965E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -2133,13 +2338,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.28191051331320338</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
@@ -2157,13 +2365,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.45185719437432381</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -2181,13 +2392,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.3721881390593047</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -2205,13 +2419,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.26923076923076922</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
@@ -2229,13 +2446,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.22687224669603523</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
@@ -2253,13 +2473,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.3157894736842105E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2277,13 +2500,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.10095312196070803</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
@@ -2301,13 +2527,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.33324183365358223</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -2327,13 +2556,16 @@
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -2353,13 +2585,16 @@
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -2379,13 +2614,16 @@
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
@@ -2405,13 +2643,16 @@
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -2431,13 +2672,16 @@
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -2457,13 +2701,16 @@
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -2483,13 +2730,16 @@
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
@@ -2509,13 +2759,16 @@
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -2535,13 +2788,16 @@
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -2561,13 +2817,16 @@
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C80" t="s">
         <v>10</v>
@@ -2587,13 +2846,16 @@
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -2613,13 +2875,16 @@
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2639,13 +2904,16 @@
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
@@ -2665,13 +2933,16 @@
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -2691,13 +2962,16 @@
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -2717,13 +2991,16 @@
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
@@ -2743,13 +3020,16 @@
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
@@ -2769,13 +3049,16 @@
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -2795,13 +3078,16 @@
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2821,13 +3107,16 @@
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
@@ -2847,13 +3136,16 @@
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -2873,13 +3165,16 @@
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -2899,13 +3194,16 @@
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2925,13 +3223,16 @@
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
@@ -2951,13 +3252,16 @@
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C95" t="s">
         <v>4</v>
@@ -2977,13 +3281,16 @@
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -3003,13 +3310,16 @@
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -3029,13 +3339,16 @@
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -3055,13 +3368,16 @@
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -3081,13 +3397,16 @@
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
@@ -3107,13 +3426,16 @@
       </c>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -3133,13 +3455,16 @@
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
@@ -3159,13 +3484,16 @@
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -3185,13 +3513,16 @@
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -3211,13 +3542,16 @@
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -3237,13 +3571,16 @@
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -3263,13 +3600,16 @@
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -3289,13 +3629,16 @@
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -3315,13 +3658,16 @@
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
@@ -3341,13 +3687,16 @@
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
@@ -3367,13 +3716,16 @@
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
@@ -3393,13 +3745,16 @@
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
@@ -3419,13 +3774,16 @@
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -3445,13 +3803,16 @@
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -3471,13 +3832,16 @@
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -3497,13 +3861,16 @@
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -3523,13 +3890,16 @@
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -3549,13 +3919,16 @@
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -3575,13 +3948,16 @@
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -3601,13 +3977,16 @@
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -3627,13 +4006,16 @@
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -3653,13 +4035,16 @@
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -3679,13 +4064,16 @@
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C123" t="s">
         <v>4</v>
@@ -3705,13 +4093,16 @@
       </c>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -3731,13 +4122,16 @@
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
@@ -3757,13 +4151,16 @@
       </c>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C126" t="s">
         <v>7</v>
@@ -3783,13 +4180,16 @@
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -3809,13 +4209,16 @@
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -3835,13 +4238,16 @@
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C129" t="s">
         <v>10</v>
@@ -3861,13 +4267,16 @@
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -3887,13 +4296,16 @@
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -3913,13 +4325,16 @@
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
@@ -3939,13 +4354,16 @@
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -3965,13 +4383,16 @@
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -3991,13 +4412,16 @@
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
@@ -4017,13 +4441,16 @@
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C136" t="s">
         <v>10</v>
@@ -4043,13 +4470,16 @@
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
@@ -4069,13 +4499,16 @@
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C138" t="s">
         <v>5</v>
@@ -4095,13 +4528,16 @@
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C139" t="s">
         <v>6</v>
@@ -4121,13 +4557,16 @@
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -4147,13 +4586,16 @@
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -4173,13 +4615,16 @@
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -4199,13 +4644,16 @@
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C143" t="s">
         <v>10</v>
@@ -4225,16 +4673,19 @@
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>55</v>
-      </c>
-      <c r="B144" t="s">
+        <v>54</v>
+      </c>
+      <c r="B144" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C144" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D144">
         <v>2014</v>
@@ -4251,13 +4702,19 @@
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" t="s">
+        <v>60</v>
+      </c>
+      <c r="K144" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>55</v>
-      </c>
-      <c r="B145" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -4277,13 +4734,16 @@
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>55</v>
-      </c>
-      <c r="B146" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -4303,13 +4763,16 @@
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>55</v>
-      </c>
-      <c r="B147" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -4329,13 +4792,16 @@
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>55</v>
-      </c>
-      <c r="B148" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -4355,13 +4821,16 @@
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>55</v>
-      </c>
-      <c r="B149" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -4381,13 +4850,16 @@
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>55</v>
-      </c>
-      <c r="B150" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C150" t="s">
         <v>10</v>
@@ -4407,13 +4879,16 @@
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>55</v>
-      </c>
-      <c r="B151" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C151" t="s">
         <v>11</v>
@@ -4433,16 +4908,19 @@
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>55</v>
-      </c>
-      <c r="B152" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C152" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D152">
         <v>2014</v>
@@ -4459,16 +4937,19 @@
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
+        <v>55</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B153" t="s">
-        <v>56</v>
-      </c>
       <c r="C153" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D153">
         <v>2014</v>
@@ -4485,13 +4966,16 @@
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
+        <v>55</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B154" t="s">
-        <v>56</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>
@@ -4511,13 +4995,16 @@
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B155" t="s">
-        <v>56</v>
       </c>
       <c r="C155" t="s">
         <v>6</v>
@@ -4537,13 +5024,16 @@
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
+        <v>55</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B156" t="s">
-        <v>56</v>
       </c>
       <c r="C156" t="s">
         <v>7</v>
@@ -4563,13 +5053,16 @@
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>55</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B157" t="s">
-        <v>56</v>
       </c>
       <c r="C157" t="s">
         <v>8</v>
@@ -4589,13 +5082,16 @@
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
+        <v>55</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B158" t="s">
-        <v>56</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
@@ -4615,13 +5111,16 @@
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>55</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B159" t="s">
-        <v>56</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
@@ -4641,13 +5140,16 @@
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>55</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B160" t="s">
-        <v>56</v>
       </c>
       <c r="C160" t="s">
         <v>11</v>
@@ -4667,16 +5169,19 @@
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J160" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>55</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B161" t="s">
-        <v>56</v>
-      </c>
       <c r="C161" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D161">
         <v>2014</v>
@@ -4693,595 +5198,232 @@
       </c>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
-    </row>
-    <row r="162" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D162" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E162" s="1">
-        <v>6</v>
-      </c>
-      <c r="F162" s="1">
-        <v>48</v>
-      </c>
-      <c r="G162" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.125</v>
-      </c>
+      <c r="J161" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="6"/>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
-      <c r="J162">
-        <v>0.161</v>
-      </c>
-      <c r="K162" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D163" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E163" s="1">
-        <v>12</v>
-      </c>
-      <c r="F163" s="1">
-        <v>221</v>
-      </c>
-      <c r="G163" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4298642533936653E-2</v>
-      </c>
+      <c r="K162" s="8"/>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="6"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
-      <c r="J163">
-        <v>0.161</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D164" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E164" s="1">
-        <v>31</v>
-      </c>
-      <c r="F164" s="1">
-        <v>243</v>
-      </c>
-      <c r="G164" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.12757201646090535</v>
-      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="6"/>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
-      <c r="J164">
-        <v>0.161</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D165" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E165" s="1">
-        <v>27</v>
-      </c>
-      <c r="F165" s="1">
-        <v>175</v>
-      </c>
-      <c r="G165" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.15428571428571428</v>
-      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="6"/>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
-      <c r="J165">
-        <v>0.129</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D166" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E166" s="1">
-        <v>33</v>
-      </c>
-      <c r="F166" s="1">
-        <v>407</v>
-      </c>
-      <c r="G166" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>8.1081081081081086E-2</v>
-      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="6"/>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
-      <c r="J166">
-        <v>0.129</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D167" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E167" s="1">
-        <v>8</v>
-      </c>
-      <c r="F167" s="1">
-        <v>147</v>
-      </c>
-      <c r="G167" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4421768707482991E-2</v>
-      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="6"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
-      <c r="J167">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D168" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E168" s="1">
-        <v>6</v>
-      </c>
-      <c r="F168" s="1">
-        <v>76</v>
-      </c>
-      <c r="G168" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.8947368421052627E-2</v>
-      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="6"/>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
-      <c r="J168">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D169" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E169" s="1">
-        <v>2</v>
-      </c>
-      <c r="F169" s="1">
-        <v>28</v>
-      </c>
-      <c r="G169" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="6"/>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
-      <c r="J169">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D170" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E170" s="1">
-        <v>1</v>
-      </c>
-      <c r="F170" s="1">
-        <f>26/2</f>
-        <v>13</v>
-      </c>
-      <c r="G170" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="6"/>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
-      <c r="J170">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D171" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E171" s="1">
-        <v>1</v>
-      </c>
-      <c r="F171" s="1">
-        <f>26/2</f>
-        <v>13</v>
-      </c>
-      <c r="G171" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="6"/>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
-      <c r="J171">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D172" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E172" s="1">
-        <v>3</v>
-      </c>
-      <c r="F172" s="1">
-        <v>191</v>
-      </c>
-      <c r="G172" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.5706806282722512E-2</v>
-      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="6"/>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
-      <c r="J172">
-        <v>0.13600000000000001</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D173" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E173" s="1">
-        <v>19</v>
-      </c>
-      <c r="F173" s="1">
-        <v>693</v>
-      </c>
-      <c r="G173" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.7417027417027416E-2</v>
-      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="6"/>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
-      <c r="J173">
-        <v>0.13600000000000001</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D174" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E174" s="1">
-        <v>14</v>
-      </c>
-      <c r="F174" s="1">
-        <v>662</v>
-      </c>
-      <c r="G174" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1148036253776436E-2</v>
-      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="6"/>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
-      <c r="J174">
-        <v>0.13600000000000001</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D175" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E175" s="1">
-        <v>24</v>
-      </c>
-      <c r="F175" s="1">
-        <v>666</v>
-      </c>
-      <c r="G175" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.6036036036036036E-2</v>
-      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="6"/>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
-      <c r="J175">
-        <v>0.20799999999999999</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D176" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E176" s="1">
-        <v>65</v>
-      </c>
-      <c r="F176" s="4">
-        <v>2272</v>
-      </c>
-      <c r="G176" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.8609154929577465E-2</v>
-      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="6"/>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
-      <c r="J176">
-        <v>0.20799999999999999</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D177" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E177" s="1">
-        <v>44</v>
-      </c>
-      <c r="F177" s="4">
-        <v>1400</v>
-      </c>
-      <c r="G177" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.1428571428571431E-2</v>
-      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="6"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
-      <c r="J177">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D178" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E178" s="1">
-        <v>30</v>
-      </c>
-      <c r="F178" s="1">
-        <v>982</v>
-      </c>
-      <c r="G178" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.0549898167006109E-2</v>
-      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="6"/>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
-      <c r="J178">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D179" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E179" s="1">
-        <v>13</v>
-      </c>
-      <c r="F179" s="1">
-        <v>617</v>
-      </c>
-      <c r="G179" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1069692058346839E-2</v>
-      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="6"/>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
-      <c r="J179">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D180" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E180" s="1">
-        <v>4</v>
-      </c>
-      <c r="F180" s="1">
-        <f>567/2</f>
-        <v>283.5</v>
-      </c>
-      <c r="G180" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
-      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="6"/>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
-      <c r="J180">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D181" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E181" s="1">
-        <v>4</v>
-      </c>
-      <c r="F181" s="1">
-        <f>567/2</f>
-        <v>283.5</v>
-      </c>
-      <c r="G181" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
-      </c>
+    </row>
+    <row r="181" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="6"/>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
-      <c r="J181">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="182" spans="1:9" ht="29.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pulled in Calibration_targets Excel sheet from master branch with updated references, usage status, and pending questions. Not using Allan data for calibration. In likeFun, ART consistentlyl classified as HIV+, not HIV-. Updated comparison years in likeFun to match years of study population in paper (McDonald: 2006, Mbulawa: 2009). Removed HPV16 data as a data load option in loadUp.m.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -271,13 +271,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,11 +302,11 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="2">
+    <tableColumn id="4" name="Mean" dataDxfId="0">
       <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="1"/>
-    <tableColumn id="6" name="UB" dataDxfId="0"/>
+    <tableColumn id="5" name="LB" dataDxfId="2"/>
+    <tableColumn id="6" name="UB" dataDxfId="1"/>
     <tableColumn id="8" name="Column1"/>
     <tableColumn id="11" name="Column2"/>
   </tableColumns>
@@ -579,21 +579,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" customWidth="1"/>
-    <col min="11" max="11" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -628,7 +628,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -676,7 +676,7 @@
         <v>5.4298642533936653E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -700,7 +700,7 @@
         <v>0.12757201646090535</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -724,7 +724,7 @@
         <v>0.15428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -748,7 +748,7 @@
         <v>8.1081081081081086E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -772,7 +772,7 @@
         <v>5.4421768707482991E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -796,7 +796,7 @@
         <v>7.8947368421052627E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -820,7 +820,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -845,7 +845,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -870,7 +870,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -894,7 +894,7 @@
         <v>1.5706806282722512E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -918,7 +918,7 @@
         <v>2.7417027417027416E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -942,7 +942,7 @@
         <v>2.1148036253776436E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -966,7 +966,7 @@
         <v>3.6036036036036036E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -990,7 +990,7 @@
         <v>2.8609154929577465E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>3.1428571428571431E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>3.0549898167006109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>2.1069692058346839E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>1.4109347442680775E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>1.4109347442680775E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>0.16317991631799164</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>0.20787746170678337</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>0.21878453038674034</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>0.14744351961950058</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>0.11534154535274356</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>6.1409179056237877E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>3.780718336483932E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>2.0155038759689922E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1352,9 +1352,9 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
@@ -1376,9 +1376,9 @@
         <v>0.16317991631799164</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
@@ -1400,9 +1400,9 @@
         <v>0.20787746170678337</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>29</v>
@@ -1424,9 +1424,9 @@
         <v>0.21878453038674034</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>29</v>
@@ -1448,9 +1448,9 @@
         <v>0.14744351961950058</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>29</v>
@@ -1472,9 +1472,9 @@
         <v>0.11534154535274356</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>29</v>
@@ -1496,9 +1496,9 @@
         <v>6.1409179056237877E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>29</v>
@@ -1520,9 +1520,9 @@
         <v>3.780718336483932E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>29</v>
@@ -1544,9 +1544,9 @@
         <v>2.0155038759689922E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>29</v>
@@ -1568,9 +1568,9 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>29</v>
@@ -1592,9 +1592,9 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>29</v>
@@ -1616,9 +1616,9 @@
         <v>0.58638743455497377</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>29</v>
@@ -1640,9 +1640,9 @@
         <v>0.34920634920634919</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>29</v>
@@ -1664,9 +1664,9 @@
         <v>0.2175226586102719</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>29</v>
@@ -1688,9 +1688,9 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>29</v>
@@ -1712,9 +1712,9 @@
         <v>0.16461267605633803</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>29</v>
@@ -1736,9 +1736,9 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>29</v>
@@ -1760,9 +1760,9 @@
         <v>0.10183299389002037</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>29</v>
@@ -1786,9 +1786,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
@@ -1812,9 +1812,9 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>29</v>
@@ -1838,7 +1838,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>0.73896528627634828</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>0.62062966115974605</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>0.47893264233014488</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>36</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>0.59252264082678208</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>36</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>0.32293097813833699</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>36</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>0.29832234128895085</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>36</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>0.27445149548815129</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>1.0135135135135136E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>40</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>8.8504182065745965E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>40</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0.28191051331320338</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>40</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.45185719437432381</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>40</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>0.3721881390593047</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>40</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>0.26923076923076922</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>40</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>0.22687224669603523</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>41</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0.10095312196070803</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>41</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>0.33324183365358223</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>41</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>41</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>41</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>41</v>
       </c>
@@ -2406,7 +2406,7 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>42</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>42</v>
       </c>
@@ -2458,7 +2458,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>42</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>42</v>
       </c>
@@ -2510,7 +2510,7 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>42</v>
       </c>
@@ -2536,7 +2536,7 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>42</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
@@ -2614,7 +2614,7 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
@@ -2640,7 +2640,7 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>43</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>43</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>43</v>
       </c>
@@ -2718,7 +2718,7 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>43</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>43</v>
       </c>
@@ -2770,7 +2770,7 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>44</v>
       </c>
@@ -2796,7 +2796,7 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>44</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>44</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>44</v>
       </c>
@@ -2874,7 +2874,7 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>44</v>
       </c>
@@ -2900,7 +2900,7 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>44</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>44</v>
       </c>
@@ -2952,7 +2952,7 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>45</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>45</v>
       </c>
@@ -3004,7 +3004,7 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>45</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>45</v>
       </c>
@@ -3056,7 +3056,7 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>45</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>45</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>45</v>
       </c>
@@ -3134,7 +3134,7 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>46</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>46</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>46</v>
       </c>
@@ -3212,7 +3212,7 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>46</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>46</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>46</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>46</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>47</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>47</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>47</v>
       </c>
@@ -3394,7 +3394,7 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>47</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>47</v>
       </c>
@@ -3446,7 +3446,7 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>47</v>
       </c>
@@ -3472,7 +3472,7 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>47</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>48</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>48</v>
       </c>
@@ -3550,7 +3550,7 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>48</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>48</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>48</v>
       </c>
@@ -3628,7 +3628,7 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>48</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>48</v>
       </c>
@@ -3680,7 +3680,7 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>49</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>49</v>
       </c>
@@ -3732,7 +3732,7 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>49</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -3784,7 +3784,7 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>49</v>
       </c>
@@ -3810,7 +3810,7 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>49</v>
       </c>
@@ -3836,7 +3836,7 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>49</v>
       </c>
@@ -3862,7 +3862,7 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>50</v>
       </c>
@@ -3888,7 +3888,7 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>50</v>
       </c>
@@ -3914,7 +3914,7 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>50</v>
       </c>
@@ -3940,7 +3940,7 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>50</v>
       </c>
@@ -3966,7 +3966,7 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>50</v>
       </c>
@@ -3992,7 +3992,7 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>50</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>50</v>
       </c>
@@ -4044,7 +4044,7 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>51</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>51</v>
       </c>
@@ -4096,7 +4096,7 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>51</v>
       </c>
@@ -4122,7 +4122,7 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>51</v>
       </c>
@@ -4148,7 +4148,7 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>51</v>
       </c>
@@ -4174,7 +4174,7 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>51</v>
       </c>
@@ -4200,7 +4200,7 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>51</v>
       </c>
@@ -4226,7 +4226,7 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>55</v>
       </c>
@@ -4252,7 +4252,7 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>55</v>
       </c>
@@ -4278,7 +4278,7 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>55</v>
       </c>
@@ -4304,7 +4304,7 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>55</v>
       </c>
@@ -4330,7 +4330,7 @@
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>55</v>
       </c>
@@ -4356,7 +4356,7 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>55</v>
       </c>
@@ -4382,7 +4382,7 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>55</v>
       </c>
@@ -4408,7 +4408,7 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>55</v>
       </c>
@@ -4434,7 +4434,7 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>55</v>
       </c>
@@ -4460,7 +4460,7 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>57</v>
       </c>
@@ -4486,7 +4486,7 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>57</v>
       </c>
@@ -4512,7 +4512,7 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>57</v>
       </c>
@@ -4538,7 +4538,7 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>57</v>
       </c>
@@ -4564,7 +4564,7 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>57</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>57</v>
       </c>
@@ -4616,7 +4616,7 @@
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>57</v>
       </c>
@@ -4642,7 +4642,7 @@
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>57</v>
       </c>
@@ -4668,7 +4668,7 @@
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>57</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
     </row>
-    <row r="162" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>59</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>59</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>59</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>59</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>59</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>0.129</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>59</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>59</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>59</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>59</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>59</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>0.33300000000000002</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>60</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>60</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>60</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>0.13600000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>60</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>60</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>60</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>60</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>60</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>60</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>60</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="29.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Verified Mbulawa and McDonald sources and added comments
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HIVHPV_Model\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -203,9 +203,6 @@
     <t>Usage Status</t>
   </si>
   <si>
-    <t>Questions</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -218,16 +215,19 @@
     <t>Africa Centre cohort (now on AHRI) for KZN. Can access the HIV prevalence estimates by putting in a data request ("ACDIS:HIV Surveillance 2010-2016.Release 2016-12").</t>
   </si>
   <si>
-    <t>Reference unverified. Reference found does not stratify by HIV status. Looks like the HIV+ and HIV- values were swapped. The following references support that these values were swapped: McDonald et al. 2014; Adebamowo et al. 2017; De Vuyst et al. 2011</t>
-  </si>
-  <si>
-    <t>What year of data in our model should we compare to…2006? Were persons on ART included in this analysis? If so, were they considered HIV+?</t>
-  </si>
-  <si>
-    <t>What year of data in our model should we compare to…2009? Were persons on ART included in this analysis? If so, were they considered HIV+?</t>
-  </si>
-  <si>
-    <t>Check whether these values came from the 2014 or 2012 paper.  What year of data in our model should we compare to…2006? Were persons on ART included in this analysis? If so, were they considered HIV+?</t>
+    <t>Reference unverified. Reference found does not stratify by HIV status. Looks like the HIV+ and HIV- values were swapped. The following references support that these values were swapped, as they all report higher prevalence among HIV-positive than HIV-negative women at all stages of infection, except in ICC when prevalence is similar: McDonald et al. 2014; Adebamowo et al. 2017; De Vuyst et al. 2011. Instead of using these data, we will use the above data on prevalence among women with CIN2/3 and the data below from McDonald 2014 on the prevalence among women regardless of cytology status.</t>
+  </si>
+  <si>
+    <t>Questions/Comments</t>
+  </si>
+  <si>
+    <t>Samples were collected 2006-2009. Compare to year 2008 to get roughly the middle of this interval. I believe the study would have included people on ART as HIV-positive. The 95% CI were derived from the published point estimates as p +/- sqrt(p*(1-p)/n)*1.96</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts include domwen aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive.</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts include domwen aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive. Note these statistics are for any HPV prevalence, not hrHPV specifically</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
     <tableColumn id="5" name="LB" dataDxfId="1"/>
     <tableColumn id="6" name="UB" dataDxfId="0"/>
     <tableColumn id="8" name="Usage Status"/>
-    <tableColumn id="11" name="Questions"/>
+    <tableColumn id="11" name="Questions/Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -594,22 +594,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L145" sqref="L145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" customWidth="1"/>
-    <col min="11" max="11" width="43.36328125" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -641,10 +641,10 @@
         <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -668,13 +668,13 @@
         <v>0.125</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -698,10 +698,10 @@
         <v>5.4298642533936653E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -725,10 +725,10 @@
         <v>0.12757201646090535</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -752,10 +752,10 @@
         <v>0.15428571428571428</v>
       </c>
       <c r="J5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -779,10 +779,10 @@
         <v>8.1081081081081086E-2</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -806,10 +806,10 @@
         <v>5.4421768707482991E-2</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -833,10 +833,10 @@
         <v>7.8947368421052627E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -860,10 +860,10 @@
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -888,10 +888,10 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -916,10 +916,10 @@
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -943,10 +943,10 @@
         <v>1.5706806282722512E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -970,10 +970,10 @@
         <v>2.7417027417027416E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -997,10 +997,10 @@
         <v>2.1148036253776436E-2</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1024,10 +1024,10 @@
         <v>3.6036036036036036E-2</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1051,10 +1051,10 @@
         <v>2.8609154929577465E-2</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1078,10 +1078,10 @@
         <v>3.1428571428571431E-2</v>
       </c>
       <c r="J17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1105,10 +1105,10 @@
         <v>3.0549898167006109E-2</v>
       </c>
       <c r="J18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1132,10 +1132,10 @@
         <v>2.1069692058346839E-2</v>
       </c>
       <c r="J19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1160,10 +1160,10 @@
         <v>1.4109347442680775E-2</v>
       </c>
       <c r="J20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1188,10 +1188,10 @@
         <v>1.4109347442680775E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1218,10 +1218,10 @@
         <v>0</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -2010,12 +2010,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>31</v>
@@ -2038,18 +2038,18 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>32</v>
@@ -2072,15 +2072,15 @@
         <v>0.73896528627634828</v>
       </c>
       <c r="J53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>33</v>
@@ -2103,15 +2103,15 @@
         <v>0.62062966115974605</v>
       </c>
       <c r="J54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>34</v>
@@ -2134,15 +2134,15 @@
         <v>0.47893264233014488</v>
       </c>
       <c r="J55" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>31</v>
@@ -2165,15 +2165,15 @@
         <v>0.59252264082678208</v>
       </c>
       <c r="J56" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>32</v>
@@ -2196,15 +2196,15 @@
         <v>0.32293097813833699</v>
       </c>
       <c r="J57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>33</v>
@@ -2227,15 +2227,15 @@
         <v>0.29832234128895085</v>
       </c>
       <c r="J58" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>34</v>
@@ -2258,15 +2258,15 @@
         <v>0.27445149548815129</v>
       </c>
       <c r="J59" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -2285,10 +2285,10 @@
         <v>1.0135135135135136E-2</v>
       </c>
       <c r="J60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>39</v>
       </c>
@@ -2312,10 +2312,10 @@
         <v>8.8504182065745965E-2</v>
       </c>
       <c r="J61" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>39</v>
       </c>
@@ -2339,10 +2339,10 @@
         <v>0.28191051331320338</v>
       </c>
       <c r="J62" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>
@@ -2366,10 +2366,10 @@
         <v>0.45185719437432381</v>
       </c>
       <c r="J63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>39</v>
       </c>
@@ -2393,10 +2393,10 @@
         <v>0.3721881390593047</v>
       </c>
       <c r="J64" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>39</v>
       </c>
@@ -2420,10 +2420,10 @@
         <v>0.26923076923076922</v>
       </c>
       <c r="J65" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>39</v>
       </c>
@@ -2447,10 +2447,10 @@
         <v>0.22687224669603523</v>
       </c>
       <c r="J66" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>40</v>
       </c>
@@ -2474,10 +2474,10 @@
         <v>1.3157894736842105E-2</v>
       </c>
       <c r="J67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>40</v>
       </c>
@@ -2501,10 +2501,10 @@
         <v>0.10095312196070803</v>
       </c>
       <c r="J68" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>40</v>
       </c>
@@ -2528,10 +2528,10 @@
         <v>0.33324183365358223</v>
       </c>
       <c r="J69" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>40</v>
       </c>
@@ -2557,10 +2557,10 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>40</v>
       </c>
@@ -2586,10 +2586,10 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>40</v>
       </c>
@@ -2615,10 +2615,10 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>40</v>
       </c>
@@ -2644,10 +2644,10 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>41</v>
       </c>
@@ -2673,10 +2673,10 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>41</v>
       </c>
@@ -2702,10 +2702,10 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>41</v>
       </c>
@@ -2731,10 +2731,10 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>41</v>
       </c>
@@ -2760,10 +2760,10 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>41</v>
       </c>
@@ -2789,10 +2789,10 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>41</v>
       </c>
@@ -2818,10 +2818,10 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>41</v>
       </c>
@@ -2847,10 +2847,10 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>42</v>
       </c>
@@ -2876,10 +2876,10 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>42</v>
       </c>
@@ -2905,10 +2905,10 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>42</v>
       </c>
@@ -2934,10 +2934,10 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>42</v>
       </c>
@@ -2963,10 +2963,10 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>42</v>
       </c>
@@ -2992,10 +2992,10 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>42</v>
       </c>
@@ -3021,10 +3021,10 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>42</v>
       </c>
@@ -3050,10 +3050,10 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>43</v>
       </c>
@@ -3079,10 +3079,10 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>43</v>
       </c>
@@ -3108,10 +3108,10 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>43</v>
       </c>
@@ -3137,10 +3137,10 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>43</v>
       </c>
@@ -3166,10 +3166,10 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>43</v>
       </c>
@@ -3195,10 +3195,10 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>43</v>
       </c>
@@ -3224,10 +3224,10 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>43</v>
       </c>
@@ -3253,10 +3253,10 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>44</v>
       </c>
@@ -3282,10 +3282,10 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>44</v>
       </c>
@@ -3311,10 +3311,10 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>44</v>
       </c>
@@ -3340,10 +3340,10 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>44</v>
       </c>
@@ -3369,10 +3369,10 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>44</v>
       </c>
@@ -3398,10 +3398,10 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>44</v>
       </c>
@@ -3427,10 +3427,10 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>44</v>
       </c>
@@ -3456,10 +3456,10 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>45</v>
       </c>
@@ -3485,10 +3485,10 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>45</v>
       </c>
@@ -3514,10 +3514,10 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>45</v>
       </c>
@@ -3543,10 +3543,10 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>45</v>
       </c>
@@ -3572,10 +3572,10 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>45</v>
       </c>
@@ -3601,10 +3601,10 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>45</v>
       </c>
@@ -3630,10 +3630,10 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>45</v>
       </c>
@@ -3659,10 +3659,10 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
       <c r="J108" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>46</v>
       </c>
@@ -3688,10 +3688,10 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>46</v>
       </c>
@@ -3717,10 +3717,10 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
       <c r="J110" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>46</v>
       </c>
@@ -3746,10 +3746,10 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>46</v>
       </c>
@@ -3775,10 +3775,10 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>46</v>
       </c>
@@ -3804,10 +3804,10 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>46</v>
       </c>
@@ -3833,10 +3833,10 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
       <c r="J114" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>46</v>
       </c>
@@ -3862,10 +3862,10 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>47</v>
       </c>
@@ -3891,10 +3891,10 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
       <c r="J116" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>47</v>
       </c>
@@ -3920,10 +3920,10 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>47</v>
       </c>
@@ -3949,10 +3949,10 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
       <c r="J118" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>47</v>
       </c>
@@ -3978,10 +3978,10 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>47</v>
       </c>
@@ -4007,10 +4007,10 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
       <c r="J120" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>47</v>
       </c>
@@ -4036,10 +4036,10 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>47</v>
       </c>
@@ -4065,10 +4065,10 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
       <c r="J122" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>48</v>
       </c>
@@ -4094,10 +4094,10 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>48</v>
       </c>
@@ -4123,10 +4123,10 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
       <c r="J124" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>48</v>
       </c>
@@ -4152,10 +4152,10 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>48</v>
       </c>
@@ -4181,10 +4181,10 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
       <c r="J126" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>48</v>
       </c>
@@ -4210,10 +4210,10 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>48</v>
       </c>
@@ -4239,10 +4239,10 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
       <c r="J128" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>48</v>
       </c>
@@ -4268,10 +4268,10 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>49</v>
       </c>
@@ -4297,10 +4297,10 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
       <c r="J130" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>49</v>
       </c>
@@ -4326,10 +4326,10 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>49</v>
       </c>
@@ -4355,10 +4355,10 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
       <c r="J132" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>49</v>
       </c>
@@ -4384,10 +4384,10 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>49</v>
       </c>
@@ -4413,10 +4413,10 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
       <c r="J134" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>49</v>
       </c>
@@ -4442,10 +4442,10 @@
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>49</v>
       </c>
@@ -4471,10 +4471,10 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
       <c r="J136" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>50</v>
       </c>
@@ -4500,10 +4500,10 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>50</v>
       </c>
@@ -4529,10 +4529,10 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
       <c r="J138" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>50</v>
       </c>
@@ -4558,10 +4558,10 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>50</v>
       </c>
@@ -4587,10 +4587,10 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
       <c r="J140" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>50</v>
       </c>
@@ -4616,10 +4616,10 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>50</v>
       </c>
@@ -4645,10 +4645,10 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>50</v>
       </c>
@@ -4674,10 +4674,10 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>54</v>
       </c>
@@ -4703,13 +4703,13 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
       <c r="J144" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K144" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>54</v>
       </c>
@@ -4735,10 +4735,10 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
       <c r="J145" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>54</v>
       </c>
@@ -4764,10 +4764,10 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
       <c r="J146" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>54</v>
       </c>
@@ -4793,10 +4793,10 @@
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
       <c r="J147" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>54</v>
       </c>
@@ -4822,10 +4822,10 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
       <c r="J148" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>54</v>
       </c>
@@ -4851,10 +4851,10 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>54</v>
       </c>
@@ -4880,10 +4880,10 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
       <c r="J150" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>54</v>
       </c>
@@ -4909,10 +4909,10 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
       <c r="J151" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>54</v>
       </c>
@@ -4938,10 +4938,10 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
       <c r="J152" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>55</v>
       </c>
@@ -4967,10 +4967,10 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>55</v>
       </c>
@@ -4996,10 +4996,10 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
       <c r="J154" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>55</v>
       </c>
@@ -5025,10 +5025,10 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
       <c r="J155" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>55</v>
       </c>
@@ -5054,10 +5054,10 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
       <c r="J156" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>55</v>
       </c>
@@ -5083,10 +5083,10 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
       <c r="J157" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>55</v>
       </c>
@@ -5112,10 +5112,10 @@
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
       <c r="J158" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>55</v>
       </c>
@@ -5141,10 +5141,10 @@
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
       <c r="J159" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>55</v>
       </c>
@@ -5170,10 +5170,10 @@
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
       <c r="J160" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>55</v>
       </c>
@@ -5199,10 +5199,10 @@
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
       <c r="J161" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -5214,7 +5214,7 @@
       <c r="I162" s="7"/>
       <c r="K162" s="8"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -5225,7 +5225,7 @@
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5236,7 +5236,7 @@
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -5247,7 +5247,7 @@
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -5258,7 +5258,7 @@
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -5269,7 +5269,7 @@
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -5280,7 +5280,7 @@
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -5291,7 +5291,7 @@
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -5302,7 +5302,7 @@
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -5313,7 +5313,7 @@
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -5324,7 +5324,7 @@
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -5335,7 +5335,7 @@
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -5346,7 +5346,7 @@
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -5357,7 +5357,7 @@
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -5368,7 +5368,7 @@
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -5379,7 +5379,7 @@
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -5390,7 +5390,7 @@
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -5401,7 +5401,7 @@
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -5412,7 +5412,7 @@
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
     </row>
-    <row r="181" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -5423,7 +5423,7 @@
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
     </row>
-    <row r="182" spans="1:9" ht="29.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating calibration data sheet with answers to questions about sources from master branch.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HIVHPV_Model\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="68">
   <si>
     <t>N</t>
   </si>
@@ -119,9 +119,6 @@
     <t>HR HPV Prevalence in HIV+ Men</t>
   </si>
   <si>
-    <t>Mbulawa</t>
-  </si>
-  <si>
     <t>18-25</t>
   </si>
   <si>
@@ -194,28 +191,43 @@
     <t>HPV Prevalence in HIV+ Women (all)</t>
   </si>
   <si>
-    <t>McDonald</t>
-  </si>
-  <si>
     <t>HPV Prevalence in HIV- Women (all)</t>
   </si>
   <si>
-    <t>McDonald 2014</t>
-  </si>
-  <si>
-    <t>CIN2/CIN3 Prevalence HPV16 (HIV+)</t>
-  </si>
-  <si>
-    <t>CIN2/CIN3 Prevalence HPV16 (HIV-)</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Proportion of HPV infections that were HPV16 among women with CIN2/CIN3</t>
+    <t>McDonald (2014) Front Oncol. "Distribution of Human Papillomavirus Genotypes among HIV-Positive and HIV-Negative Women in Cape Town, South Africa</t>
+  </si>
+  <si>
+    <t>McDonald (2014) Front Oncol.</t>
+  </si>
+  <si>
+    <t>Usage Status</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Mbulawa (2015) BMC Infect Dis. "Human papillomavirus prevalence in South African women and men according to age and human immunodeficiency virus status</t>
+  </si>
+  <si>
+    <t>Mbulawa (2015) BMC Infect Dis.</t>
+  </si>
+  <si>
+    <t>Africa Centre cohort (now on AHRI) for KZN. Can access the HIV prevalence estimates by putting in a data request ("ACDIS:HIV Surveillance 2010-2016.Release 2016-12").</t>
+  </si>
+  <si>
+    <t>Reference unverified. Reference found does not stratify by HIV status. Looks like the HIV+ and HIV- values were swapped. The following references support that these values were swapped, as they all report higher prevalence among HIV-positive than HIV-negative women at all stages of infection, except in ICC when prevalence is similar: McDonald et al. 2014; Adebamowo et al. 2017; De Vuyst et al. 2011. Instead of using these data, we will use the above data on prevalence among women with CIN2/3 and the data below from McDonald 2014 on the prevalence among women regardless of cytology status.</t>
+  </si>
+  <si>
+    <t>Questions/Comments</t>
+  </si>
+  <si>
+    <t>Samples were collected 2006-2009. Compare to year 2008 to get roughly the middle of this interval. I believe the study would have included people on ART as HIV-positive. The 95% CI were derived from the published point estimates as p +/- sqrt(p*(1-p)/n)*1.96</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts include domwen aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive.</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts include domwen aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive. Note these statistics are for any HPV prevalence, not hrHPV specifically</t>
   </si>
 </sst>
 </file>
@@ -251,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,19 +277,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,13 +317,13 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="0">
+    <tableColumn id="4" name="Mean" dataDxfId="2">
       <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="2"/>
-    <tableColumn id="6" name="UB" dataDxfId="1"/>
-    <tableColumn id="8" name="Column1"/>
-    <tableColumn id="11" name="Column2"/>
+    <tableColumn id="5" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" name="UB" dataDxfId="0"/>
+    <tableColumn id="8" name="Usage Status"/>
+    <tableColumn id="11" name="Questions/Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,18 +594,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L145" sqref="L145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -604,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -616,24 +632,24 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -650,6 +666,12 @@
       <c r="G2">
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -657,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -674,6 +696,9 @@
       <c r="G3">
         <f>Table1[Pos]/Table1[N]</f>
         <v>5.4298642533936653E-2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -681,7 +706,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -698,6 +723,9 @@
       <c r="G4">
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.12757201646090535</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -705,7 +733,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -722,6 +750,9 @@
       <c r="G5">
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.15428571428571428</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -729,7 +760,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -746,6 +777,9 @@
       <c r="G6">
         <f>Table1[Pos]/Table1[N]</f>
         <v>8.1081081081081086E-2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -753,7 +787,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -770,6 +804,9 @@
       <c r="G7">
         <f>Table1[Pos]/Table1[N]</f>
         <v>5.4421768707482991E-2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -777,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -794,6 +831,9 @@
       <c r="G8">
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.8947368421052627E-2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -801,7 +841,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -818,6 +858,9 @@
       <c r="G9">
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -825,7 +868,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -844,13 +887,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.6923076923076927E-2</v>
       </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
@@ -869,13 +915,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.6923076923076927E-2</v>
       </c>
+      <c r="J11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -892,6 +941,9 @@
       <c r="G12">
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.5706806282722512E-2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -899,7 +951,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -916,6 +968,9 @@
       <c r="G13">
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.7417027417027416E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -923,7 +978,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -940,6 +995,9 @@
       <c r="G14">
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.1148036253776436E-2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -947,7 +1005,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -964,6 +1022,9 @@
       <c r="G15">
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.6036036036036036E-2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -971,7 +1032,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -989,13 +1050,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.8609154929577465E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1013,13 +1077,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.1428571428571431E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
@@ -1037,13 +1104,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.0549898167006109E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -1061,13 +1131,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.1069692058346839E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
@@ -1086,13 +1159,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.4109347442680775E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
@@ -1111,8 +1187,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.4109347442680775E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1135,8 +1214,14 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16317991631799164</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1159,8 +1244,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.20787746170678337</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1183,8 +1271,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.21878453038674034</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1207,8 +1298,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14744351961950058</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1231,8 +1325,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.11534154535274356</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1255,8 +1352,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>6.1409179056237877E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1279,8 +1379,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.780718336483932E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1303,8 +1406,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.0155038759689922E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1327,8 +1433,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1351,8 +1460,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1375,8 +1487,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16317991631799164</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1399,8 +1514,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.20787746170678337</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -1423,8 +1541,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.21878453038674034</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -1447,8 +1568,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14744351961950058</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -1471,8 +1595,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.11534154535274356</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1495,8 +1622,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>6.1409179056237877E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1519,8 +1649,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.780718336483932E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -1543,8 +1676,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.0155038759689922E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1567,8 +1703,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -1591,8 +1730,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1615,8 +1757,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.58638743455497377</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1639,8 +1784,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.34920634920634919</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -1663,8 +1811,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.2175226586102719</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -1687,8 +1838,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1711,8 +1865,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16461267605633803</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -1735,8 +1892,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14499999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
@@ -1759,8 +1919,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.10183299389002037</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
@@ -1785,8 +1948,11 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
@@ -1811,8 +1977,11 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -1837,16 +2006,19 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="5">
@@ -1865,16 +2037,22 @@
       <c r="I52" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>59</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="5">
@@ -1893,16 +2071,19 @@
       <c r="I53" s="1">
         <v>0.73896528627634828</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="5">
@@ -1921,16 +2102,19 @@
       <c r="I54" s="1">
         <v>0.62062966115974605</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="5">
@@ -1949,16 +2133,19 @@
       <c r="I55" s="1">
         <v>0.47893264233014488</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="5">
@@ -1977,16 +2164,19 @@
       <c r="I56" s="1">
         <v>0.59252264082678208</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="5">
@@ -2005,16 +2195,19 @@
       <c r="I57" s="1">
         <v>0.32293097813833699</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="5">
@@ -2033,16 +2226,19 @@
       <c r="I58" s="1">
         <v>0.29832234128895085</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="5">
@@ -2061,13 +2257,16 @@
       <c r="I59" s="1">
         <v>0.27445149548815129</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -2085,13 +2284,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.0135135135135136E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -2109,13 +2311,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>8.8504182065745965E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -2133,13 +2338,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.28191051331320338</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
@@ -2157,13 +2365,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.45185719437432381</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -2181,13 +2392,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.3721881390593047</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -2205,13 +2419,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.26923076923076922</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
@@ -2229,13 +2446,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.22687224669603523</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
@@ -2253,13 +2473,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.3157894736842105E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2277,13 +2500,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.10095312196070803</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
@@ -2301,13 +2527,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.33324183365358223</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -2327,13 +2556,16 @@
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -2353,13 +2585,16 @@
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -2379,13 +2614,16 @@
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
@@ -2405,13 +2643,16 @@
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -2431,13 +2672,16 @@
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -2457,13 +2701,16 @@
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -2483,13 +2730,16 @@
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
@@ -2509,13 +2759,16 @@
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -2535,13 +2788,16 @@
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -2561,13 +2817,16 @@
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C80" t="s">
         <v>10</v>
@@ -2587,13 +2846,16 @@
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -2613,13 +2875,16 @@
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2639,13 +2904,16 @@
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
@@ -2665,13 +2933,16 @@
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -2691,13 +2962,16 @@
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -2717,13 +2991,16 @@
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
@@ -2743,13 +3020,16 @@
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
@@ -2769,13 +3049,16 @@
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -2795,13 +3078,16 @@
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2821,13 +3107,16 @@
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
@@ -2847,13 +3136,16 @@
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -2873,13 +3165,16 @@
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -2899,13 +3194,16 @@
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2925,13 +3223,16 @@
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
@@ -2951,13 +3252,16 @@
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C95" t="s">
         <v>4</v>
@@ -2977,13 +3281,16 @@
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -3003,13 +3310,16 @@
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -3029,13 +3339,16 @@
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -3055,13 +3368,16 @@
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -3081,13 +3397,16 @@
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
@@ -3107,13 +3426,16 @@
       </c>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -3133,13 +3455,16 @@
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
@@ -3159,13 +3484,16 @@
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -3185,13 +3513,16 @@
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -3211,13 +3542,16 @@
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -3237,13 +3571,16 @@
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -3263,13 +3600,16 @@
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -3289,13 +3629,16 @@
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -3315,13 +3658,16 @@
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
@@ -3341,13 +3687,16 @@
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
@@ -3367,13 +3716,16 @@
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
@@ -3393,13 +3745,16 @@
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
@@ -3419,13 +3774,16 @@
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -3445,13 +3803,16 @@
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -3471,13 +3832,16 @@
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -3497,13 +3861,16 @@
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -3523,13 +3890,16 @@
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -3549,13 +3919,16 @@
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -3575,13 +3948,16 @@
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -3601,13 +3977,16 @@
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -3627,13 +4006,16 @@
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -3653,13 +4035,16 @@
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -3679,13 +4064,16 @@
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C123" t="s">
         <v>4</v>
@@ -3705,13 +4093,16 @@
       </c>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -3731,13 +4122,16 @@
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
@@ -3757,13 +4151,16 @@
       </c>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C126" t="s">
         <v>7</v>
@@ -3783,13 +4180,16 @@
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -3809,13 +4209,16 @@
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -3835,13 +4238,16 @@
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C129" t="s">
         <v>10</v>
@@ -3861,13 +4267,16 @@
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -3887,13 +4296,16 @@
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -3913,13 +4325,16 @@
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
@@ -3939,13 +4354,16 @@
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -3965,13 +4383,16 @@
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -3991,13 +4412,16 @@
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
@@ -4017,13 +4441,16 @@
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C136" t="s">
         <v>10</v>
@@ -4043,13 +4470,16 @@
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
@@ -4069,13 +4499,16 @@
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C138" t="s">
         <v>5</v>
@@ -4095,13 +4528,16 @@
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C139" t="s">
         <v>6</v>
@@ -4121,13 +4557,16 @@
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -4147,13 +4586,16 @@
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -4173,13 +4615,16 @@
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -4199,13 +4644,16 @@
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C143" t="s">
         <v>10</v>
@@ -4225,16 +4673,19 @@
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>55</v>
-      </c>
-      <c r="B144" t="s">
+        <v>54</v>
+      </c>
+      <c r="B144" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C144" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D144">
         <v>2014</v>
@@ -4251,13 +4702,19 @@
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" t="s">
+        <v>59</v>
+      </c>
+      <c r="K144" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>55</v>
-      </c>
-      <c r="B145" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -4277,13 +4734,16 @@
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>55</v>
-      </c>
-      <c r="B146" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -4303,13 +4763,16 @@
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>55</v>
-      </c>
-      <c r="B147" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -4329,13 +4792,16 @@
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>55</v>
-      </c>
-      <c r="B148" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -4355,13 +4821,16 @@
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>55</v>
-      </c>
-      <c r="B149" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -4381,13 +4850,16 @@
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>55</v>
-      </c>
-      <c r="B150" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C150" t="s">
         <v>10</v>
@@ -4407,13 +4879,16 @@
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>55</v>
-      </c>
-      <c r="B151" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C151" t="s">
         <v>11</v>
@@ -4433,16 +4908,19 @@
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>55</v>
-      </c>
-      <c r="B152" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C152" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D152">
         <v>2014</v>
@@ -4459,16 +4937,19 @@
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>55</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B153" t="s">
-        <v>56</v>
-      </c>
       <c r="C153" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D153">
         <v>2014</v>
@@ -4485,13 +4966,16 @@
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>55</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B154" t="s">
-        <v>56</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>
@@ -4511,13 +4995,16 @@
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B155" t="s">
-        <v>56</v>
       </c>
       <c r="C155" t="s">
         <v>6</v>
@@ -4537,13 +5024,16 @@
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>55</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B156" t="s">
-        <v>56</v>
       </c>
       <c r="C156" t="s">
         <v>7</v>
@@ -4563,13 +5053,16 @@
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>55</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B157" t="s">
-        <v>56</v>
       </c>
       <c r="C157" t="s">
         <v>8</v>
@@ -4589,13 +5082,16 @@
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>55</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B158" t="s">
-        <v>56</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
@@ -4615,13 +5111,16 @@
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>55</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B159" t="s">
-        <v>56</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
@@ -4641,13 +5140,16 @@
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>55</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B160" t="s">
-        <v>56</v>
       </c>
       <c r="C160" t="s">
         <v>11</v>
@@ -4667,16 +5169,19 @@
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
+      <c r="J160" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>55</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B161" t="s">
-        <v>56</v>
-      </c>
       <c r="C161" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D161">
         <v>2014</v>
@@ -4693,595 +5198,232 @@
       </c>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
-    </row>
-    <row r="162" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D162" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E162" s="1">
-        <v>6</v>
-      </c>
-      <c r="F162" s="1">
-        <v>48</v>
-      </c>
-      <c r="G162" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.125</v>
-      </c>
+      <c r="J161" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="6"/>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
-      <c r="J162">
-        <v>0.161</v>
-      </c>
-      <c r="K162" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="K162" s="8"/>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D163" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E163" s="1">
-        <v>12</v>
-      </c>
-      <c r="F163" s="1">
-        <v>221</v>
-      </c>
-      <c r="G163" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4298642533936653E-2</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="6"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
-      <c r="J163">
-        <v>0.161</v>
-      </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D164" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E164" s="1">
-        <v>31</v>
-      </c>
-      <c r="F164" s="1">
-        <v>243</v>
-      </c>
-      <c r="G164" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.12757201646090535</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="6"/>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
-      <c r="J164">
-        <v>0.161</v>
-      </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D165" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E165" s="1">
-        <v>27</v>
-      </c>
-      <c r="F165" s="1">
-        <v>175</v>
-      </c>
-      <c r="G165" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.15428571428571428</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="6"/>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
-      <c r="J165">
-        <v>0.129</v>
-      </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D166" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E166" s="1">
-        <v>33</v>
-      </c>
-      <c r="F166" s="1">
-        <v>407</v>
-      </c>
-      <c r="G166" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>8.1081081081081086E-2</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="6"/>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
-      <c r="J166">
-        <v>0.129</v>
-      </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D167" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E167" s="1">
-        <v>8</v>
-      </c>
-      <c r="F167" s="1">
-        <v>147</v>
-      </c>
-      <c r="G167" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4421768707482991E-2</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="6"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
-      <c r="J167">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D168" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E168" s="1">
-        <v>6</v>
-      </c>
-      <c r="F168" s="1">
-        <v>76</v>
-      </c>
-      <c r="G168" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.8947368421052627E-2</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="6"/>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
-      <c r="J168">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D169" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E169" s="1">
-        <v>2</v>
-      </c>
-      <c r="F169" s="1">
-        <v>28</v>
-      </c>
-      <c r="G169" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="6"/>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
-      <c r="J169">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D170" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E170" s="1">
-        <v>1</v>
-      </c>
-      <c r="F170" s="1">
-        <f>26/2</f>
-        <v>13</v>
-      </c>
-      <c r="G170" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="6"/>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
-      <c r="J170">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D171" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E171" s="1">
-        <v>1</v>
-      </c>
-      <c r="F171" s="1">
-        <f>26/2</f>
-        <v>13</v>
-      </c>
-      <c r="G171" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="6"/>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
-      <c r="J171">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D172" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E172" s="1">
-        <v>3</v>
-      </c>
-      <c r="F172" s="1">
-        <v>191</v>
-      </c>
-      <c r="G172" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.5706806282722512E-2</v>
-      </c>
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="6"/>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
-      <c r="J172">
-        <v>0.13600000000000001</v>
-      </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D173" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E173" s="1">
-        <v>19</v>
-      </c>
-      <c r="F173" s="1">
-        <v>693</v>
-      </c>
-      <c r="G173" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.7417027417027416E-2</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="6"/>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
-      <c r="J173">
-        <v>0.13600000000000001</v>
-      </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D174" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E174" s="1">
-        <v>14</v>
-      </c>
-      <c r="F174" s="1">
-        <v>662</v>
-      </c>
-      <c r="G174" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1148036253776436E-2</v>
-      </c>
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="6"/>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
-      <c r="J174">
-        <v>0.13600000000000001</v>
-      </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D175" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E175" s="1">
-        <v>24</v>
-      </c>
-      <c r="F175" s="1">
-        <v>666</v>
-      </c>
-      <c r="G175" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.6036036036036036E-2</v>
-      </c>
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="6"/>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
-      <c r="J175">
-        <v>0.20799999999999999</v>
-      </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D176" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E176" s="1">
-        <v>65</v>
-      </c>
-      <c r="F176" s="4">
-        <v>2272</v>
-      </c>
-      <c r="G176" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.8609154929577465E-2</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="6"/>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
-      <c r="J176">
-        <v>0.20799999999999999</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D177" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E177" s="1">
-        <v>44</v>
-      </c>
-      <c r="F177" s="4">
-        <v>1400</v>
-      </c>
-      <c r="G177" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.1428571428571431E-2</v>
-      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="6"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
-      <c r="J177">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D178" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E178" s="1">
-        <v>30</v>
-      </c>
-      <c r="F178" s="1">
-        <v>982</v>
-      </c>
-      <c r="G178" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.0549898167006109E-2</v>
-      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="6"/>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
-      <c r="J178">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D179" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E179" s="1">
-        <v>13</v>
-      </c>
-      <c r="F179" s="1">
-        <v>617</v>
-      </c>
-      <c r="G179" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1069692058346839E-2</v>
-      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="6"/>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
-      <c r="J179">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D180" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E180" s="1">
-        <v>4</v>
-      </c>
-      <c r="F180" s="1">
-        <f>567/2</f>
-        <v>283.5</v>
-      </c>
-      <c r="G180" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
-      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="6"/>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
-      <c r="J180">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D181" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E181" s="1">
-        <v>4</v>
-      </c>
-      <c r="F181" s="1">
-        <f>567/2</f>
-        <v>283.5</v>
-      </c>
-      <c r="G181" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
-      </c>
+    </row>
+    <row r="181" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="6"/>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
-      <c r="J181">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="182" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Catching up or reverting to changes in master branch.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HIVHPV_Model\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="68">
   <si>
     <t>N</t>
   </si>
@@ -119,9 +119,6 @@
     <t>HR HPV Prevalence in HIV+ Men</t>
   </si>
   <si>
-    <t>Mbulawa</t>
-  </si>
-  <si>
     <t>18-25</t>
   </si>
   <si>
@@ -194,28 +191,43 @@
     <t>HPV Prevalence in HIV+ Women (all)</t>
   </si>
   <si>
-    <t>McDonald</t>
-  </si>
-  <si>
     <t>HPV Prevalence in HIV- Women (all)</t>
   </si>
   <si>
-    <t>McDonald 2014</t>
-  </si>
-  <si>
-    <t>CIN2/CIN3 Prevalence HPV16 (HIV+)</t>
-  </si>
-  <si>
-    <t>CIN2/CIN3 Prevalence HPV16 (HIV-)</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Proportion of HPV infections that were HPV16 among women with CIN2/CIN3</t>
+    <t>McDonald (2014) Front Oncol. "Distribution of Human Papillomavirus Genotypes among HIV-Positive and HIV-Negative Women in Cape Town, South Africa</t>
+  </si>
+  <si>
+    <t>McDonald (2014) Front Oncol.</t>
+  </si>
+  <si>
+    <t>Usage Status</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Mbulawa (2015) BMC Infect Dis. "Human papillomavirus prevalence in South African women and men according to age and human immunodeficiency virus status</t>
+  </si>
+  <si>
+    <t>Mbulawa (2015) BMC Infect Dis.</t>
+  </si>
+  <si>
+    <t>Africa Centre cohort (now on AHRI) for KZN. Can access the HIV prevalence estimates by putting in a data request ("ACDIS:HIV Surveillance 2010-2016.Release 2016-12").</t>
+  </si>
+  <si>
+    <t>Reference unverified. Reference found does not stratify by HIV status. Looks like the HIV+ and HIV- values were swapped. The following references support that these values were swapped, as they all report higher prevalence among HIV-positive than HIV-negative women at all stages of infection, except in ICC when prevalence is similar: McDonald et al. 2014; Adebamowo et al. 2017; De Vuyst et al. 2011. Instead of using these data, we will use the above data on prevalence among women with CIN2/3 and the data below from McDonald 2014 on the prevalence among women regardless of cytology status.</t>
+  </si>
+  <si>
+    <t>Questions/Comments</t>
+  </si>
+  <si>
+    <t>Samples were collected 2006-2009. Compare to year 2008 to get roughly the middle of this interval. I believe the study would have included people on ART as HIV-positive. The 95% CI were derived from the published point estimates as p +/- sqrt(p*(1-p)/n)*1.96</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts include domwen aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive.</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts include domwen aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive. Note these statistics are for any HPV prevalence, not hrHPV specifically</t>
   </si>
 </sst>
 </file>
@@ -251,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,19 +277,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,13 +317,13 @@
     <tableColumn id="7" name="Year"/>
     <tableColumn id="10" name="Pos"/>
     <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Mean" dataDxfId="0">
+    <tableColumn id="4" name="Mean" dataDxfId="2">
       <calculatedColumnFormula>Table1[Pos]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="2"/>
-    <tableColumn id="6" name="UB" dataDxfId="1"/>
-    <tableColumn id="8" name="Column1"/>
-    <tableColumn id="11" name="Column2"/>
+    <tableColumn id="5" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" name="UB" dataDxfId="0"/>
+    <tableColumn id="8" name="Usage Status"/>
+    <tableColumn id="11" name="Questions/Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,18 +594,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L145" sqref="L145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -604,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -616,24 +632,24 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
-        <v>38</v>
-      </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
+      <c r="B2" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -650,6 +666,12 @@
       <c r="G2">
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -657,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
@@ -674,6 +696,9 @@
       <c r="G3">
         <f>Table1[Pos]/Table1[N]</f>
         <v>5.4298642533936653E-2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -681,7 +706,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -698,6 +723,9 @@
       <c r="G4">
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.12757201646090535</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -705,7 +733,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -722,6 +750,9 @@
       <c r="G5">
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.15428571428571428</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -729,7 +760,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -746,6 +777,9 @@
       <c r="G6">
         <f>Table1[Pos]/Table1[N]</f>
         <v>8.1081081081081086E-2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -753,7 +787,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -770,6 +804,9 @@
       <c r="G7">
         <f>Table1[Pos]/Table1[N]</f>
         <v>5.4421768707482991E-2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -777,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -794,6 +831,9 @@
       <c r="G8">
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.8947368421052627E-2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -801,7 +841,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -818,6 +858,9 @@
       <c r="G9">
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -825,7 +868,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -844,13 +887,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.6923076923076927E-2</v>
       </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
@@ -869,13 +915,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>7.6923076923076927E-2</v>
       </c>
+      <c r="J11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -892,6 +941,9 @@
       <c r="G12">
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.5706806282722512E-2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -899,7 +951,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
@@ -916,6 +968,9 @@
       <c r="G13">
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.7417027417027416E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -923,7 +978,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -940,6 +995,9 @@
       <c r="G14">
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.1148036253776436E-2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -947,7 +1005,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
@@ -964,6 +1022,9 @@
       <c r="G15">
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.6036036036036036E-2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -971,7 +1032,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -989,13 +1050,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.8609154929577465E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1013,13 +1077,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.1428571428571431E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
@@ -1037,13 +1104,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.0549898167006109E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -1061,13 +1131,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.1069692058346839E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
@@ -1086,13 +1159,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.4109347442680775E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
@@ -1111,8 +1187,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.4109347442680775E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1135,8 +1214,14 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16317991631799164</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1159,8 +1244,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.20787746170678337</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1183,8 +1271,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.21878453038674034</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1207,8 +1298,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14744351961950058</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1231,8 +1325,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.11534154535274356</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1255,8 +1352,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>6.1409179056237877E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1279,8 +1379,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.780718336483932E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1303,8 +1406,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.0155038759689922E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1327,8 +1433,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1351,8 +1460,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1375,8 +1487,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16317991631799164</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -1399,8 +1514,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.20787746170678337</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
@@ -1423,8 +1541,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.21878453038674034</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -1447,8 +1568,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14744351961950058</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -1471,8 +1595,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.11534154535274356</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -1495,8 +1622,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>6.1409179056237877E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1519,8 +1649,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>3.780718336483932E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -1543,8 +1676,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.0155038759689922E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1567,8 +1703,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -1591,8 +1730,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>2.6981450252951095E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1615,8 +1757,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.58638743455497377</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1639,8 +1784,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.34920634920634919</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -1663,8 +1811,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.2175226586102719</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
@@ -1687,8 +1838,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1711,8 +1865,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.16461267605633803</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>27</v>
       </c>
@@ -1735,8 +1892,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.14499999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
@@ -1759,8 +1919,11 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.10183299389002037</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
@@ -1785,8 +1948,11 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>27</v>
       </c>
@@ -1811,8 +1977,11 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -1837,16 +2006,19 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="5">
@@ -1865,16 +2037,22 @@
       <c r="I52" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>59</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="5">
@@ -1893,16 +2071,19 @@
       <c r="I53" s="1">
         <v>0.73896528627634828</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="5">
@@ -1921,16 +2102,19 @@
       <c r="I54" s="1">
         <v>0.62062966115974605</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="5">
@@ -1949,16 +2133,19 @@
       <c r="I55" s="1">
         <v>0.47893264233014488</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="5">
@@ -1977,16 +2164,19 @@
       <c r="I56" s="1">
         <v>0.59252264082678208</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="5">
@@ -2005,16 +2195,19 @@
       <c r="I57" s="1">
         <v>0.32293097813833699</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="5">
@@ -2033,16 +2226,19 @@
       <c r="I58" s="1">
         <v>0.29832234128895085</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="5">
@@ -2061,13 +2257,16 @@
       <c r="I59" s="1">
         <v>0.27445149548815129</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -2085,13 +2284,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.0135135135135136E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -2109,13 +2311,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>8.8504182065745965E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -2133,13 +2338,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.28191051331320338</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
@@ -2157,13 +2365,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.45185719437432381</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
@@ -2181,13 +2392,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.3721881390593047</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
         <v>9</v>
@@ -2205,13 +2419,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.26923076923076922</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
@@ -2229,13 +2446,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.22687224669603523</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
@@ -2253,13 +2473,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>1.3157894736842105E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2277,13 +2500,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.10095312196070803</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
@@ -2301,13 +2527,16 @@
         <f>Table1[Pos]/Table1[N]</f>
         <v>0.33324183365358223</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -2327,13 +2556,16 @@
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -2353,13 +2585,16 @@
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
@@ -2379,13 +2614,16 @@
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
@@ -2405,13 +2643,16 @@
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C74" t="s">
         <v>4</v>
@@ -2431,13 +2672,16 @@
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -2457,13 +2701,16 @@
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -2483,13 +2730,16 @@
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
@@ -2509,13 +2759,16 @@
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
@@ -2535,13 +2788,16 @@
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -2561,13 +2817,16 @@
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C80" t="s">
         <v>10</v>
@@ -2587,13 +2846,16 @@
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -2613,13 +2875,16 @@
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2639,13 +2904,16 @@
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
@@ -2665,13 +2933,16 @@
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -2691,13 +2962,16 @@
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -2717,13 +2991,16 @@
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
@@ -2743,13 +3020,16 @@
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
@@ -2769,13 +3049,16 @@
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -2795,13 +3078,16 @@
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2821,13 +3107,16 @@
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
@@ -2847,13 +3136,16 @@
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -2873,13 +3165,16 @@
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -2899,13 +3194,16 @@
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
@@ -2925,13 +3223,16 @@
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
@@ -2951,13 +3252,16 @@
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C95" t="s">
         <v>4</v>
@@ -2977,13 +3281,16 @@
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -3003,13 +3310,16 @@
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
@@ -3029,13 +3339,16 @@
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -3055,13 +3368,16 @@
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -3081,13 +3397,16 @@
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C100" t="s">
         <v>9</v>
@@ -3107,13 +3426,16 @@
       </c>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -3133,13 +3455,16 @@
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
         <v>4</v>
@@ -3159,13 +3484,16 @@
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -3185,13 +3513,16 @@
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -3211,13 +3542,16 @@
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -3237,13 +3571,16 @@
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -3263,13 +3600,16 @@
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -3289,13 +3629,16 @@
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -3315,13 +3658,16 @@
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C109" t="s">
         <v>4</v>
@@ -3341,13 +3687,16 @@
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
@@ -3367,13 +3716,16 @@
       </c>
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
@@ -3393,13 +3745,16 @@
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
@@ -3419,13 +3774,16 @@
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C113" t="s">
         <v>8</v>
@@ -3445,13 +3803,16 @@
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C114" t="s">
         <v>9</v>
@@ -3471,13 +3832,16 @@
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -3497,13 +3861,16 @@
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -3523,13 +3890,16 @@
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -3549,13 +3919,16 @@
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -3575,13 +3948,16 @@
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -3601,13 +3977,16 @@
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C120" t="s">
         <v>8</v>
@@ -3627,13 +4006,16 @@
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C121" t="s">
         <v>9</v>
@@ -3653,13 +4035,16 @@
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C122" t="s">
         <v>10</v>
@@ -3679,13 +4064,16 @@
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C123" t="s">
         <v>4</v>
@@ -3705,13 +4093,16 @@
       </c>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C124" t="s">
         <v>5</v>
@@ -3731,13 +4122,16 @@
       </c>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
@@ -3757,13 +4151,16 @@
       </c>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C126" t="s">
         <v>7</v>
@@ -3783,13 +4180,16 @@
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C127" t="s">
         <v>8</v>
@@ -3809,13 +4209,16 @@
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C128" t="s">
         <v>9</v>
@@ -3835,13 +4238,16 @@
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C129" t="s">
         <v>10</v>
@@ -3861,13 +4267,16 @@
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C130" t="s">
         <v>4</v>
@@ -3887,13 +4296,16 @@
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -3913,13 +4325,16 @@
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
@@ -3939,13 +4354,16 @@
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -3965,13 +4383,16 @@
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -3991,13 +4412,16 @@
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C135" t="s">
         <v>9</v>
@@ -4017,13 +4441,16 @@
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C136" t="s">
         <v>10</v>
@@ -4043,13 +4470,16 @@
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C137" t="s">
         <v>4</v>
@@ -4069,13 +4499,16 @@
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C138" t="s">
         <v>5</v>
@@ -4095,13 +4528,16 @@
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C139" t="s">
         <v>6</v>
@@ -4121,13 +4557,16 @@
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -4147,13 +4586,16 @@
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C141" t="s">
         <v>8</v>
@@ -4173,13 +4615,16 @@
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -4199,13 +4644,16 @@
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C143" t="s">
         <v>10</v>
@@ -4225,16 +4673,19 @@
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>55</v>
-      </c>
-      <c r="B144" t="s">
+        <v>54</v>
+      </c>
+      <c r="B144" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C144" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D144">
         <v>2014</v>
@@ -4251,13 +4702,19 @@
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" t="s">
+        <v>59</v>
+      </c>
+      <c r="K144" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>55</v>
-      </c>
-      <c r="B145" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -4277,13 +4734,16 @@
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>55</v>
-      </c>
-      <c r="B146" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -4303,13 +4763,16 @@
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>55</v>
-      </c>
-      <c r="B147" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -4329,13 +4792,16 @@
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>55</v>
-      </c>
-      <c r="B148" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C148" t="s">
         <v>8</v>
@@ -4355,13 +4821,16 @@
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>55</v>
-      </c>
-      <c r="B149" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C149" t="s">
         <v>9</v>
@@ -4381,13 +4850,16 @@
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>55</v>
-      </c>
-      <c r="B150" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C150" t="s">
         <v>10</v>
@@ -4407,13 +4879,16 @@
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>55</v>
-      </c>
-      <c r="B151" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C151" t="s">
         <v>11</v>
@@ -4433,16 +4908,19 @@
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>55</v>
-      </c>
-      <c r="B152" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C152" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D152">
         <v>2014</v>
@@ -4459,16 +4937,19 @@
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>55</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B153" t="s">
-        <v>56</v>
-      </c>
       <c r="C153" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D153">
         <v>2014</v>
@@ -4485,13 +4966,16 @@
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>55</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B154" t="s">
-        <v>56</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>
@@ -4511,13 +4995,16 @@
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>55</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B155" t="s">
-        <v>56</v>
       </c>
       <c r="C155" t="s">
         <v>6</v>
@@ -4537,13 +5024,16 @@
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>55</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B156" t="s">
-        <v>56</v>
       </c>
       <c r="C156" t="s">
         <v>7</v>
@@ -4563,13 +5053,16 @@
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>55</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B157" t="s">
-        <v>56</v>
       </c>
       <c r="C157" t="s">
         <v>8</v>
@@ -4589,13 +5082,16 @@
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>55</v>
+      </c>
+      <c r="B158" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B158" t="s">
-        <v>56</v>
       </c>
       <c r="C158" t="s">
         <v>9</v>
@@ -4615,13 +5111,16 @@
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>55</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B159" t="s">
-        <v>56</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
@@ -4641,13 +5140,16 @@
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>55</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B160" t="s">
-        <v>56</v>
       </c>
       <c r="C160" t="s">
         <v>11</v>
@@ -4667,16 +5169,19 @@
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
+      <c r="J160" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>55</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B161" t="s">
-        <v>56</v>
-      </c>
       <c r="C161" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D161">
         <v>2014</v>
@@ -4693,595 +5198,232 @@
       </c>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
-    </row>
-    <row r="162" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D162" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E162" s="1">
-        <v>6</v>
-      </c>
-      <c r="F162" s="1">
-        <v>48</v>
-      </c>
-      <c r="G162" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.125</v>
-      </c>
+      <c r="J161" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="1"/>
+      <c r="G162" s="6"/>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
-      <c r="J162">
-        <v>0.161</v>
-      </c>
-      <c r="K162" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="K162" s="8"/>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D163" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E163" s="1">
-        <v>12</v>
-      </c>
-      <c r="F163" s="1">
-        <v>221</v>
-      </c>
-      <c r="G163" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4298642533936653E-2</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="6"/>
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
-      <c r="J163">
-        <v>0.161</v>
-      </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D164" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E164" s="1">
-        <v>31</v>
-      </c>
-      <c r="F164" s="1">
-        <v>243</v>
-      </c>
-      <c r="G164" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.12757201646090535</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="6"/>
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
-      <c r="J164">
-        <v>0.161</v>
-      </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D165" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E165" s="1">
-        <v>27</v>
-      </c>
-      <c r="F165" s="1">
-        <v>175</v>
-      </c>
-      <c r="G165" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>0.15428571428571428</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="6"/>
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
-      <c r="J165">
-        <v>0.129</v>
-      </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D166" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E166" s="1">
-        <v>33</v>
-      </c>
-      <c r="F166" s="1">
-        <v>407</v>
-      </c>
-      <c r="G166" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>8.1081081081081086E-2</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="6"/>
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
-      <c r="J166">
-        <v>0.129</v>
-      </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D167" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E167" s="1">
-        <v>8</v>
-      </c>
-      <c r="F167" s="1">
-        <v>147</v>
-      </c>
-      <c r="G167" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>5.4421768707482991E-2</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="6"/>
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
-      <c r="J167">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D168" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E168" s="1">
-        <v>6</v>
-      </c>
-      <c r="F168" s="1">
-        <v>76</v>
-      </c>
-      <c r="G168" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.8947368421052627E-2</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="6"/>
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
-      <c r="J168">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D169" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E169" s="1">
-        <v>2</v>
-      </c>
-      <c r="F169" s="1">
-        <v>28</v>
-      </c>
-      <c r="G169" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="6"/>
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
-      <c r="J169">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D170" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E170" s="1">
-        <v>1</v>
-      </c>
-      <c r="F170" s="1">
-        <f>26/2</f>
-        <v>13</v>
-      </c>
-      <c r="G170" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="6"/>
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
-      <c r="J170">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D171" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E171" s="1">
-        <v>1</v>
-      </c>
-      <c r="F171" s="1">
-        <f>26/2</f>
-        <v>13</v>
-      </c>
-      <c r="G171" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="6"/>
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
-      <c r="J171">
-        <v>0.33300000000000002</v>
-      </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D172" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E172" s="1">
-        <v>3</v>
-      </c>
-      <c r="F172" s="1">
-        <v>191</v>
-      </c>
-      <c r="G172" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.5706806282722512E-2</v>
-      </c>
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="6"/>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
-      <c r="J172">
-        <v>0.13600000000000001</v>
-      </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D173" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E173" s="1">
-        <v>19</v>
-      </c>
-      <c r="F173" s="1">
-        <v>693</v>
-      </c>
-      <c r="G173" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.7417027417027416E-2</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="6"/>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
-      <c r="J173">
-        <v>0.13600000000000001</v>
-      </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D174" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E174" s="1">
-        <v>14</v>
-      </c>
-      <c r="F174" s="1">
-        <v>662</v>
-      </c>
-      <c r="G174" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1148036253776436E-2</v>
-      </c>
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="6"/>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
-      <c r="J174">
-        <v>0.13600000000000001</v>
-      </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D175" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E175" s="1">
-        <v>24</v>
-      </c>
-      <c r="F175" s="1">
-        <v>666</v>
-      </c>
-      <c r="G175" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.6036036036036036E-2</v>
-      </c>
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="6"/>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
-      <c r="J175">
-        <v>0.20799999999999999</v>
-      </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D176" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E176" s="1">
-        <v>65</v>
-      </c>
-      <c r="F176" s="4">
-        <v>2272</v>
-      </c>
-      <c r="G176" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.8609154929577465E-2</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="6"/>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
-      <c r="J176">
-        <v>0.20799999999999999</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D177" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E177" s="1">
-        <v>44</v>
-      </c>
-      <c r="F177" s="4">
-        <v>1400</v>
-      </c>
-      <c r="G177" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.1428571428571431E-2</v>
-      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="6"/>
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
-      <c r="J177">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D178" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E178" s="1">
-        <v>30</v>
-      </c>
-      <c r="F178" s="1">
-        <v>982</v>
-      </c>
-      <c r="G178" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>3.0549898167006109E-2</v>
-      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="6"/>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
-      <c r="J178">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D179" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E179" s="1">
-        <v>13</v>
-      </c>
-      <c r="F179" s="1">
-        <v>617</v>
-      </c>
-      <c r="G179" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>2.1069692058346839E-2</v>
-      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="6"/>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
-      <c r="J179">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D180" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E180" s="1">
-        <v>4</v>
-      </c>
-      <c r="F180" s="1">
-        <f>567/2</f>
-        <v>283.5</v>
-      </c>
-      <c r="G180" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
-      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="6"/>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
-      <c r="J180">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D181" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E181" s="1">
-        <v>4</v>
-      </c>
-      <c r="F181" s="1">
-        <f>567/2</f>
-        <v>283.5</v>
-      </c>
-      <c r="G181" s="6">
-        <f>Table1[Pos]/Table1[N]</f>
-        <v>1.4109347442680775E-2</v>
-      </c>
+    </row>
+    <row r="181" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="6"/>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
-      <c r="J181">
-        <v>0.28899999999999998</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="182" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add CC type distribution to calibration targets.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="84">
   <si>
     <t>N</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Africa Centre cohort (now on AHRI) for KZN. Can access the HIV prevalence estimates by putting in a data request ("ACDIS:HIV Surveillance 2010-2016.Release 2016-12").</t>
   </si>
   <si>
-    <t>Questions/Comments</t>
-  </si>
-  <si>
     <t>Occurances</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t xml:space="preserve">Reference unverified. Reference found does not stratify by HIV status. Looks like the HIV+ and HIV- values were swapped. The following references support that these values were swapped, as they all report higher prevalence among HIV-positive than HIV-negative women at all stages of infection, except in ICC when prevalence is similar: McDonald et al. 2014; Adebamowo et al. 2017; De Vuyst et al. 2011. Instead of using these data, we will use the above data on prevalence among women with CIN2/3 and the data below from McDonald 2014 on the prevalence among women regardless of cytology status. </t>
   </si>
   <si>
-    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts included women aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive. Note these statistics are for any HPV prevalence, not hrHPV specifically. Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution.</t>
-  </si>
-  <si>
     <t>15–19 years</t>
   </si>
   <si>
@@ -246,6 +240,36 @@
   </si>
   <si>
     <t>Prev/Inc Rate</t>
+  </si>
+  <si>
+    <t>Samples were collected 2006-2009. Compare to year 2008 to get roughly the middle of this interval. I believe the study would have included people on ART as HIV-positive. The 95% CI were derived from the published point estimates as p +/- sqrt(p*(1-p)/n)*1.96. Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
+  </si>
+  <si>
+    <t>Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
+  </si>
+  <si>
+    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts included women aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive. Note these statistics are for any HPV prevalence, not hrHPV specifically. Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
+  </si>
+  <si>
+    <t>See notes</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>all women</t>
+  </si>
+  <si>
+    <t>Guan (2012) IJC.</t>
+  </si>
+  <si>
+    <t>Proportion CC attributable to 9v HPV</t>
+  </si>
+  <si>
+    <t>Proportion CC attributable to non-9v HPV</t>
+  </si>
+  <si>
+    <t>Guan (2012) is a meta-analysis reporting HPV type distribution for Africa based on studies from 1990 to 2011. Going to compare to year 2011. Number of women from African studies who were HPV-positive and had ICC was 2402. Assume a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
   </si>
   <si>
     <r>
@@ -258,16 +282,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.8000000000000007"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>=λ and variance=λ  and λ =CC incidence rate per year</t>
+      <t>µ=λ and variance=λ  and λ =CC incidence rate per year</t>
     </r>
     <r>
       <rPr>
@@ -291,16 +306,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.8000000000000007"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>=prevalence proportion (p) and variance=(p(1-p))/n</t>
+      <t>µ=prevalence proportion (p) and variance=(p(1-p))/n</t>
     </r>
     <r>
       <rPr>
@@ -312,21 +318,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>Samples were collected 2006-2009. Compare to year 2008 to get roughly the middle of this interval. I believe the study would have included people on ART as HIV-positive. The 95% CI were derived from the published point estimates as p +/- sqrt(p*(1-p)/n)*1.96. Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
-  </si>
-  <si>
-    <t>Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
-  </si>
-  <si>
-    <t>Data are from 3 cohorts of women recruited in 1998-1999, 2000-2002, and 2004-2006. The first 2 cohorts included women aged 35-65, and the 3rd cohort included women age 17-34. Data are pulled from the supplemental appendix, and were not presented disaggregated by year. Let's compare to 2002 as it falls in the middle of the range, but make note of the lack of precision for temporal trends. I believe persons on ART were included as HIV-positive. Note these statistics are for any HPV prevalence, not hrHPV specifically. Initially assumed a binomial distribution. Now assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
-  </si>
-  <si>
-    <t>See notes</t>
-  </si>
-  <si>
-    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -348,10 +339,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8.8000000000000007"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -374,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -398,22 +390,26 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -444,14 +440,14 @@
     <tableColumn id="4" name="Prev/Inc Rate" dataDxfId="4">
       <calculatedColumnFormula>Table1[Occurances]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Mean" dataDxfId="1">
+    <tableColumn id="13" name="Mean" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[Prev/Inc Rate]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Variance" dataDxfId="0">
+    <tableColumn id="12" name="Variance" dataDxfId="2">
       <calculatedColumnFormula>(Table1[[#This Row],[Prev/Inc Rate]]*(1-Table1[[#This Row],[Prev/Inc Rate]]))/Table1[[#This Row],[N]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="3"/>
-    <tableColumn id="6" name="UB" dataDxfId="2"/>
+    <tableColumn id="5" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" name="UB" dataDxfId="0"/>
     <tableColumn id="8" name="Usage Status"/>
     <tableColumn id="11" name="Comments"/>
   </tableColumns>
@@ -724,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F175" sqref="F175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,7 +733,8 @@
     <col min="5" max="5" width="14.36328125" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" customWidth="1"/>
-    <col min="8" max="9" width="13.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
     <col min="12" max="12" width="14.81640625" customWidth="1"/>
     <col min="13" max="13" width="43.453125" customWidth="1"/>
   </cols>
@@ -756,19 +753,19 @@
         <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J1" t="s">
         <v>35</v>
@@ -780,10 +777,10 @@
         <v>57</v>
       </c>
       <c r="M1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="188.5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -817,8 +814,8 @@
       <c r="L2" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>75</v>
+      <c r="M2" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1525,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -2590,7 +2587,7 @@
         <v>58</v>
       </c>
       <c r="M52" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
@@ -2915,7 +2912,7 @@
         <v>58</v>
       </c>
       <c r="M60" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
@@ -6007,8 +6004,8 @@
       <c r="L144" t="s">
         <v>58</v>
       </c>
-      <c r="M144" s="8" t="s">
-        <v>78</v>
+      <c r="M144" s="14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.35">
@@ -6642,13 +6639,13 @@
     </row>
     <row r="162" spans="1:13" ht="203" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D162" s="1">
         <v>2011</v>
@@ -6676,16 +6673,16 @@
       <c r="L162" t="s">
         <v>58</v>
       </c>
-      <c r="M162" s="8" t="s">
-        <v>74</v>
+      <c r="M162" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>13</v>
@@ -6704,11 +6701,11 @@
         <v>0.22319525433322426</v>
       </c>
       <c r="H163" s="1">
-        <f t="shared" ref="H163:H174" si="1">G163</f>
+        <f t="shared" ref="H163:H175" si="1">G163</f>
         <v>0.22319525433322426</v>
       </c>
       <c r="I163" s="6">
-        <f t="shared" ref="I163:I174" si="2">H163</f>
+        <f t="shared" ref="I163:I175" si="2">H163</f>
         <v>0.22319525433322426</v>
       </c>
       <c r="J163" s="7"/>
@@ -6719,10 +6716,10 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>14</v>
@@ -6756,10 +6753,10 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>15</v>
@@ -6793,10 +6790,10 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>16</v>
@@ -6830,10 +6827,10 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>17</v>
@@ -6867,10 +6864,10 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>18</v>
@@ -6904,10 +6901,10 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>19</v>
@@ -6941,10 +6938,10 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>20</v>
@@ -6978,13 +6975,13 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D171" s="1">
         <v>2011</v>
@@ -7015,13 +7012,13 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D172" s="1">
         <v>2011</v>
@@ -7052,13 +7049,13 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D173" s="1">
         <v>2011</v>
@@ -7089,13 +7086,13 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D174" s="1">
         <v>2011</v>
@@ -7124,30 +7121,73 @@
         <v>58</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
-      <c r="D175" s="1"/>
+    <row r="175" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+      <c r="A175" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B175" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D175" s="12">
+        <v>2011</v>
+      </c>
       <c r="E175" s="12"/>
       <c r="F175" s="11"/>
-      <c r="G175" s="6"/>
-      <c r="H175" s="6"/>
-      <c r="I175" s="6"/>
+      <c r="G175" s="6">
+        <f>0.531+0.198+0.219</f>
+        <v>0.94800000000000006</v>
+      </c>
+      <c r="H175" s="13">
+        <f t="shared" si="1"/>
+        <v>0.94800000000000006</v>
+      </c>
+      <c r="I175" s="6">
+        <f>(H175*(1-H175))/2402</f>
+        <v>2.0522897585345521E-5</v>
+      </c>
       <c r="J175" s="7"/>
       <c r="K175" s="7"/>
+      <c r="L175" t="s">
+        <v>58</v>
+      </c>
+      <c r="M175" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
-      <c r="C176" s="1"/>
-      <c r="D176" s="1"/>
+      <c r="A176" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B176" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D176" s="12">
+        <v>2011</v>
+      </c>
       <c r="E176" s="1"/>
       <c r="F176" s="4"/>
-      <c r="G176" s="6"/>
-      <c r="H176" s="6"/>
-      <c r="I176" s="6"/>
+      <c r="G176" s="6">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="H176" s="13">
+        <f>G176</f>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I176" s="6">
+        <f>(H176*(1-H176))/2402</f>
+        <v>2.0522897585345542E-5</v>
+      </c>
       <c r="J176" s="7"/>
       <c r="K176" s="7"/>
+      <c r="L176" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" s="1"/>

</xml_diff>

<commit_message>
Update baseline transition rates to values that best fit type distribution with hand calibration. Add CIN3, CIN1, and HPV type distributions as calibration targets and update Calibration_taragets Excel doc, calibData.mat, and likeFun accordingly. Comment out HIV data as calibration targets for HPV transition rates.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="93">
   <si>
     <t>N</t>
   </si>
@@ -319,12 +319,39 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>Proportion HPV attributable to 9v HPV</t>
+  </si>
+  <si>
+    <t>Proportion CIN1 attributable to 9v HPV</t>
+  </si>
+  <si>
+    <t>Proportion CIN3 attributable to 9v HPV</t>
+  </si>
+  <si>
+    <t>Proportion HPV attributable to non-9v HPV</t>
+  </si>
+  <si>
+    <t>Proportion CIN1 attributable to non-9v HPV</t>
+  </si>
+  <si>
+    <t>Proportion CIN3 attributable to non-9v HPV</t>
+  </si>
+  <si>
+    <t>Number of women from African studies who were HPV-positive and had normal cytology was 2221.</t>
+  </si>
+  <si>
+    <t>Number of women from African studies who were HPV-positive and had LSIL was 299.</t>
+  </si>
+  <si>
+    <t>Number of women from African studies who were HPV-positive and had HSIL was 185.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,13 +364,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -720,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G189" sqref="G189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6705,7 +6725,7 @@
         <v>0.22319525433322426</v>
       </c>
       <c r="I163" s="6">
-        <f t="shared" ref="I163:I175" si="2">H163</f>
+        <f t="shared" ref="I163:I174" si="2">H163</f>
         <v>0.22319525433322426</v>
       </c>
       <c r="J163" s="7"/>
@@ -7188,73 +7208,190 @@
       <c r="L176" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
-      <c r="D177" s="1"/>
+      <c r="M176" s="8"/>
+    </row>
+    <row r="177" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A177" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B177" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C177" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D177" s="12">
+        <v>2011</v>
+      </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
-      <c r="G177" s="6"/>
-      <c r="H177" s="6"/>
-      <c r="I177" s="6"/>
+      <c r="G177" s="6">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H177" s="13">
+        <f t="shared" ref="H177:H182" si="3">G177</f>
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="I177" s="6">
+        <f>(H177*(1-H177))/2221</f>
+        <v>1.0953444394416931E-4</v>
+      </c>
       <c r="J177" s="7"/>
       <c r="K177" s="7"/>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
-      <c r="D178" s="1"/>
+      <c r="M177" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A178" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B178" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C178" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D178" s="12">
+        <v>2011</v>
+      </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
-      <c r="G178" s="6"/>
-      <c r="H178" s="6"/>
-      <c r="I178" s="6"/>
+      <c r="G178" s="6">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="H178" s="13">
+        <f t="shared" si="3"/>
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="I178" s="6">
+        <f>(H178*(1-H178))/2221</f>
+        <v>1.0953444394416931E-4</v>
+      </c>
       <c r="J178" s="7"/>
       <c r="K178" s="7"/>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
-      <c r="D179" s="1"/>
+      <c r="M178" s="8"/>
+    </row>
+    <row r="179" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A179" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B179" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C179" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D179" s="12">
+        <v>2011</v>
+      </c>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
-      <c r="G179" s="6"/>
-      <c r="H179" s="6"/>
-      <c r="I179" s="6"/>
+      <c r="G179" s="6">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="H179" s="13">
+        <f t="shared" si="3"/>
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="I179" s="6">
+        <f>(H179*(1-H179))/299</f>
+        <v>7.3832441471571896E-4</v>
+      </c>
       <c r="J179" s="7"/>
       <c r="K179" s="7"/>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
-      <c r="D180" s="1"/>
+      <c r="M179" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A180" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B180" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D180" s="12">
+        <v>2011</v>
+      </c>
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
-      <c r="G180" s="6"/>
-      <c r="H180" s="6"/>
-      <c r="I180" s="6"/>
+      <c r="G180" s="6">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="H180" s="13">
+        <f t="shared" si="3"/>
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="I180" s="6">
+        <f>(H180*(1-H180))/299</f>
+        <v>7.3832441471571907E-4</v>
+      </c>
       <c r="J180" s="7"/>
       <c r="K180" s="7"/>
-    </row>
-    <row r="181" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
+      <c r="M180" s="8"/>
+    </row>
+    <row r="181" spans="1:13" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B181" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C181" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D181" s="12">
+        <v>2011</v>
+      </c>
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
-      <c r="G181" s="6"/>
-      <c r="H181" s="6"/>
-      <c r="I181" s="6"/>
+      <c r="G181" s="6">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="H181" s="13">
+        <f t="shared" si="3"/>
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="I181" s="6">
+        <f>(H181*(1-H181))/185</f>
+        <v>7.6626486486486495E-4</v>
+      </c>
       <c r="J181" s="7"/>
       <c r="K181" s="7"/>
-    </row>
-    <row r="182" spans="1:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="M181" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B182" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D182" s="12">
+        <v>2011</v>
+      </c>
+      <c r="G182" s="6">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H182" s="13">
+        <f t="shared" si="3"/>
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="I182" s="6">
+        <f>(H182*(1-H182))/185</f>
+        <v>7.6626486486486485E-4</v>
+      </c>
+      <c r="M182" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update HPV type distribution calibration targets based on more literature sources. Calculate variance.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="97">
   <si>
     <t>N</t>
   </si>
@@ -270,30 +270,6 @@
   </si>
   <si>
     <t>Guan (2012) is a meta-analysis reporting HPV type distribution for Africa based on studies from 1990 to 2011. Going to compare to year 2011. Number of women from African studies who were HPV-positive and had ICC was 2402. Assume a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Population by five-year age groups and sex come from the Statistics South Africa 2011 Census as used by NCR to calculate incidence (Census Products/Census in Brief p.30 found at http://www.statssa.gov.za/census/census_2011/census_products/Census_2011_Census_in_brief.pdf). The frequency of histologically diagnosed cervical cancer in South African black females (most common ethnic group by far in SA) is used for the number of new cases.  Incidence rates converted to per 100,000 women. Assume a normal approximation of the Poisson distribution where </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>µ=λ and variance=λ  and λ =CC incidence rate per year</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -346,12 +322,52 @@
   <si>
     <t>Number of women from African studies who were HPV-positive and had HSIL was 185.</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Population by five-year age groups and sex come from the Statistics South Africa 2011 Census as used by NCR to calculate incidence (Census Products/Census in Brief p.30 found at http://www.statssa.gov.za/census/census_2011/census_products/Census_2011_Census_in_brief.pdf). The frequency of histologically diagnosed cervical cancer in South African black females (most common ethnic group by far in SA) is used for the number of new cases.  Incidence rates converted to per 100,000 women. Assume a normal approximation of the Poisson distribution where </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ=λ and variance=λ  and λ=CC incidence rate per year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Mean type distribution is an average of Bruni, de Sanjose for Africa, Denny, van Aardt (2015) from HPV_parameters Excel document "Plots and final type dist" tab. Denny and van Aardt both have small sample sizes but are South Africa-specific. Number of women who were HPV-positive and had ICC was 2000 for Bruni (assumed b/c compilation of several studies), 544 for de Sanjose, 181 for Denny, and 197 for van Aardt (2015). Assume a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n. Variance calculated for the average as = (1/n)^2 * (sum of the variances).</t>
+  </si>
+  <si>
+    <t>Mean type distribution is an average of Bruni and van Aardt (2013) from HPV_parameters Excel document "Plots and final type dist" tab. Both are South Africa. Bruni estimates sum to 100 (they don’t say how they accounted for multiple infection, but they seem to have), and they are consistent with data from van Aardt, which included 845 women. Number of women who were HPV-positive and had normal cytology was 2000 for Bruni (assumed b/c compilation of several studies) and 845 for van Aardt (2013).</t>
+  </si>
+  <si>
+    <t>Mean type distribution is an average of Bruni and Clifford 2005 from HPV_parameters Excel document "Plots and final type dist" tab. Number of women who were HPV-positive and had low-grade lesions was 2000 for Bruni (assumed b/c compilation of several studies) and 62 for Clifford. Clifford sample size was 62-178 depending on HPV type, so used the smaller size to be conservative.</t>
+  </si>
+  <si>
+    <t>Mean type distribution is an average of Bruni, Dartell, and van Aardt (2016) from HPV_parameters Excel document "Plots and final type dist" tab. Number of women who were HPV-positive and had high-grade lesions was 2000 for Bruni (assumed b/c compilation of several studies), 137 for Dartell, and 270 for van Aardt.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +380,25 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -386,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -414,6 +449,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,28 +797,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M182"/>
+  <dimension ref="A1:X190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G189" sqref="G189"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J185" sqref="J185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="43.453125" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="61.42578125" customWidth="1"/>
+    <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -800,7 +860,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="203" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -835,10 +895,10 @@
         <v>58</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -873,7 +933,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -908,7 +968,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -943,7 +1003,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -978,7 +1038,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1013,7 +1073,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1048,7 +1108,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1083,7 +1143,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1179,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +1215,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1190,7 +1250,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1225,7 +1285,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1260,7 +1320,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1295,7 +1355,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1330,7 +1390,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1365,7 +1425,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1400,7 +1460,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1435,7 +1495,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1471,7 +1531,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1507,7 +1567,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1545,7 +1605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1580,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1615,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1650,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1685,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1720,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1755,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1825,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1860,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -1895,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -1930,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -1965,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2000,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2035,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2070,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2105,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2140,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -2175,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2210,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -2245,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -2280,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
@@ -2315,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -2350,7 +2410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
@@ -2385,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
@@ -2420,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2455,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2492,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -2529,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>26</v>
       </c>
@@ -2566,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -2610,7 +2670,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>29</v>
       </c>
@@ -2651,7 +2711,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
@@ -2692,7 +2752,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2733,7 +2793,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>34</v>
       </c>
@@ -2774,7 +2834,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
@@ -2815,7 +2875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -2856,7 +2916,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>34</v>
       </c>
@@ -2897,7 +2957,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>38</v>
       </c>
@@ -2935,7 +2995,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>38</v>
       </c>
@@ -2970,7 +3030,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -3005,7 +3065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
@@ -3040,7 +3100,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>38</v>
       </c>
@@ -3075,7 +3135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>38</v>
       </c>
@@ -3110,7 +3170,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>38</v>
       </c>
@@ -3145,7 +3205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>39</v>
       </c>
@@ -3180,7 +3240,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>39</v>
       </c>
@@ -3215,7 +3275,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>39</v>
       </c>
@@ -3250,7 +3310,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>39</v>
       </c>
@@ -3287,7 +3347,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>39</v>
       </c>
@@ -3324,7 +3384,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>39</v>
       </c>
@@ -3361,7 +3421,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>39</v>
       </c>
@@ -3398,7 +3458,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>40</v>
       </c>
@@ -3435,7 +3495,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>40</v>
       </c>
@@ -3472,7 +3532,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>40</v>
       </c>
@@ -3509,7 +3569,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>40</v>
       </c>
@@ -3546,7 +3606,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>40</v>
       </c>
@@ -3583,7 +3643,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>40</v>
       </c>
@@ -3620,7 +3680,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>40</v>
       </c>
@@ -3657,7 +3717,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>41</v>
       </c>
@@ -3694,7 +3754,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>41</v>
       </c>
@@ -3731,7 +3791,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>41</v>
       </c>
@@ -3768,7 +3828,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>41</v>
       </c>
@@ -3805,7 +3865,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>41</v>
       </c>
@@ -3842,7 +3902,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>41</v>
       </c>
@@ -3879,7 +3939,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -3916,7 +3976,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>42</v>
       </c>
@@ -3953,7 +4013,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>42</v>
       </c>
@@ -3990,7 +4050,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>42</v>
       </c>
@@ -4027,7 +4087,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
@@ -4064,7 +4124,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>42</v>
       </c>
@@ -4101,7 +4161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>42</v>
       </c>
@@ -4138,7 +4198,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
@@ -4175,7 +4235,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>43</v>
       </c>
@@ -4212,7 +4272,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>43</v>
       </c>
@@ -4249,7 +4309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>43</v>
       </c>
@@ -4286,7 +4346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>43</v>
       </c>
@@ -4323,7 +4383,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>43</v>
       </c>
@@ -4360,7 +4420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>43</v>
       </c>
@@ -4397,7 +4457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>43</v>
       </c>
@@ -4434,7 +4494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>44</v>
       </c>
@@ -4471,7 +4531,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>44</v>
       </c>
@@ -4508,7 +4568,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>44</v>
       </c>
@@ -4545,7 +4605,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>44</v>
       </c>
@@ -4582,7 +4642,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>44</v>
       </c>
@@ -4619,7 +4679,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>44</v>
       </c>
@@ -4656,7 +4716,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>44</v>
       </c>
@@ -4693,7 +4753,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>45</v>
       </c>
@@ -4730,7 +4790,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>45</v>
       </c>
@@ -4767,7 +4827,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>45</v>
       </c>
@@ -4804,7 +4864,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>45</v>
       </c>
@@ -4841,7 +4901,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>45</v>
       </c>
@@ -4878,7 +4938,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>45</v>
       </c>
@@ -4915,7 +4975,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>45</v>
       </c>
@@ -4952,7 +5012,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>46</v>
       </c>
@@ -4989,7 +5049,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>46</v>
       </c>
@@ -5026,7 +5086,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>46</v>
       </c>
@@ -5063,7 +5123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>46</v>
       </c>
@@ -5100,7 +5160,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>46</v>
       </c>
@@ -5137,7 +5197,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>46</v>
       </c>
@@ -5174,7 +5234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>46</v>
       </c>
@@ -5211,7 +5271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>47</v>
       </c>
@@ -5248,7 +5308,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>47</v>
       </c>
@@ -5285,7 +5345,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>47</v>
       </c>
@@ -5322,7 +5382,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>47</v>
       </c>
@@ -5359,7 +5419,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>47</v>
       </c>
@@ -5396,7 +5456,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>47</v>
       </c>
@@ -5433,7 +5493,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>47</v>
       </c>
@@ -5470,7 +5530,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>48</v>
       </c>
@@ -5507,7 +5567,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>48</v>
       </c>
@@ -5544,7 +5604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>48</v>
       </c>
@@ -5581,7 +5641,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>48</v>
       </c>
@@ -5618,7 +5678,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>48</v>
       </c>
@@ -5655,7 +5715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>48</v>
       </c>
@@ -5692,7 +5752,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>48</v>
       </c>
@@ -5729,7 +5789,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>49</v>
       </c>
@@ -5766,7 +5826,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>49</v>
       </c>
@@ -5803,7 +5863,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>49</v>
       </c>
@@ -5840,7 +5900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>49</v>
       </c>
@@ -5877,7 +5937,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>49</v>
       </c>
@@ -5914,7 +5974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>49</v>
       </c>
@@ -5951,7 +6011,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>49</v>
       </c>
@@ -5988,7 +6048,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>53</v>
       </c>
@@ -6028,7 +6088,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>53</v>
       </c>
@@ -6065,7 +6125,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -6102,7 +6162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>53</v>
       </c>
@@ -6139,7 +6199,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>53</v>
       </c>
@@ -6176,7 +6236,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>53</v>
       </c>
@@ -6213,7 +6273,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>53</v>
       </c>
@@ -6250,7 +6310,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>53</v>
       </c>
@@ -6287,7 +6347,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>53</v>
       </c>
@@ -6324,7 +6384,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>54</v>
       </c>
@@ -6361,7 +6421,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>54</v>
       </c>
@@ -6398,7 +6458,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>54</v>
       </c>
@@ -6435,7 +6495,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>54</v>
       </c>
@@ -6472,7 +6532,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>54</v>
       </c>
@@ -6509,7 +6569,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>54</v>
       </c>
@@ -6546,7 +6606,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>54</v>
       </c>
@@ -6583,7 +6643,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>54</v>
       </c>
@@ -6620,7 +6680,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>54</v>
       </c>
@@ -6657,7 +6717,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="203" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>70</v>
       </c>
@@ -6694,10 +6754,10 @@
         <v>58</v>
       </c>
       <c r="M162" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>70</v>
       </c>
@@ -6734,7 +6794,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>70</v>
       </c>
@@ -6771,7 +6831,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>70</v>
       </c>
@@ -6808,7 +6868,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>70</v>
       </c>
@@ -6845,7 +6905,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>70</v>
       </c>
@@ -6882,7 +6942,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>70</v>
       </c>
@@ -6919,7 +6979,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>70</v>
       </c>
@@ -6956,7 +7016,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>70</v>
       </c>
@@ -6993,7 +7053,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>70</v>
       </c>
@@ -7030,7 +7090,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>70</v>
       </c>
@@ -7067,7 +7127,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>70</v>
       </c>
@@ -7104,7 +7164,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>70</v>
       </c>
@@ -7141,7 +7201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>79</v>
       </c>
@@ -7171,13 +7231,13 @@
       <c r="J175" s="7"/>
       <c r="K175" s="7"/>
       <c r="L175" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="M175" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
         <v>80</v>
       </c>
@@ -7206,13 +7266,13 @@
       <c r="J176" s="7"/>
       <c r="K176" s="7"/>
       <c r="L176" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="M176" s="8"/>
     </row>
-    <row r="177" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B177" s="12" t="s">
         <v>78</v>
@@ -7238,13 +7298,16 @@
       </c>
       <c r="J177" s="7"/>
       <c r="K177" s="7"/>
+      <c r="L177" t="s">
+        <v>0</v>
+      </c>
       <c r="M177" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B178" s="12" t="s">
         <v>78</v>
@@ -7270,11 +7333,14 @@
       </c>
       <c r="J178" s="7"/>
       <c r="K178" s="7"/>
+      <c r="L178" t="s">
+        <v>0</v>
+      </c>
       <c r="M178" s="8"/>
     </row>
-    <row r="179" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B179" s="12" t="s">
         <v>78</v>
@@ -7300,13 +7366,16 @@
       </c>
       <c r="J179" s="7"/>
       <c r="K179" s="7"/>
+      <c r="L179" t="s">
+        <v>0</v>
+      </c>
       <c r="M179" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B180" s="12" t="s">
         <v>78</v>
@@ -7332,11 +7401,14 @@
       </c>
       <c r="J180" s="7"/>
       <c r="K180" s="7"/>
+      <c r="L180" t="s">
+        <v>0</v>
+      </c>
       <c r="M180" s="8"/>
     </row>
-    <row r="181" spans="1:13" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:24" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B181" s="12" t="s">
         <v>78</v>
@@ -7362,13 +7434,16 @@
       </c>
       <c r="J181" s="7"/>
       <c r="K181" s="7"/>
+      <c r="L181" t="s">
+        <v>0</v>
+      </c>
       <c r="M181" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="182" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B182" s="12" t="s">
         <v>78</v>
@@ -7390,7 +7465,414 @@
         <f>(H182*(1-H182))/185</f>
         <v>7.6626486486486485E-4</v>
       </c>
+      <c r="L182" t="s">
+        <v>0</v>
+      </c>
       <c r="M182" s="8"/>
+    </row>
+    <row r="183" spans="1:24" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G183" s="17">
+        <f>1-G184</f>
+        <v>0.85780595009985727</v>
+      </c>
+      <c r="H183" s="17">
+        <f>G183</f>
+        <v>0.85780595009985727</v>
+      </c>
+      <c r="I183">
+        <f>(0.25^2)*SUM(U183:X183)</f>
+        <v>9.5934786594766949E-5</v>
+      </c>
+      <c r="L183" t="s">
+        <v>58</v>
+      </c>
+      <c r="M183" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="O183" s="27">
+        <f>1-O184</f>
+        <v>0.83819095477386929</v>
+      </c>
+      <c r="P183">
+        <f>1-P184</f>
+        <v>0.86764705882352933</v>
+      </c>
+      <c r="Q183">
+        <f>1-Q184</f>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="R183">
+        <f>1-R184</f>
+        <v>0.8923857868020304</v>
+      </c>
+      <c r="S183" s="28">
+        <f>AVERAGE(O183:R183)</f>
+        <v>0.85780595009985738</v>
+      </c>
+      <c r="U183">
+        <f>(O183*(1-O183))/2000</f>
+        <v>6.7813439054569349E-5</v>
+      </c>
+      <c r="V183">
+        <f>(P183*(1-P183))/544</f>
+        <v>2.1109492672501538E-4</v>
+      </c>
+      <c r="W183">
+        <f>(Q183*(1-Q183))/181</f>
+        <v>7.6856906077348074E-4</v>
+      </c>
+      <c r="X183">
+        <f>(R183*(1-R183))/197</f>
+        <v>4.874791589632058E-4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A184" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G184" s="18">
+        <v>0.14219404990014273</v>
+      </c>
+      <c r="H184" s="17">
+        <f t="shared" ref="H184:H190" si="4">G184</f>
+        <v>0.14219404990014273</v>
+      </c>
+      <c r="I184">
+        <f>(0.25^2)*SUM(U184:X184)</f>
+        <v>9.5934786594766935E-5</v>
+      </c>
+      <c r="L184" t="s">
+        <v>58</v>
+      </c>
+      <c r="O184" s="25">
+        <v>0.16180904522613065</v>
+      </c>
+      <c r="P184" s="19">
+        <v>0.13235294117647067</v>
+      </c>
+      <c r="Q184" s="26">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="R184" s="19">
+        <v>0.10761421319796954</v>
+      </c>
+      <c r="S184" s="28">
+        <f>AVERAGE(O184:R184)</f>
+        <v>0.14219404990014273</v>
+      </c>
+      <c r="U184">
+        <f>(O184*(1-O184))/2000</f>
+        <v>6.7813439054569322E-5</v>
+      </c>
+      <c r="V184">
+        <f>(P184*(1-P184))/544</f>
+        <v>2.1109492672501538E-4</v>
+      </c>
+      <c r="W184">
+        <f>(Q184*(1-Q184))/181</f>
+        <v>7.6856906077348074E-4</v>
+      </c>
+      <c r="X184">
+        <f>(R184*(1-R184))/197</f>
+        <v>4.8747915896320553E-4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G185" s="17">
+        <f>1-G186</f>
+        <v>0.46822135734532</v>
+      </c>
+      <c r="H185" s="17">
+        <f t="shared" si="4"/>
+        <v>0.46822135734532</v>
+      </c>
+      <c r="I185">
+        <f>(0.5^2)*SUM(S185:T185)</f>
+        <v>1.0483495851331361E-4</v>
+      </c>
+      <c r="L185" t="s">
+        <v>58</v>
+      </c>
+      <c r="M185" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="O185">
+        <f>1-O186</f>
+        <v>0.46309999999999996</v>
+      </c>
+      <c r="P185">
+        <f>1-P186</f>
+        <v>0.47340000000000004</v>
+      </c>
+      <c r="Q185" s="20">
+        <f>AVERAGE(O185:P185)</f>
+        <v>0.46825</v>
+      </c>
+      <c r="S185">
+        <f>(O185*(1-O185))/2000</f>
+        <v>1.2431919499999999E-4</v>
+      </c>
+      <c r="T185">
+        <f>(P185*(1-P185))/845</f>
+        <v>2.9502063905325444E-4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A186" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G186" s="17">
+        <v>0.53177864265468</v>
+      </c>
+      <c r="H186" s="17">
+        <f t="shared" si="4"/>
+        <v>0.53177864265468</v>
+      </c>
+      <c r="I186">
+        <f>(0.5^2)*SUM(S186:T186)</f>
+        <v>1.0483495851331361E-4</v>
+      </c>
+      <c r="L186" t="s">
+        <v>58</v>
+      </c>
+      <c r="O186">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="P186" s="19">
+        <v>0.52659999999999996</v>
+      </c>
+      <c r="Q186" s="20">
+        <f>AVERAGE(O186:P186)</f>
+        <v>0.53174999999999994</v>
+      </c>
+      <c r="S186">
+        <f>(O186*(1-O186))/2000</f>
+        <v>1.2431919499999999E-4</v>
+      </c>
+      <c r="T186">
+        <f>(P186*(1-P186))/845</f>
+        <v>2.9502063905325444E-4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C187" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G187" s="17">
+        <f>1-G188</f>
+        <v>0.51915783320342934</v>
+      </c>
+      <c r="H187" s="17">
+        <f t="shared" si="4"/>
+        <v>0.51915783320342934</v>
+      </c>
+      <c r="I187">
+        <f>(0.5^2)*SUM(S187:T187)</f>
+        <v>1.0176762375286258E-3</v>
+      </c>
+      <c r="L187" t="s">
+        <v>58</v>
+      </c>
+      <c r="M187" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="O187" s="22">
+        <f>1-O188</f>
+        <v>0.46531566640685873</v>
+      </c>
+      <c r="P187">
+        <f>1-P188</f>
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="Q187" s="20">
+        <f>AVERAGE(O187:P187)</f>
+        <v>0.51915783320342934</v>
+      </c>
+      <c r="S187">
+        <f>(O187*(1-O187))/2000</f>
+        <v>1.2439849850159985E-4</v>
+      </c>
+      <c r="T187">
+        <f>(P187*(1-P187))/62</f>
+        <v>3.9463064516129034E-3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A188" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G188" s="17">
+        <v>0.48084216679657066</v>
+      </c>
+      <c r="H188" s="17">
+        <f t="shared" si="4"/>
+        <v>0.48084216679657066</v>
+      </c>
+      <c r="I188">
+        <f>(0.5^2)*SUM(S188:T188)</f>
+        <v>1.0176762375286258E-3</v>
+      </c>
+      <c r="L188" t="s">
+        <v>58</v>
+      </c>
+      <c r="O188" s="21">
+        <v>0.53468433359314127</v>
+      </c>
+      <c r="P188" s="16">
+        <v>0.42700000000000005</v>
+      </c>
+      <c r="Q188" s="20">
+        <f>AVERAGE(O188:P188)</f>
+        <v>0.48084216679657066</v>
+      </c>
+      <c r="S188">
+        <f>(O188*(1-O188))/2000</f>
+        <v>1.2439849850159985E-4</v>
+      </c>
+      <c r="T188">
+        <f>(P188*(1-P188))/62</f>
+        <v>3.9463064516129034E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+      <c r="A189" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C189" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G189" s="17">
+        <f>1-G190</f>
+        <v>0.73709892344552175</v>
+      </c>
+      <c r="H189" s="17">
+        <f t="shared" si="4"/>
+        <v>0.73709892344552175</v>
+      </c>
+      <c r="I189">
+        <f>((1/3)^2)*SUM(V189:X189)</f>
+        <v>2.4583988317562153E-4</v>
+      </c>
+      <c r="L189" t="s">
+        <v>58</v>
+      </c>
+      <c r="M189" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="O189" s="22">
+        <f>1-O190</f>
+        <v>0.58539765319426329</v>
+      </c>
+      <c r="P189" s="22">
+        <f t="shared" ref="P189:R189" si="5">1-P190</f>
+        <v>0.67319804058782362</v>
+      </c>
+      <c r="Q189" s="22">
+        <f t="shared" si="5"/>
+        <v>0.85680000000000001</v>
+      </c>
+      <c r="R189" s="22">
+        <f t="shared" si="5"/>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="S189" s="22">
+        <f>AVERAGE(Q189:R189)</f>
+        <v>0.84489999999999998</v>
+      </c>
+      <c r="T189" s="24">
+        <f>AVERAGE(O189:S189)</f>
+        <v>0.75865913875641744</v>
+      </c>
+      <c r="V189">
+        <f>(O189*(1-O189))/2000</f>
+        <v>1.2135362041445617E-4</v>
+      </c>
+      <c r="W189">
+        <f>(P189*(1-P189))/137</f>
+        <v>1.6058572170550263E-3</v>
+      </c>
+      <c r="X189">
+        <f>(S189*(1-S189))/270</f>
+        <v>4.8534811111111112E-4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A190" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C190" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G190" s="17">
+        <v>0.26290107655447825</v>
+      </c>
+      <c r="H190" s="17">
+        <f t="shared" si="4"/>
+        <v>0.26290107655447825</v>
+      </c>
+      <c r="I190">
+        <f>((1/3)^2)*SUM(V190:X190)</f>
+        <v>2.4583988317562153E-4</v>
+      </c>
+      <c r="L190" t="s">
+        <v>58</v>
+      </c>
+      <c r="O190" s="21">
+        <v>0.41460234680573665</v>
+      </c>
+      <c r="P190" s="23">
+        <v>0.32680195941217638</v>
+      </c>
+      <c r="Q190" s="16">
+        <v>0.14319999999999999</v>
+      </c>
+      <c r="R190" s="16">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="S190" s="22">
+        <f>AVERAGE(Q190:R190)</f>
+        <v>0.15510000000000002</v>
+      </c>
+      <c r="T190" s="24">
+        <f>AVERAGE(O190:R190)</f>
+        <v>0.26290107655447825</v>
+      </c>
+      <c r="V190">
+        <f>(O190*(1-O190))/2000</f>
+        <v>1.2135362041445614E-4</v>
+      </c>
+      <c r="W190">
+        <f>(P190*(1-P190))/137</f>
+        <v>1.6058572170550263E-3</v>
+      </c>
+      <c r="X190">
+        <f>(S190*(1-S190))/270</f>
+        <v>4.8534811111111112E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update HPV type distribution calibration data labels.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="97">
   <si>
     <t>N</t>
   </si>
@@ -364,8 +364,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -453,26 +453,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +800,7 @@
   <dimension ref="A1:X190"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J185" sqref="J185"/>
+      <selection activeCell="G185" sqref="G185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7474,8 +7474,14 @@
       <c r="A183" s="15" t="s">
         <v>79</v>
       </c>
+      <c r="B183" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C183" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D183" s="12">
+        <v>2011</v>
       </c>
       <c r="G183" s="17">
         <f>1-G184</f>
@@ -7536,8 +7542,14 @@
       <c r="A184" s="15" t="s">
         <v>80</v>
       </c>
+      <c r="B184" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C184" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D184" s="12">
+        <v>2011</v>
       </c>
       <c r="G184" s="18">
         <v>0.14219404990014273</v>
@@ -7590,8 +7602,14 @@
       <c r="A185" s="15" t="s">
         <v>83</v>
       </c>
+      <c r="B185" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C185" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D185" s="12">
+        <v>2011</v>
       </c>
       <c r="G185" s="17">
         <f>1-G186</f>
@@ -7636,8 +7654,14 @@
       <c r="A186" s="15" t="s">
         <v>86</v>
       </c>
+      <c r="B186" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C186" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D186" s="12">
+        <v>2011</v>
       </c>
       <c r="G186" s="17">
         <v>0.53177864265468</v>
@@ -7676,8 +7700,14 @@
       <c r="A187" s="15" t="s">
         <v>84</v>
       </c>
+      <c r="B187" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C187" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D187" s="12">
+        <v>2011</v>
       </c>
       <c r="G187" s="17">
         <f>1-G188</f>
@@ -7722,8 +7752,14 @@
       <c r="A188" s="15" t="s">
         <v>87</v>
       </c>
+      <c r="B188" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C188" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D188" s="12">
+        <v>2011</v>
       </c>
       <c r="G188" s="17">
         <v>0.48084216679657066</v>
@@ -7762,8 +7798,14 @@
       <c r="A189" s="15" t="s">
         <v>85</v>
       </c>
+      <c r="B189" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C189" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D189" s="12">
+        <v>2011</v>
       </c>
       <c r="G189" s="17">
         <f>1-G190</f>
@@ -7824,8 +7866,14 @@
       <c r="A190" s="15" t="s">
         <v>88</v>
       </c>
+      <c r="B190" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C190" s="12" t="s">
         <v>77</v>
+      </c>
+      <c r="D190" s="12">
+        <v>2011</v>
       </c>
       <c r="G190" s="17">
         <v>0.26290107655447825</v>

</xml_diff>

<commit_message>
Calculate observed KZN population proportion over time and add this to Excel sheet as a calibration target.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="112">
   <si>
     <t>N</t>
   </si>
@@ -357,6 +357,51 @@
   </si>
   <si>
     <t>Mean type distribution is an average of Bruni, Dartell, and van Aardt (2016) from HPV_parameters Excel document "Plots and final type dist" tab. Number of women who were HPV-positive and had high-grade lesions was 2000 for Bruni (assumed b/c compilation of several studies), 137 for Dartell, and 270 for van Aardt.</t>
+  </si>
+  <si>
+    <t>0-4 years</t>
+  </si>
+  <si>
+    <t>5-9 years</t>
+  </si>
+  <si>
+    <t>10-14 years</t>
+  </si>
+  <si>
+    <t>15-19 years</t>
+  </si>
+  <si>
+    <t>20-24 years</t>
+  </si>
+  <si>
+    <t>25-29 years</t>
+  </si>
+  <si>
+    <t>30-34 years</t>
+  </si>
+  <si>
+    <t>35-39 years</t>
+  </si>
+  <si>
+    <t>40-44 years</t>
+  </si>
+  <si>
+    <t>45-49 years</t>
+  </si>
+  <si>
+    <t>50-54 years</t>
+  </si>
+  <si>
+    <t>55-59 years</t>
+  </si>
+  <si>
+    <t>60-64 years</t>
+  </si>
+  <si>
+    <t>Population age distribution</t>
+  </si>
+  <si>
+    <t>KZN population data from Statistics South Africa. Primary tables Census '96 and 2001 compared. KwaZulu-Natal Table 4.1 and 4.3. South Africa Table 4.1. Statistics South Africa Statistical Release P0301 Community Survey 2016 Table 2.1: Censuss 2011 and Community Survey 2016. Statistics South Africa Statistical Release P0302 2019 Mid-year population estimates Table 6 and Table 11. Assume a normal approximation of the binomial distribution where µ=proportion (p) and variance=(p(1-p))/n.</t>
   </si>
 </sst>
 </file>
@@ -385,6 +430,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -421,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -473,6 +519,8 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,29 +845,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X190"/>
+  <dimension ref="A1:X270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E189" sqref="E189"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B273" sqref="B273"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" customWidth="1"/>
+    <col min="13" max="13" width="61.453125" customWidth="1"/>
     <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -860,7 +909,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -898,7 +947,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -933,7 +982,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -968,7 +1017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1003,7 +1052,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1038,7 +1087,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1073,7 +1122,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1157,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1143,7 +1192,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1228,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1215,7 +1264,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1250,7 +1299,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1285,7 +1334,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1355,7 +1404,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1390,7 +1439,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1425,7 +1474,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1460,7 +1509,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1495,7 +1544,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1531,7 +1580,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1567,7 +1616,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1605,7 +1654,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1640,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1675,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1710,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1745,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1780,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1850,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1885,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1920,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -1955,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -1990,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2025,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2060,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2095,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2130,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2165,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2200,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -2235,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2270,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -2305,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -2340,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
@@ -2375,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -2410,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
@@ -2480,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2515,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2552,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -2589,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>26</v>
       </c>
@@ -2626,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -2670,7 +2719,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>29</v>
       </c>
@@ -2711,7 +2760,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
@@ -2752,7 +2801,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2793,7 +2842,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>34</v>
       </c>
@@ -2834,7 +2883,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
@@ -2875,7 +2924,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -2916,7 +2965,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>34</v>
       </c>
@@ -2957,7 +3006,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>38</v>
       </c>
@@ -2995,7 +3044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>38</v>
       </c>
@@ -3030,7 +3079,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -3065,7 +3114,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
@@ -3100,7 +3149,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>38</v>
       </c>
@@ -3135,7 +3184,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>38</v>
       </c>
@@ -3170,7 +3219,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>38</v>
       </c>
@@ -3205,7 +3254,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>39</v>
       </c>
@@ -3240,7 +3289,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>39</v>
       </c>
@@ -3275,7 +3324,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>39</v>
       </c>
@@ -3310,7 +3359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>39</v>
       </c>
@@ -3347,7 +3396,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>39</v>
       </c>
@@ -3384,7 +3433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>39</v>
       </c>
@@ -3421,7 +3470,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>39</v>
       </c>
@@ -3458,7 +3507,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>40</v>
       </c>
@@ -3495,7 +3544,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>40</v>
       </c>
@@ -3532,7 +3581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>40</v>
       </c>
@@ -3569,7 +3618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>40</v>
       </c>
@@ -3606,7 +3655,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>40</v>
       </c>
@@ -3643,7 +3692,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>40</v>
       </c>
@@ -3680,7 +3729,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>40</v>
       </c>
@@ -3717,7 +3766,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>41</v>
       </c>
@@ -3754,7 +3803,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>41</v>
       </c>
@@ -3791,7 +3840,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>41</v>
       </c>
@@ -3828,7 +3877,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>41</v>
       </c>
@@ -3865,7 +3914,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>41</v>
       </c>
@@ -3902,7 +3951,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>41</v>
       </c>
@@ -3939,7 +3988,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -3976,7 +4025,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>42</v>
       </c>
@@ -4013,7 +4062,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>42</v>
       </c>
@@ -4050,7 +4099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>42</v>
       </c>
@@ -4087,7 +4136,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
@@ -4124,7 +4173,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>42</v>
       </c>
@@ -4161,7 +4210,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>42</v>
       </c>
@@ -4198,7 +4247,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
@@ -4235,7 +4284,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>43</v>
       </c>
@@ -4272,7 +4321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>43</v>
       </c>
@@ -4309,7 +4358,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>43</v>
       </c>
@@ -4346,7 +4395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>43</v>
       </c>
@@ -4383,7 +4432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>43</v>
       </c>
@@ -4420,7 +4469,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>43</v>
       </c>
@@ -4457,7 +4506,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>43</v>
       </c>
@@ -4494,7 +4543,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>44</v>
       </c>
@@ -4531,7 +4580,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>44</v>
       </c>
@@ -4568,7 +4617,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>44</v>
       </c>
@@ -4605,7 +4654,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>44</v>
       </c>
@@ -4642,7 +4691,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>44</v>
       </c>
@@ -4679,7 +4728,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>44</v>
       </c>
@@ -4716,7 +4765,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>44</v>
       </c>
@@ -4753,7 +4802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>45</v>
       </c>
@@ -4790,7 +4839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>45</v>
       </c>
@@ -4827,7 +4876,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>45</v>
       </c>
@@ -4864,7 +4913,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>45</v>
       </c>
@@ -4901,7 +4950,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>45</v>
       </c>
@@ -4938,7 +4987,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>45</v>
       </c>
@@ -4975,7 +5024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>45</v>
       </c>
@@ -5012,7 +5061,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>46</v>
       </c>
@@ -5049,7 +5098,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>46</v>
       </c>
@@ -5086,7 +5135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>46</v>
       </c>
@@ -5123,7 +5172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>46</v>
       </c>
@@ -5160,7 +5209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>46</v>
       </c>
@@ -5197,7 +5246,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>46</v>
       </c>
@@ -5234,7 +5283,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>46</v>
       </c>
@@ -5271,7 +5320,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>47</v>
       </c>
@@ -5308,7 +5357,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>47</v>
       </c>
@@ -5345,7 +5394,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>47</v>
       </c>
@@ -5382,7 +5431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>47</v>
       </c>
@@ -5419,7 +5468,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>47</v>
       </c>
@@ -5456,7 +5505,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>47</v>
       </c>
@@ -5493,7 +5542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>47</v>
       </c>
@@ -5530,7 +5579,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>48</v>
       </c>
@@ -5567,7 +5616,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>48</v>
       </c>
@@ -5604,7 +5653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>48</v>
       </c>
@@ -5641,7 +5690,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>48</v>
       </c>
@@ -5678,7 +5727,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>48</v>
       </c>
@@ -5715,7 +5764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>48</v>
       </c>
@@ -5752,7 +5801,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>48</v>
       </c>
@@ -5789,7 +5838,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>49</v>
       </c>
@@ -5826,7 +5875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>49</v>
       </c>
@@ -5863,7 +5912,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>49</v>
       </c>
@@ -5900,7 +5949,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>49</v>
       </c>
@@ -5937,7 +5986,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>49</v>
       </c>
@@ -5974,7 +6023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>49</v>
       </c>
@@ -6011,7 +6060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>49</v>
       </c>
@@ -6048,7 +6097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>53</v>
       </c>
@@ -6088,7 +6137,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>53</v>
       </c>
@@ -6125,7 +6174,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -6162,7 +6211,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>53</v>
       </c>
@@ -6199,7 +6248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>53</v>
       </c>
@@ -6236,7 +6285,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>53</v>
       </c>
@@ -6273,7 +6322,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>53</v>
       </c>
@@ -6310,7 +6359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>53</v>
       </c>
@@ -6347,7 +6396,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>53</v>
       </c>
@@ -6384,7 +6433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>54</v>
       </c>
@@ -6421,7 +6470,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>54</v>
       </c>
@@ -6458,7 +6507,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>54</v>
       </c>
@@ -6495,7 +6544,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>54</v>
       </c>
@@ -6532,7 +6581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>54</v>
       </c>
@@ -6569,7 +6618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>54</v>
       </c>
@@ -6606,7 +6655,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>54</v>
       </c>
@@ -6643,7 +6692,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>54</v>
       </c>
@@ -6680,7 +6729,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>54</v>
       </c>
@@ -6717,7 +6766,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" ht="145" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>70</v>
       </c>
@@ -6757,7 +6806,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>70</v>
       </c>
@@ -6794,7 +6843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>70</v>
       </c>
@@ -6831,7 +6880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>70</v>
       </c>
@@ -6868,7 +6917,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>70</v>
       </c>
@@ -6905,7 +6954,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>70</v>
       </c>
@@ -6942,7 +6991,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>70</v>
       </c>
@@ -6979,7 +7028,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>70</v>
       </c>
@@ -7016,7 +7065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>70</v>
       </c>
@@ -7053,7 +7102,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>70</v>
       </c>
@@ -7090,7 +7139,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>70</v>
       </c>
@@ -7127,7 +7176,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>70</v>
       </c>
@@ -7164,7 +7213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>70</v>
       </c>
@@ -7201,7 +7250,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A175" s="12" t="s">
         <v>79</v>
       </c>
@@ -7237,7 +7286,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A176" s="12" t="s">
         <v>80</v>
       </c>
@@ -7270,7 +7319,7 @@
       </c>
       <c r="M176" s="8"/>
     </row>
-    <row r="177" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A177" s="12" t="s">
         <v>83</v>
       </c>
@@ -7305,7 +7354,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A178" s="12" t="s">
         <v>86</v>
       </c>
@@ -7338,7 +7387,7 @@
       </c>
       <c r="M178" s="8"/>
     </row>
-    <row r="179" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="12" t="s">
         <v>84</v>
       </c>
@@ -7373,7 +7422,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A180" s="12" t="s">
         <v>87</v>
       </c>
@@ -7406,7 +7455,7 @@
       </c>
       <c r="M180" s="8"/>
     </row>
-    <row r="181" spans="1:24" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="12" t="s">
         <v>85</v>
       </c>
@@ -7441,7 +7490,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="182" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="12" t="s">
         <v>88</v>
       </c>
@@ -7470,7 +7519,7 @@
       </c>
       <c r="M182" s="8"/>
     </row>
-    <row r="183" spans="1:24" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="165.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="15" t="s">
         <v>79</v>
       </c>
@@ -7538,7 +7587,7 @@
         <v>4.874791589632058E-4</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A184" s="15" t="s">
         <v>80</v>
       </c>
@@ -7598,7 +7647,7 @@
         <v>4.8747915896320553E-4</v>
       </c>
     </row>
-    <row r="185" spans="1:24" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" ht="137.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="15" t="s">
         <v>83</v>
       </c>
@@ -7650,7 +7699,7 @@
         <v>2.9502063905325444E-4</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A186" s="15" t="s">
         <v>86</v>
       </c>
@@ -7696,7 +7745,7 @@
         <v>2.9502063905325444E-4</v>
       </c>
     </row>
-    <row r="187" spans="1:24" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" ht="108.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="15" t="s">
         <v>84</v>
       </c>
@@ -7748,7 +7797,7 @@
         <v>3.9463064516129034E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A188" s="15" t="s">
         <v>87</v>
       </c>
@@ -7794,7 +7843,7 @@
         <v>3.9463064516129034E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A189" s="15" t="s">
         <v>85</v>
       </c>
@@ -7862,7 +7911,7 @@
         <v>4.8534811111111112E-4</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A190" s="15" t="s">
         <v>88</v>
       </c>
@@ -7920,6 +7969,2744 @@
       <c r="X190">
         <f>(S190*(1-S190))/270</f>
         <v>4.8534811111111112E-4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+      <c r="A191" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C191" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D191" s="12">
+        <v>1996</v>
+      </c>
+      <c r="E191">
+        <v>964546</v>
+      </c>
+      <c r="F191">
+        <v>8244075</v>
+      </c>
+      <c r="G191">
+        <v>0.11699869300073083</v>
+      </c>
+      <c r="H191" s="30">
+        <f>G191</f>
+        <v>0.11699869300073083</v>
+      </c>
+      <c r="I191">
+        <f>(H191*(1-H191))/F191</f>
+        <v>1.253142394226782E-8</v>
+      </c>
+      <c r="L191" t="s">
+        <v>58</v>
+      </c>
+      <c r="M191" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A192" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C192" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D192">
+        <f>D191</f>
+        <v>1996</v>
+      </c>
+      <c r="E192">
+        <v>1005944</v>
+      </c>
+      <c r="F192">
+        <v>8244075</v>
+      </c>
+      <c r="G192">
+        <v>0.12202023877754629</v>
+      </c>
+      <c r="H192" s="30">
+        <f t="shared" ref="H192:H255" si="6">G192</f>
+        <v>0.12202023877754629</v>
+      </c>
+      <c r="I192">
+        <f t="shared" ref="I192:I255" si="7">(H192*(1-H192))/F192</f>
+        <v>1.2994944867218806E-8</v>
+      </c>
+      <c r="L192" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A193" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C193" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D193">
+        <f t="shared" ref="D193:D206" si="8">D192</f>
+        <v>1996</v>
+      </c>
+      <c r="E193">
+        <v>1018218</v>
+      </c>
+      <c r="F193">
+        <v>8244075</v>
+      </c>
+      <c r="G193">
+        <v>0.12350906560165938</v>
+      </c>
+      <c r="H193" s="30">
+        <f t="shared" si="6"/>
+        <v>0.12350906560165938</v>
+      </c>
+      <c r="I193">
+        <f t="shared" si="7"/>
+        <v>1.3131197413398637E-8</v>
+      </c>
+      <c r="L193" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A194" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C194" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D194">
+        <f>D193</f>
+        <v>1996</v>
+      </c>
+      <c r="E194">
+        <v>914305</v>
+      </c>
+      <c r="F194">
+        <v>8244075</v>
+      </c>
+      <c r="G194">
+        <v>0.11090449807892334</v>
+      </c>
+      <c r="H194" s="30">
+        <f t="shared" si="6"/>
+        <v>0.11090449807892334</v>
+      </c>
+      <c r="I194">
+        <f t="shared" si="7"/>
+        <v>1.1960673621332343E-8</v>
+      </c>
+      <c r="L194" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A195" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C195" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E195">
+        <v>851953</v>
+      </c>
+      <c r="F195">
+        <v>8244075</v>
+      </c>
+      <c r="G195">
+        <v>0.10334124810849003</v>
+      </c>
+      <c r="H195" s="30">
+        <f t="shared" si="6"/>
+        <v>0.10334124810849003</v>
+      </c>
+      <c r="I195">
+        <f t="shared" si="7"/>
+        <v>1.1239809747954688E-8</v>
+      </c>
+      <c r="L195" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A196" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C196" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D196">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E196">
+        <v>684675</v>
+      </c>
+      <c r="F196">
+        <v>8244075</v>
+      </c>
+      <c r="G196">
+        <v>8.3050554489133108E-2</v>
+      </c>
+      <c r="H196" s="30">
+        <f t="shared" si="6"/>
+        <v>8.3050554489133108E-2</v>
+      </c>
+      <c r="I196">
+        <f t="shared" si="7"/>
+        <v>9.2373201224128406E-9</v>
+      </c>
+      <c r="L196" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A197" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C197" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D197">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E197">
+        <v>590583</v>
+      </c>
+      <c r="F197">
+        <v>8244075</v>
+      </c>
+      <c r="G197">
+        <v>7.1637266764312549E-2</v>
+      </c>
+      <c r="H197" s="30">
+        <f t="shared" si="6"/>
+        <v>7.1637266764312549E-2</v>
+      </c>
+      <c r="I197">
+        <f t="shared" si="7"/>
+        <v>8.0670504301393744E-9</v>
+      </c>
+      <c r="L197" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A198" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C198" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D198">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E198">
+        <v>504746</v>
+      </c>
+      <c r="F198">
+        <v>8244075</v>
+      </c>
+      <c r="G198">
+        <v>6.1225304233646589E-2</v>
+      </c>
+      <c r="H198" s="30">
+        <f t="shared" si="6"/>
+        <v>6.1225304233646589E-2</v>
+      </c>
+      <c r="I198">
+        <f t="shared" si="7"/>
+        <v>6.9718878534152113E-9</v>
+      </c>
+      <c r="L198" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A199" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C199" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D199">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E199">
+        <v>408926</v>
+      </c>
+      <c r="F199">
+        <v>8244075</v>
+      </c>
+      <c r="G199">
+        <v>4.9602411428814025E-2</v>
+      </c>
+      <c r="H199" s="30">
+        <f t="shared" si="6"/>
+        <v>4.9602411428814025E-2</v>
+      </c>
+      <c r="I199">
+        <f t="shared" si="7"/>
+        <v>5.7182900700516043E-9</v>
+      </c>
+      <c r="L199" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A200" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C200" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D200">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E200">
+        <v>337933</v>
+      </c>
+      <c r="F200">
+        <v>8244075</v>
+      </c>
+      <c r="G200">
+        <v>4.0991014759084551E-2</v>
+      </c>
+      <c r="H200" s="30">
+        <f t="shared" si="6"/>
+        <v>4.0991014759084551E-2</v>
+      </c>
+      <c r="I200">
+        <f t="shared" si="7"/>
+        <v>4.7683641243080716E-9</v>
+      </c>
+      <c r="L200" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A201" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C201" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D201">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E201">
+        <v>248877</v>
+      </c>
+      <c r="F201">
+        <v>8244075</v>
+      </c>
+      <c r="G201">
+        <v>3.0188589987354554E-2</v>
+      </c>
+      <c r="H201" s="30">
+        <f t="shared" si="6"/>
+        <v>3.0188589987354554E-2</v>
+      </c>
+      <c r="I201">
+        <f t="shared" si="7"/>
+        <v>3.551306729005977E-9</v>
+      </c>
+      <c r="L201" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A202" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C202" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D202">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E202">
+        <v>212751</v>
+      </c>
+      <c r="F202">
+        <v>8244075</v>
+      </c>
+      <c r="G202">
+        <v>2.58065337833535E-2</v>
+      </c>
+      <c r="H202" s="30">
+        <f t="shared" si="6"/>
+        <v>2.58065337833535E-2</v>
+      </c>
+      <c r="I202">
+        <f t="shared" si="7"/>
+        <v>3.0495303108525985E-9</v>
+      </c>
+      <c r="L202" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A203" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C203" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D203">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E203">
+        <v>178471</v>
+      </c>
+      <c r="F203">
+        <v>8244075</v>
+      </c>
+      <c r="G203">
+        <v>2.1648395969226384E-2</v>
+      </c>
+      <c r="H203" s="30">
+        <f t="shared" si="6"/>
+        <v>2.1648395969226384E-2</v>
+      </c>
+      <c r="I203">
+        <f t="shared" si="7"/>
+        <v>2.5690866375167577E-9</v>
+      </c>
+      <c r="L203" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A204" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C204" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D204">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E204">
+        <v>158208</v>
+      </c>
+      <c r="F204">
+        <v>8244075</v>
+      </c>
+      <c r="G204">
+        <v>1.9190509547766122E-2</v>
+      </c>
+      <c r="H204" s="30">
+        <f t="shared" si="6"/>
+        <v>1.9190509547766122E-2</v>
+      </c>
+      <c r="I204">
+        <f t="shared" si="7"/>
+        <v>2.2831225930214389E-9</v>
+      </c>
+      <c r="L204" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A205" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C205" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D205">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E205">
+        <v>95372</v>
+      </c>
+      <c r="F205">
+        <v>8244075</v>
+      </c>
+      <c r="G205">
+        <v>1.1568550747051671E-2</v>
+      </c>
+      <c r="H205" s="30">
+        <f t="shared" si="6"/>
+        <v>1.1568550747051671E-2</v>
+      </c>
+      <c r="I205">
+        <f t="shared" si="7"/>
+        <v>1.3870227260989937E-9</v>
+      </c>
+      <c r="L205" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A206" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C206" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D206">
+        <f t="shared" si="8"/>
+        <v>1996</v>
+      </c>
+      <c r="E206">
+        <v>68567</v>
+      </c>
+      <c r="F206">
+        <v>8244075</v>
+      </c>
+      <c r="G206">
+        <v>8.3171247229070575E-3</v>
+      </c>
+      <c r="H206" s="30">
+        <f t="shared" si="6"/>
+        <v>8.3171247229070575E-3</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="7"/>
+        <v>1.0004700538569418E-9</v>
+      </c>
+      <c r="L206" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A207" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C207" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D207">
+        <v>2001</v>
+      </c>
+      <c r="E207">
+        <v>1012649</v>
+      </c>
+      <c r="F207" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G207">
+        <v>0.10832581493420429</v>
+      </c>
+      <c r="H207" s="30">
+        <f t="shared" si="6"/>
+        <v>0.10832581493420429</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="7"/>
+        <v>1.0332637306761254E-8</v>
+      </c>
+      <c r="L207" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A208" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C208" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D208">
+        <v>2001</v>
+      </c>
+      <c r="E208">
+        <v>1117011</v>
+      </c>
+      <c r="F208" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G208">
+        <v>0.11948970162955819</v>
+      </c>
+      <c r="H208" s="30">
+        <f t="shared" si="6"/>
+        <v>0.11948970162955819</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="7"/>
+        <v>1.1254804180454987E-8</v>
+      </c>
+      <c r="L208" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A209" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C209" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D209">
+        <v>2001</v>
+      </c>
+      <c r="E209">
+        <v>1141322</v>
+      </c>
+      <c r="F209" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G209">
+        <v>0.12209031535343037</v>
+      </c>
+      <c r="H209" s="30">
+        <f t="shared" si="6"/>
+        <v>0.12209031535343037</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="7"/>
+        <v>1.1465792612242759E-8</v>
+      </c>
+      <c r="L209" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A210" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C210" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D210">
+        <v>2001</v>
+      </c>
+      <c r="E210">
+        <v>1126495</v>
+      </c>
+      <c r="F210" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G210">
+        <v>0.12050423087793151</v>
+      </c>
+      <c r="H210" s="30">
+        <f t="shared" si="6"/>
+        <v>0.12050423087793151</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="7"/>
+        <v>1.1337285321102111E-8</v>
+      </c>
+      <c r="L210" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A211" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C211" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D211">
+        <v>2001</v>
+      </c>
+      <c r="E211">
+        <v>905222</v>
+      </c>
+      <c r="F211" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G211">
+        <v>9.6834056861133791E-2</v>
+      </c>
+      <c r="H211" s="30">
+        <f t="shared" si="6"/>
+        <v>9.6834056861133791E-2</v>
+      </c>
+      <c r="I211">
+        <f t="shared" si="7"/>
+        <v>9.3555366931340526E-9</v>
+      </c>
+      <c r="L211" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A212" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C212" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D212">
+        <v>2001</v>
+      </c>
+      <c r="E212">
+        <v>790823</v>
+      </c>
+      <c r="F212" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G212">
+        <v>8.4596485004885438E-2</v>
+      </c>
+      <c r="H212" s="30">
+        <f t="shared" si="6"/>
+        <v>8.4596485004885438E-2</v>
+      </c>
+      <c r="I212">
+        <f t="shared" si="7"/>
+        <v>8.2839586205679468E-9</v>
+      </c>
+      <c r="L212" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A213" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C213" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D213">
+        <v>2001</v>
+      </c>
+      <c r="E213">
+        <v>633129</v>
+      </c>
+      <c r="F213" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G213">
+        <v>6.7727529364545694E-2</v>
+      </c>
+      <c r="H213" s="30">
+        <f t="shared" si="6"/>
+        <v>6.7727529364545694E-2</v>
+      </c>
+      <c r="I213">
+        <f t="shared" si="7"/>
+        <v>6.7543120307208839E-9</v>
+      </c>
+      <c r="L213" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A214" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C214" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D214">
+        <v>2001</v>
+      </c>
+      <c r="E214">
+        <v>585772</v>
+      </c>
+      <c r="F214" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G214">
+        <v>6.2661622403852382E-2</v>
+      </c>
+      <c r="H214" s="30">
+        <f t="shared" si="6"/>
+        <v>6.2661622403852382E-2</v>
+      </c>
+      <c r="I214">
+        <f t="shared" si="7"/>
+        <v>6.2830578837469086E-9</v>
+      </c>
+      <c r="L214" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A215" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C215" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D215">
+        <v>2001</v>
+      </c>
+      <c r="E215">
+        <v>491309</v>
+      </c>
+      <c r="F215" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G215">
+        <v>5.2556658634441922E-2</v>
+      </c>
+      <c r="H215" s="30">
+        <f t="shared" si="6"/>
+        <v>5.2556658634441922E-2</v>
+      </c>
+      <c r="I215">
+        <f t="shared" si="7"/>
+        <v>5.3266482802985421E-9</v>
+      </c>
+      <c r="L215" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A216" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C216" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D216">
+        <v>2001</v>
+      </c>
+      <c r="E216">
+        <v>396021</v>
+      </c>
+      <c r="F216" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G216">
+        <v>4.2363442373476418E-2</v>
+      </c>
+      <c r="H216" s="30">
+        <f t="shared" si="6"/>
+        <v>4.2363442373476418E-2</v>
+      </c>
+      <c r="I216">
+        <f t="shared" si="7"/>
+        <v>4.3397527436625145E-9</v>
+      </c>
+      <c r="L216" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A217" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C217" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D217">
+        <v>2001</v>
+      </c>
+      <c r="E217">
+        <v>332888</v>
+      </c>
+      <c r="F217" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G217">
+        <v>3.5609933828816692E-2</v>
+      </c>
+      <c r="H217" s="30">
+        <f t="shared" si="6"/>
+        <v>3.5609933828816692E-2</v>
+      </c>
+      <c r="I217">
+        <f t="shared" si="7"/>
+        <v>3.6736427613513551E-9</v>
+      </c>
+      <c r="L217" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A218" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C218" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D218">
+        <v>2001</v>
+      </c>
+      <c r="E218">
+        <v>240916</v>
+      </c>
+      <c r="F218" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G218">
+        <v>2.5771439097543928E-2</v>
+      </c>
+      <c r="H218" s="30">
+        <f t="shared" si="6"/>
+        <v>2.5771439097543928E-2</v>
+      </c>
+      <c r="I218">
+        <f t="shared" si="7"/>
+        <v>2.6857931058207825E-9</v>
+      </c>
+      <c r="L218" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A219" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C219" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D219">
+        <v>2001</v>
+      </c>
+      <c r="E219">
+        <v>215539</v>
+      </c>
+      <c r="F219" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G219">
+        <v>2.3056792457310932E-2</v>
+      </c>
+      <c r="H219" s="30">
+        <f t="shared" si="6"/>
+        <v>2.3056792457310932E-2</v>
+      </c>
+      <c r="I219">
+        <f t="shared" si="7"/>
+        <v>2.4095793617634816E-9</v>
+      </c>
+      <c r="L219" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A220" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C220" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D220">
+        <v>2001</v>
+      </c>
+      <c r="E220">
+        <v>154802</v>
+      </c>
+      <c r="F220" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G220">
+        <v>1.6559590542670453E-2</v>
+      </c>
+      <c r="H220" s="30">
+        <f t="shared" si="6"/>
+        <v>1.6559590542670453E-2</v>
+      </c>
+      <c r="I220">
+        <f t="shared" si="7"/>
+        <v>1.7420903307285709E-9</v>
+      </c>
+      <c r="L220" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A221" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C221" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D221">
+        <v>2001</v>
+      </c>
+      <c r="E221">
+        <v>131779</v>
+      </c>
+      <c r="F221" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G221">
+        <v>1.4096757678341169E-2</v>
+      </c>
+      <c r="H221" s="30">
+        <f t="shared" si="6"/>
+        <v>1.4096757678341169E-2</v>
+      </c>
+      <c r="I221">
+        <f t="shared" si="7"/>
+        <v>1.486711004144262E-9</v>
+      </c>
+      <c r="L221" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A222" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C222" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D222">
+        <v>2001</v>
+      </c>
+      <c r="E222">
+        <v>72501</v>
+      </c>
+      <c r="F222" s="12">
+        <v>9348178</v>
+      </c>
+      <c r="G222">
+        <v>7.7556289578568144E-3</v>
+      </c>
+      <c r="H222" s="30">
+        <f t="shared" si="6"/>
+        <v>7.7556289578568144E-3</v>
+      </c>
+      <c r="I222">
+        <f t="shared" si="7"/>
+        <v>8.2320631649556376E-10</v>
+      </c>
+      <c r="L222" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A223" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C223" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D223">
+        <v>2011</v>
+      </c>
+      <c r="E223">
+        <v>1198134</v>
+      </c>
+      <c r="F223" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G223">
+        <v>0.11793677819173529</v>
+      </c>
+      <c r="H223" s="30">
+        <f t="shared" si="6"/>
+        <v>0.11793677819173529</v>
+      </c>
+      <c r="I223">
+        <f t="shared" si="7"/>
+        <v>1.0239832219882873E-8</v>
+      </c>
+      <c r="L223" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A224" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C224" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D224">
+        <v>2011</v>
+      </c>
+      <c r="E224">
+        <v>1042528</v>
+      </c>
+      <c r="F224" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G224">
+        <v>0.10261990185961954</v>
+      </c>
+      <c r="H224" s="30">
+        <f t="shared" si="6"/>
+        <v>0.10261990185961954</v>
+      </c>
+      <c r="I224">
+        <f t="shared" si="7"/>
+        <v>9.0646678587588034E-9</v>
+      </c>
+      <c r="L224" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A225" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C225" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D225">
+        <v>2011</v>
+      </c>
+      <c r="E225">
+        <v>1038857</v>
+      </c>
+      <c r="F225" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G225">
+        <v>0.10225855169950235</v>
+      </c>
+      <c r="H225" s="30">
+        <f t="shared" si="6"/>
+        <v>0.10225855169950235</v>
+      </c>
+      <c r="I225">
+        <f t="shared" si="7"/>
+        <v>9.0363861503197521E-9</v>
+      </c>
+      <c r="L225" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A226" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C226" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D226">
+        <v>2011</v>
+      </c>
+      <c r="E226">
+        <v>1119535</v>
+      </c>
+      <c r="F226" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G226">
+        <v>0.11019998679019573</v>
+      </c>
+      <c r="H226" s="30">
+        <f t="shared" si="6"/>
+        <v>0.11019998679019573</v>
+      </c>
+      <c r="I226">
+        <f t="shared" si="7"/>
+        <v>9.6520112027050787E-9</v>
+      </c>
+      <c r="L226" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A227" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C227" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D227">
+        <v>2011</v>
+      </c>
+      <c r="E227">
+        <v>1102388</v>
+      </c>
+      <c r="F227" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G227">
+        <v>0.10851214391481311</v>
+      </c>
+      <c r="H227" s="30">
+        <f t="shared" si="6"/>
+        <v>0.10851214391481311</v>
+      </c>
+      <c r="I227">
+        <f t="shared" si="7"/>
+        <v>9.5222075352605795E-9</v>
+      </c>
+      <c r="L227" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A228" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C228" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D228">
+        <v>2011</v>
+      </c>
+      <c r="E228">
+        <v>980929</v>
+      </c>
+      <c r="F228" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G228">
+        <v>9.655648357766386E-2</v>
+      </c>
+      <c r="H228" s="30">
+        <f t="shared" si="6"/>
+        <v>9.655648357766386E-2</v>
+      </c>
+      <c r="I228">
+        <f t="shared" si="7"/>
+        <v>8.5867004691429685E-9</v>
+      </c>
+      <c r="L228" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A229" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C229" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D229">
+        <v>2011</v>
+      </c>
+      <c r="E229">
+        <v>729230</v>
+      </c>
+      <c r="F229" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G229">
+        <v>7.1780816470243827E-2</v>
+      </c>
+      <c r="H229" s="30">
+        <f t="shared" si="6"/>
+        <v>7.1780816470243827E-2</v>
+      </c>
+      <c r="I229">
+        <f t="shared" si="7"/>
+        <v>6.5584739917074511E-9</v>
+      </c>
+      <c r="L229" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A230" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C230" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D230">
+        <v>2011</v>
+      </c>
+      <c r="E230">
+        <v>612615</v>
+      </c>
+      <c r="F230" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G230">
+        <v>6.030196903846307E-2</v>
+      </c>
+      <c r="H230" s="30">
+        <f t="shared" si="6"/>
+        <v>6.030196903846307E-2</v>
+      </c>
+      <c r="I230">
+        <f t="shared" si="7"/>
+        <v>5.5778094943989062E-9</v>
+      </c>
+      <c r="L230" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A231" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C231" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D231">
+        <v>2011</v>
+      </c>
+      <c r="E231">
+        <v>499102</v>
+      </c>
+      <c r="F231" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G231">
+        <v>4.9128462984149905E-2</v>
+      </c>
+      <c r="H231" s="30">
+        <f t="shared" si="6"/>
+        <v>4.9128462984149905E-2</v>
+      </c>
+      <c r="I231">
+        <f t="shared" si="7"/>
+        <v>4.5983168336084311E-9</v>
+      </c>
+      <c r="L231" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A232" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C232" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D232">
+        <v>2011</v>
+      </c>
+      <c r="E232">
+        <v>454637</v>
+      </c>
+      <c r="F232" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G232">
+        <v>4.4751607939308921E-2</v>
+      </c>
+      <c r="H232" s="30">
+        <f t="shared" si="6"/>
+        <v>4.4751607939308921E-2</v>
+      </c>
+      <c r="I232">
+        <f t="shared" si="7"/>
+        <v>4.2079331003297735E-9</v>
+      </c>
+      <c r="L232" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A233" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C233" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D233">
+        <v>2011</v>
+      </c>
+      <c r="E233">
+        <v>384397</v>
+      </c>
+      <c r="F233" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G233">
+        <v>3.7837623944040041E-2</v>
+      </c>
+      <c r="H233" s="30">
+        <f t="shared" si="6"/>
+        <v>3.7837623944040041E-2</v>
+      </c>
+      <c r="I233">
+        <f t="shared" si="7"/>
+        <v>3.5835716651381008E-9</v>
+      </c>
+      <c r="L233" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A234" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C234" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D234">
+        <v>2011</v>
+      </c>
+      <c r="E234">
+        <v>325571</v>
+      </c>
+      <c r="F234" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G234">
+        <v>3.2047162348002353E-2</v>
+      </c>
+      <c r="H234" s="30">
+        <f t="shared" si="6"/>
+        <v>3.2047162348002353E-2</v>
+      </c>
+      <c r="I234">
+        <f t="shared" si="7"/>
+        <v>3.0534277260250306E-9</v>
+      </c>
+      <c r="L234" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A235" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C235" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D235">
+        <v>2011</v>
+      </c>
+      <c r="E235">
+        <v>271326</v>
+      </c>
+      <c r="F235" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G235">
+        <v>2.6707625590836056E-2</v>
+      </c>
+      <c r="H235" s="30">
+        <f t="shared" si="6"/>
+        <v>2.6707625590836056E-2</v>
+      </c>
+      <c r="I235">
+        <f t="shared" si="7"/>
+        <v>2.5587182519172453E-9</v>
+      </c>
+      <c r="L235" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A236" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C236" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D236">
+        <v>2011</v>
+      </c>
+      <c r="E236">
+        <v>175673</v>
+      </c>
+      <c r="F236" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G236">
+        <v>1.7292145649215124E-2</v>
+      </c>
+      <c r="H236" s="30">
+        <f t="shared" si="6"/>
+        <v>1.7292145649215124E-2</v>
+      </c>
+      <c r="I236">
+        <f t="shared" si="7"/>
+        <v>1.6726966189359743E-9</v>
+      </c>
+      <c r="L236" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A237" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C237" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D237">
+        <v>2011</v>
+      </c>
+      <c r="E237">
+        <v>137821</v>
+      </c>
+      <c r="F237" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G237">
+        <v>1.3566232747892263E-2</v>
+      </c>
+      <c r="H237" s="30">
+        <f t="shared" si="6"/>
+        <v>1.3566232747892263E-2</v>
+      </c>
+      <c r="I237">
+        <f t="shared" si="7"/>
+        <v>1.317258656228455E-9</v>
+      </c>
+      <c r="L237" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A238" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C238" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D238">
+        <v>2011</v>
+      </c>
+      <c r="E238">
+        <v>86378</v>
+      </c>
+      <c r="F238" s="12">
+        <v>10159121</v>
+      </c>
+      <c r="G238">
+        <v>8.502507254318557E-3</v>
+      </c>
+      <c r="H238" s="30">
+        <f t="shared" si="6"/>
+        <v>8.502507254318557E-3</v>
+      </c>
+      <c r="I238">
+        <f t="shared" si="7"/>
+        <v>8.2981732619473843E-10</v>
+      </c>
+      <c r="L238" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A239" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C239" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D239">
+        <v>2016</v>
+      </c>
+      <c r="E239">
+        <v>1343532</v>
+      </c>
+      <c r="F239">
+        <v>10987234</v>
+      </c>
+      <c r="G239">
+        <v>0.12228118560139886</v>
+      </c>
+      <c r="H239" s="30">
+        <f t="shared" si="6"/>
+        <v>0.12228118560139886</v>
+      </c>
+      <c r="I239">
+        <f t="shared" si="7"/>
+        <v>9.7684728703616492E-9</v>
+      </c>
+      <c r="L239" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A240" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C240" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D240">
+        <v>2016</v>
+      </c>
+      <c r="E240">
+        <v>1291700</v>
+      </c>
+      <c r="F240">
+        <v>10987234</v>
+      </c>
+      <c r="G240">
+        <v>0.11756371075741173</v>
+      </c>
+      <c r="H240" s="30">
+        <f t="shared" si="6"/>
+        <v>0.11756371075741173</v>
+      </c>
+      <c r="I240">
+        <f t="shared" si="7"/>
+        <v>9.4420929480849662E-9</v>
+      </c>
+      <c r="L240" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A241" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C241" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D241">
+        <v>2016</v>
+      </c>
+      <c r="E241">
+        <v>1213716</v>
+      </c>
+      <c r="F241">
+        <v>10987234</v>
+      </c>
+      <c r="G241">
+        <v>0.11046601901807133</v>
+      </c>
+      <c r="H241" s="30">
+        <f t="shared" si="6"/>
+        <v>0.11046601901807133</v>
+      </c>
+      <c r="I241">
+        <f t="shared" si="7"/>
+        <v>8.9434044692568144E-9</v>
+      </c>
+      <c r="L241" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A242" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C242" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D242">
+        <v>2016</v>
+      </c>
+      <c r="E242">
+        <v>1079257</v>
+      </c>
+      <c r="F242">
+        <v>10987234</v>
+      </c>
+      <c r="G242">
+        <v>9.8228271100806633E-2</v>
+      </c>
+      <c r="H242" s="30">
+        <f t="shared" si="6"/>
+        <v>9.8228271100806633E-2</v>
+      </c>
+      <c r="I242">
+        <f t="shared" si="7"/>
+        <v>8.0620361646391683E-9</v>
+      </c>
+      <c r="L242" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A243" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C243" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D243">
+        <v>2016</v>
+      </c>
+      <c r="E243">
+        <v>1071893</v>
+      </c>
+      <c r="F243">
+        <v>10987234</v>
+      </c>
+      <c r="G243">
+        <v>9.7558038720209295E-2</v>
+      </c>
+      <c r="H243" s="30">
+        <f t="shared" si="6"/>
+        <v>9.7558038720209295E-2</v>
+      </c>
+      <c r="I243">
+        <f t="shared" si="7"/>
+        <v>8.0129783165877258E-9</v>
+      </c>
+      <c r="L243" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A244" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C244" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D244">
+        <v>2016</v>
+      </c>
+      <c r="E244">
+        <v>1044784</v>
+      </c>
+      <c r="F244">
+        <v>10987234</v>
+      </c>
+      <c r="G244">
+        <v>9.5090720740087994E-2</v>
+      </c>
+      <c r="H244" s="30">
+        <f t="shared" si="6"/>
+        <v>9.5090720740087994E-2</v>
+      </c>
+      <c r="I244">
+        <f t="shared" si="7"/>
+        <v>7.831677706074032E-9</v>
+      </c>
+      <c r="L244" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A245" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C245" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D245">
+        <v>2016</v>
+      </c>
+      <c r="E245">
+        <v>853251</v>
+      </c>
+      <c r="F245">
+        <v>10987234</v>
+      </c>
+      <c r="G245">
+        <v>7.7658398829041048E-2</v>
+      </c>
+      <c r="H245" s="30">
+        <f t="shared" si="6"/>
+        <v>7.7658398829041048E-2</v>
+      </c>
+      <c r="I245">
+        <f t="shared" si="7"/>
+        <v>6.5191632325615928E-9</v>
+      </c>
+      <c r="L245" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A246" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C246" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D246">
+        <v>2016</v>
+      </c>
+      <c r="E246">
+        <v>665736</v>
+      </c>
+      <c r="F246">
+        <v>10987234</v>
+      </c>
+      <c r="G246">
+        <v>6.0591774053415079E-2</v>
+      </c>
+      <c r="H246" s="30">
+        <f t="shared" si="6"/>
+        <v>6.0591774053415079E-2</v>
+      </c>
+      <c r="I246">
+        <f t="shared" si="7"/>
+        <v>5.1805951316295778E-9</v>
+      </c>
+      <c r="L246" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A247" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C247" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D247">
+        <v>2016</v>
+      </c>
+      <c r="E247">
+        <v>538152</v>
+      </c>
+      <c r="F247">
+        <v>10987234</v>
+      </c>
+      <c r="G247">
+        <v>4.897975231982863E-2</v>
+      </c>
+      <c r="H247" s="30">
+        <f t="shared" si="6"/>
+        <v>4.897975231982863E-2</v>
+      </c>
+      <c r="I247">
+        <f t="shared" si="7"/>
+        <v>4.2395325504596404E-9</v>
+      </c>
+      <c r="L247" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A248" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C248" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D248">
+        <v>2016</v>
+      </c>
+      <c r="E248">
+        <v>446144</v>
+      </c>
+      <c r="F248">
+        <v>10987234</v>
+      </c>
+      <c r="G248">
+        <v>4.0605670180502207E-2</v>
+      </c>
+      <c r="H248" s="30">
+        <f t="shared" si="6"/>
+        <v>4.0605670180502207E-2</v>
+      </c>
+      <c r="I248">
+        <f t="shared" si="7"/>
+        <v>3.5456466777438688E-9</v>
+      </c>
+      <c r="L248" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A249" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C249" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D249">
+        <v>2016</v>
+      </c>
+      <c r="E249">
+        <v>383581</v>
+      </c>
+      <c r="F249">
+        <v>10987234</v>
+      </c>
+      <c r="G249">
+        <v>3.4911516401671248E-2</v>
+      </c>
+      <c r="H249" s="30">
+        <f t="shared" si="6"/>
+        <v>3.4911516401671248E-2</v>
+      </c>
+      <c r="I249">
+        <f t="shared" si="7"/>
+        <v>3.0665317971936424E-9</v>
+      </c>
+      <c r="L249" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A250" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C250" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D250">
+        <v>2016</v>
+      </c>
+      <c r="E250">
+        <v>327522</v>
+      </c>
+      <c r="F250">
+        <v>10987234</v>
+      </c>
+      <c r="G250">
+        <v>2.9809322346279327E-2</v>
+      </c>
+      <c r="H250" s="30">
+        <f t="shared" si="6"/>
+        <v>2.9809322346279327E-2</v>
+      </c>
+      <c r="I250">
+        <f t="shared" si="7"/>
+        <v>2.6322117693620562E-9</v>
+      </c>
+      <c r="L250" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A251" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C251" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D251">
+        <v>2016</v>
+      </c>
+      <c r="E251">
+        <v>278361</v>
+      </c>
+      <c r="F251">
+        <v>10987234</v>
+      </c>
+      <c r="G251">
+        <v>2.5334947813071062E-2</v>
+      </c>
+      <c r="H251" s="30">
+        <f t="shared" si="6"/>
+        <v>2.5334947813071062E-2</v>
+      </c>
+      <c r="I251">
+        <f t="shared" si="7"/>
+        <v>2.2474344527822039E-9</v>
+      </c>
+      <c r="L251" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A252" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C252" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D252">
+        <v>2016</v>
+      </c>
+      <c r="E252">
+        <v>220261</v>
+      </c>
+      <c r="F252">
+        <v>10987234</v>
+      </c>
+      <c r="G252">
+        <v>2.0046992719004619E-2</v>
+      </c>
+      <c r="H252" s="30">
+        <f t="shared" si="6"/>
+        <v>2.0046992719004619E-2</v>
+      </c>
+      <c r="I252">
+        <f t="shared" si="7"/>
+        <v>1.7879942123676255E-9</v>
+      </c>
+      <c r="L252" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A253" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C253" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D253">
+        <v>2016</v>
+      </c>
+      <c r="E253">
+        <v>144852</v>
+      </c>
+      <c r="F253">
+        <v>10987234</v>
+      </c>
+      <c r="G253">
+        <v>1.3183663877550983E-2</v>
+      </c>
+      <c r="H253" s="30">
+        <f t="shared" si="6"/>
+        <v>1.3183663877550983E-2</v>
+      </c>
+      <c r="I253">
+        <f t="shared" si="7"/>
+        <v>1.1840882686502118E-9</v>
+      </c>
+      <c r="L253" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A254" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C254" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D254">
+        <v>2016</v>
+      </c>
+      <c r="E254">
+        <v>84492</v>
+      </c>
+      <c r="F254">
+        <v>10987234</v>
+      </c>
+      <c r="G254">
+        <v>7.6900155216499443E-3</v>
+      </c>
+      <c r="H254" s="30">
+        <f t="shared" si="6"/>
+        <v>7.6900155216499443E-3</v>
+      </c>
+      <c r="I254">
+        <f t="shared" si="7"/>
+        <v>6.9452231407165145E-10</v>
+      </c>
+      <c r="L254" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A255" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C255" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D255">
+        <v>2019</v>
+      </c>
+      <c r="E255">
+        <v>1231101</v>
+      </c>
+      <c r="F255">
+        <v>11192662</v>
+      </c>
+      <c r="G255">
+        <v>0.1099917964108985</v>
+      </c>
+      <c r="H255" s="30">
+        <f t="shared" si="6"/>
+        <v>0.1099917964108985</v>
+      </c>
+      <c r="I255">
+        <f t="shared" si="7"/>
+        <v>8.746230443946397E-9</v>
+      </c>
+      <c r="L255" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A256" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C256" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D256">
+        <v>2019</v>
+      </c>
+      <c r="E256">
+        <v>1196909</v>
+      </c>
+      <c r="F256">
+        <v>11192662</v>
+      </c>
+      <c r="G256">
+        <v>0.10693693779013429</v>
+      </c>
+      <c r="H256" s="30">
+        <f t="shared" ref="H256:H270" si="9">G256</f>
+        <v>0.10693693779013429</v>
+      </c>
+      <c r="I256">
+        <f t="shared" ref="I256:I270" si="10">(H256*(1-H256))/F256</f>
+        <v>8.5325036283775244E-9</v>
+      </c>
+      <c r="L256" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A257" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C257" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D257">
+        <v>2019</v>
+      </c>
+      <c r="E257">
+        <v>1136163</v>
+      </c>
+      <c r="F257">
+        <v>11192662</v>
+      </c>
+      <c r="G257">
+        <v>0.10150963193563783</v>
+      </c>
+      <c r="H257" s="30">
+        <f t="shared" si="9"/>
+        <v>0.10150963193563783</v>
+      </c>
+      <c r="I257">
+        <f t="shared" si="10"/>
+        <v>8.1486804979842301E-9</v>
+      </c>
+      <c r="L257" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A258" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C258" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D258">
+        <v>2019</v>
+      </c>
+      <c r="E258">
+        <v>980573</v>
+      </c>
+      <c r="F258">
+        <v>11192662</v>
+      </c>
+      <c r="G258">
+        <v>8.7608559965448793E-2</v>
+      </c>
+      <c r="H258" s="30">
+        <f t="shared" si="9"/>
+        <v>8.7608559965448793E-2</v>
+      </c>
+      <c r="I258">
+        <f t="shared" si="10"/>
+        <v>7.1415808130567291E-9</v>
+      </c>
+      <c r="L258" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A259" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C259" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D259">
+        <v>2019</v>
+      </c>
+      <c r="E259">
+        <v>1006031</v>
+      </c>
+      <c r="F259">
+        <v>11192662</v>
+      </c>
+      <c r="G259">
+        <v>8.9883085900387238E-2</v>
+      </c>
+      <c r="H259" s="30">
+        <f t="shared" si="9"/>
+        <v>8.9883085900387238E-2</v>
+      </c>
+      <c r="I259">
+        <f t="shared" si="10"/>
+        <v>7.3087275189236353E-9</v>
+      </c>
+      <c r="L259" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A260" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C260" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D260">
+        <v>2019</v>
+      </c>
+      <c r="E260">
+        <v>1061072</v>
+      </c>
+      <c r="F260">
+        <v>11192662</v>
+      </c>
+      <c r="G260">
+        <v>9.480068280450174E-2</v>
+      </c>
+      <c r="H260" s="30">
+        <f t="shared" si="9"/>
+        <v>9.480068280450174E-2</v>
+      </c>
+      <c r="I260">
+        <f t="shared" si="10"/>
+        <v>7.6669440517637356E-9</v>
+      </c>
+      <c r="L260" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A261" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C261" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D261">
+        <v>2019</v>
+      </c>
+      <c r="E261">
+        <v>1008573</v>
+      </c>
+      <c r="F261">
+        <v>11192662</v>
+      </c>
+      <c r="G261">
+        <v>9.0110198985728335E-2</v>
+      </c>
+      <c r="H261" s="30">
+        <f t="shared" si="9"/>
+        <v>9.0110198985728335E-2</v>
+      </c>
+      <c r="I261">
+        <f t="shared" si="10"/>
+        <v>7.32536647890205E-9</v>
+      </c>
+      <c r="L261" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A262" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C262" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D262">
+        <v>2019</v>
+      </c>
+      <c r="E262">
+        <v>805405</v>
+      </c>
+      <c r="F262">
+        <v>11192662</v>
+      </c>
+      <c r="G262">
+        <v>7.195830625458001E-2</v>
+      </c>
+      <c r="H262" s="30">
+        <f t="shared" si="9"/>
+        <v>7.195830625458001E-2</v>
+      </c>
+      <c r="I262">
+        <f t="shared" si="10"/>
+        <v>5.9664366185231072E-9</v>
+      </c>
+      <c r="L262" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A263" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C263" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D263">
+        <v>2019</v>
+      </c>
+      <c r="E263">
+        <v>613052</v>
+      </c>
+      <c r="F263">
+        <v>11192662</v>
+      </c>
+      <c r="G263">
+        <v>5.4772671595014664E-2</v>
+      </c>
+      <c r="H263" s="30">
+        <f t="shared" si="9"/>
+        <v>5.4772671595014664E-2</v>
+      </c>
+      <c r="I263">
+        <f t="shared" si="10"/>
+        <v>4.6255864816930365E-9</v>
+      </c>
+      <c r="L263" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A264" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C264" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D264">
+        <v>2019</v>
+      </c>
+      <c r="E264">
+        <v>517032</v>
+      </c>
+      <c r="F264">
+        <v>11192662</v>
+      </c>
+      <c r="G264">
+        <v>4.6193836640470338E-2</v>
+      </c>
+      <c r="H264" s="30">
+        <f t="shared" si="9"/>
+        <v>4.6193836640470338E-2</v>
+      </c>
+      <c r="I264">
+        <f t="shared" si="10"/>
+        <v>3.9365046578645785E-9</v>
+      </c>
+      <c r="L264" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A265" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C265" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D265">
+        <v>2019</v>
+      </c>
+      <c r="E265">
+        <v>423932</v>
+      </c>
+      <c r="F265">
+        <v>11192662</v>
+      </c>
+      <c r="G265">
+        <v>3.7875886898040875E-2</v>
+      </c>
+      <c r="H265" s="30">
+        <f t="shared" si="9"/>
+        <v>3.7875886898040875E-2</v>
+      </c>
+      <c r="I265">
+        <f t="shared" si="10"/>
+        <v>3.2558210093119662E-9</v>
+      </c>
+      <c r="L265" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A266" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C266" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D266">
+        <v>2019</v>
+      </c>
+      <c r="E266">
+        <v>376538</v>
+      </c>
+      <c r="F266">
+        <v>11192662</v>
+      </c>
+      <c r="G266">
+        <v>3.3641505479214864E-2</v>
+      </c>
+      <c r="H266" s="30">
+        <f t="shared" si="9"/>
+        <v>3.3641505479214864E-2</v>
+      </c>
+      <c r="I266">
+        <f t="shared" si="10"/>
+        <v>2.9045596649221447E-9</v>
+      </c>
+      <c r="L266" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A267" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C267" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D267">
+        <v>2019</v>
+      </c>
+      <c r="E267">
+        <v>306529</v>
+      </c>
+      <c r="F267">
+        <v>11192662</v>
+      </c>
+      <c r="G267">
+        <v>2.7386603830259502E-2</v>
+      </c>
+      <c r="H267" s="30">
+        <f t="shared" si="9"/>
+        <v>2.7386603830259502E-2</v>
+      </c>
+      <c r="I267">
+        <f t="shared" si="10"/>
+        <v>2.3798250819066919E-9</v>
+      </c>
+      <c r="L267" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A268" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C268" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D268">
+        <v>2019</v>
+      </c>
+      <c r="E268">
+        <v>244864</v>
+      </c>
+      <c r="F268">
+        <v>11192662</v>
+      </c>
+      <c r="G268">
+        <v>2.1877190609347445E-2</v>
+      </c>
+      <c r="H268" s="30">
+        <f t="shared" si="9"/>
+        <v>2.1877190609347445E-2</v>
+      </c>
+      <c r="I268">
+        <f t="shared" si="10"/>
+        <v>1.9118400198620957E-9</v>
+      </c>
+      <c r="L268" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A269" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C269" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D269">
+        <v>2019</v>
+      </c>
+      <c r="E269">
+        <v>178784</v>
+      </c>
+      <c r="F269">
+        <v>11192662</v>
+      </c>
+      <c r="G269">
+        <v>1.597332252148774E-2</v>
+      </c>
+      <c r="H269" s="30">
+        <f t="shared" si="9"/>
+        <v>1.597332252148774E-2</v>
+      </c>
+      <c r="I269">
+        <f t="shared" si="10"/>
+        <v>1.404328611827309E-9</v>
+      </c>
+      <c r="L269" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A270" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C270" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D270">
+        <v>2019</v>
+      </c>
+      <c r="E270">
+        <v>106104</v>
+      </c>
+      <c r="F270">
+        <v>11192662</v>
+      </c>
+      <c r="G270">
+        <v>9.4797823788478567E-3</v>
+      </c>
+      <c r="H270" s="30">
+        <f t="shared" si="9"/>
+        <v>9.4797823788478567E-3</v>
+      </c>
+      <c r="I270">
+        <f t="shared" si="10"/>
+        <v>8.3893501875581897E-10</v>
+      </c>
+      <c r="L270" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add total population size calibration targets
Add total population size in 2001 and 2011 as calibration targets.
Reduce years we calibrate to the population age distribution to only
1996 and 2016 in order to try to prioritize other targets in the
likelihood function. Change variable name used in calculation of the
population age distribution likelihood to be more accurate.

Closes #68
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="116">
   <si>
     <t>N</t>
   </si>
@@ -402,6 +402,18 @@
   </si>
   <si>
     <t>KZN population data from Statistics South Africa. Primary tables Census '96 and 2001 compared. KwaZulu-Natal Table 4.1 and 4.3. South Africa Table 4.1. Statistics South Africa Statistical Release P0301 Community Survey 2016 Table 2.1: Censuss 2011 and Community Survey 2016. Statistics South Africa Statistical Release P0302 2019 Mid-year population estimates Table 6 and Table 11. Assume a normal approximation of the binomial distribution where µ=proportion (p) and variance=(p(1-p))/n.</t>
+  </si>
+  <si>
+    <t>all men &amp; women</t>
+  </si>
+  <si>
+    <t>Total population size</t>
+  </si>
+  <si>
+    <t>Absolute error for KZN from the Statistics South Africa Census 2001 Post-enumeration survey, Table 2.7: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution.</t>
+  </si>
+  <si>
+    <t>Absolute error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution.</t>
   </si>
 </sst>
 </file>
@@ -467,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -521,6 +533,10 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,30 +861,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X270"/>
+  <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B273" sqref="B273"/>
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F279" sqref="F279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="37.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="61.453125" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="61.42578125" customWidth="1"/>
     <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -909,7 +925,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -947,7 +963,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -982,7 +998,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1017,7 +1033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1052,7 +1068,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1087,7 +1103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1122,7 +1138,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1157,7 +1173,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1192,7 +1208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1244,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1264,7 +1280,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1299,7 +1315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1334,7 +1350,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +1385,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1404,7 +1420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1439,7 +1455,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1474,7 +1490,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1509,7 +1525,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1544,7 +1560,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1580,7 +1596,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1616,7 +1632,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1654,7 +1670,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1724,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1759,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1794,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1829,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1864,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1899,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1934,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1969,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2004,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
@@ -2039,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -2074,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
@@ -2109,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -2144,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -2179,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -2214,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2249,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>25</v>
       </c>
@@ -2284,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -2319,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -2354,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -2389,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>26</v>
       </c>
@@ -2424,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -2459,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
@@ -2494,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
@@ -2529,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -2564,7 +2580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2601,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -2638,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>26</v>
       </c>
@@ -2675,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -2719,7 +2735,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>29</v>
       </c>
@@ -2760,7 +2776,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
@@ -2801,7 +2817,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2842,7 +2858,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>34</v>
       </c>
@@ -2883,7 +2899,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>34</v>
       </c>
@@ -2924,7 +2940,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -2965,7 +2981,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>34</v>
       </c>
@@ -3006,7 +3022,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>38</v>
       </c>
@@ -3044,7 +3060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>38</v>
       </c>
@@ -3079,7 +3095,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -3114,7 +3130,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
@@ -3149,7 +3165,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>38</v>
       </c>
@@ -3184,7 +3200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>38</v>
       </c>
@@ -3219,7 +3235,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>38</v>
       </c>
@@ -3254,7 +3270,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>39</v>
       </c>
@@ -3289,7 +3305,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>39</v>
       </c>
@@ -3324,7 +3340,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>39</v>
       </c>
@@ -3359,7 +3375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>39</v>
       </c>
@@ -3396,7 +3412,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>39</v>
       </c>
@@ -3433,7 +3449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>39</v>
       </c>
@@ -3470,7 +3486,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>39</v>
       </c>
@@ -3507,7 +3523,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>40</v>
       </c>
@@ -3544,7 +3560,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>40</v>
       </c>
@@ -3581,7 +3597,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>40</v>
       </c>
@@ -3618,7 +3634,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>40</v>
       </c>
@@ -3655,7 +3671,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>40</v>
       </c>
@@ -3692,7 +3708,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>40</v>
       </c>
@@ -3729,7 +3745,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>40</v>
       </c>
@@ -3766,7 +3782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>41</v>
       </c>
@@ -3803,7 +3819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>41</v>
       </c>
@@ -3840,7 +3856,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>41</v>
       </c>
@@ -3877,7 +3893,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>41</v>
       </c>
@@ -3914,7 +3930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>41</v>
       </c>
@@ -3951,7 +3967,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>41</v>
       </c>
@@ -3988,7 +4004,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -4025,7 +4041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>42</v>
       </c>
@@ -4062,7 +4078,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>42</v>
       </c>
@@ -4099,7 +4115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>42</v>
       </c>
@@ -4136,7 +4152,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
@@ -4173,7 +4189,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>42</v>
       </c>
@@ -4210,7 +4226,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>42</v>
       </c>
@@ -4247,7 +4263,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
@@ -4284,7 +4300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>43</v>
       </c>
@@ -4321,7 +4337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>43</v>
       </c>
@@ -4358,7 +4374,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>43</v>
       </c>
@@ -4395,7 +4411,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>43</v>
       </c>
@@ -4432,7 +4448,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>43</v>
       </c>
@@ -4469,7 +4485,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>43</v>
       </c>
@@ -4506,7 +4522,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>43</v>
       </c>
@@ -4543,7 +4559,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>44</v>
       </c>
@@ -4580,7 +4596,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>44</v>
       </c>
@@ -4617,7 +4633,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>44</v>
       </c>
@@ -4654,7 +4670,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>44</v>
       </c>
@@ -4691,7 +4707,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>44</v>
       </c>
@@ -4728,7 +4744,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>44</v>
       </c>
@@ -4765,7 +4781,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>44</v>
       </c>
@@ -4802,7 +4818,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>45</v>
       </c>
@@ -4839,7 +4855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>45</v>
       </c>
@@ -4876,7 +4892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>45</v>
       </c>
@@ -4913,7 +4929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>45</v>
       </c>
@@ -4950,7 +4966,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>45</v>
       </c>
@@ -4987,7 +5003,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>45</v>
       </c>
@@ -5024,7 +5040,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>45</v>
       </c>
@@ -5061,7 +5077,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>46</v>
       </c>
@@ -5098,7 +5114,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>46</v>
       </c>
@@ -5135,7 +5151,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>46</v>
       </c>
@@ -5172,7 +5188,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>46</v>
       </c>
@@ -5209,7 +5225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>46</v>
       </c>
@@ -5246,7 +5262,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>46</v>
       </c>
@@ -5283,7 +5299,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>46</v>
       </c>
@@ -5320,7 +5336,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>47</v>
       </c>
@@ -5357,7 +5373,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>47</v>
       </c>
@@ -5394,7 +5410,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>47</v>
       </c>
@@ -5431,7 +5447,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>47</v>
       </c>
@@ -5468,7 +5484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>47</v>
       </c>
@@ -5505,7 +5521,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>47</v>
       </c>
@@ -5542,7 +5558,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>47</v>
       </c>
@@ -5579,7 +5595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>48</v>
       </c>
@@ -5616,7 +5632,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>48</v>
       </c>
@@ -5653,7 +5669,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>48</v>
       </c>
@@ -5690,7 +5706,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>48</v>
       </c>
@@ -5727,7 +5743,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>48</v>
       </c>
@@ -5764,7 +5780,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>48</v>
       </c>
@@ -5801,7 +5817,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>48</v>
       </c>
@@ -5838,7 +5854,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>49</v>
       </c>
@@ -5875,7 +5891,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>49</v>
       </c>
@@ -5912,7 +5928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>49</v>
       </c>
@@ -5949,7 +5965,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>49</v>
       </c>
@@ -5986,7 +6002,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>49</v>
       </c>
@@ -6023,7 +6039,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>49</v>
       </c>
@@ -6060,7 +6076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>49</v>
       </c>
@@ -6097,7 +6113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>53</v>
       </c>
@@ -6137,7 +6153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>53</v>
       </c>
@@ -6174,7 +6190,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>53</v>
       </c>
@@ -6211,7 +6227,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>53</v>
       </c>
@@ -6248,7 +6264,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>53</v>
       </c>
@@ -6285,7 +6301,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>53</v>
       </c>
@@ -6322,7 +6338,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>53</v>
       </c>
@@ -6359,7 +6375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>53</v>
       </c>
@@ -6396,7 +6412,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>53</v>
       </c>
@@ -6433,7 +6449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>54</v>
       </c>
@@ -6470,7 +6486,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>54</v>
       </c>
@@ -6507,7 +6523,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>54</v>
       </c>
@@ -6544,7 +6560,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>54</v>
       </c>
@@ -6581,7 +6597,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>54</v>
       </c>
@@ -6618,7 +6634,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>54</v>
       </c>
@@ -6655,7 +6671,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>54</v>
       </c>
@@ -6692,7 +6708,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>54</v>
       </c>
@@ -6729,7 +6745,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>54</v>
       </c>
@@ -6766,7 +6782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="145" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>70</v>
       </c>
@@ -6806,7 +6822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>70</v>
       </c>
@@ -6843,7 +6859,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>70</v>
       </c>
@@ -6880,7 +6896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>70</v>
       </c>
@@ -6917,7 +6933,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>70</v>
       </c>
@@ -6954,7 +6970,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>70</v>
       </c>
@@ -6991,7 +7007,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>70</v>
       </c>
@@ -7028,7 +7044,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>70</v>
       </c>
@@ -7065,7 +7081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>70</v>
       </c>
@@ -7102,7 +7118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>70</v>
       </c>
@@ -7139,7 +7155,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>70</v>
       </c>
@@ -7176,7 +7192,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>70</v>
       </c>
@@ -7213,7 +7229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>70</v>
       </c>
@@ -7250,7 +7266,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>79</v>
       </c>
@@ -7286,7 +7302,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
         <v>80</v>
       </c>
@@ -7319,7 +7335,7 @@
       </c>
       <c r="M176" s="8"/>
     </row>
-    <row r="177" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>83</v>
       </c>
@@ -7354,7 +7370,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>86</v>
       </c>
@@ -7387,7 +7403,7 @@
       </c>
       <c r="M178" s="8"/>
     </row>
-    <row r="179" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>84</v>
       </c>
@@ -7422,7 +7438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>87</v>
       </c>
@@ -7455,7 +7471,7 @@
       </c>
       <c r="M180" s="8"/>
     </row>
-    <row r="181" spans="1:24" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:24" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>85</v>
       </c>
@@ -7490,7 +7506,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="182" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>88</v>
       </c>
@@ -7519,7 +7535,7 @@
       </c>
       <c r="M182" s="8"/>
     </row>
-    <row r="183" spans="1:24" ht="165.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:24" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="15" t="s">
         <v>79</v>
       </c>
@@ -7587,7 +7603,7 @@
         <v>4.874791589632058E-4</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="15" t="s">
         <v>80</v>
       </c>
@@ -7647,7 +7663,7 @@
         <v>4.8747915896320553E-4</v>
       </c>
     </row>
-    <row r="185" spans="1:24" ht="137.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:24" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="15" t="s">
         <v>83</v>
       </c>
@@ -7699,7 +7715,7 @@
         <v>2.9502063905325444E-4</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A186" s="15" t="s">
         <v>86</v>
       </c>
@@ -7745,7 +7761,7 @@
         <v>2.9502063905325444E-4</v>
       </c>
     </row>
-    <row r="187" spans="1:24" ht="108.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:24" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="15" t="s">
         <v>84</v>
       </c>
@@ -7797,7 +7813,7 @@
         <v>3.9463064516129034E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" s="15" t="s">
         <v>87</v>
       </c>
@@ -7843,7 +7859,7 @@
         <v>3.9463064516129034E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:24" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A189" s="15" t="s">
         <v>85</v>
       </c>
@@ -7911,7 +7927,7 @@
         <v>4.8534811111111112E-4</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A190" s="15" t="s">
         <v>88</v>
       </c>
@@ -7971,7 +7987,7 @@
         <v>4.8534811111111112E-4</v>
       </c>
     </row>
-    <row r="191" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A191" s="15" t="s">
         <v>110</v>
       </c>
@@ -8008,7 +8024,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="15" t="s">
         <v>110</v>
       </c>
@@ -8043,7 +8059,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="15" t="s">
         <v>110</v>
       </c>
@@ -8078,7 +8094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="15" t="s">
         <v>110</v>
       </c>
@@ -8113,7 +8129,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="15" t="s">
         <v>110</v>
       </c>
@@ -8148,7 +8164,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="15" t="s">
         <v>110</v>
       </c>
@@ -8183,7 +8199,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="15" t="s">
         <v>110</v>
       </c>
@@ -8218,7 +8234,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="15" t="s">
         <v>110</v>
       </c>
@@ -8253,7 +8269,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="15" t="s">
         <v>110</v>
       </c>
@@ -8288,7 +8304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="15" t="s">
         <v>110</v>
       </c>
@@ -8323,7 +8339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="15" t="s">
         <v>110</v>
       </c>
@@ -8358,7 +8374,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="15" t="s">
         <v>110</v>
       </c>
@@ -8393,7 +8409,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="15" t="s">
         <v>110</v>
       </c>
@@ -8428,7 +8444,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="15" t="s">
         <v>110</v>
       </c>
@@ -8463,7 +8479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="15" t="s">
         <v>110</v>
       </c>
@@ -8498,7 +8514,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" s="15" t="s">
         <v>110</v>
       </c>
@@ -8533,7 +8549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="15" t="s">
         <v>110</v>
       </c>
@@ -8564,10 +8580,10 @@
         <v>1.0332637306761254E-8</v>
       </c>
       <c r="L207" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" s="15" t="s">
         <v>110</v>
       </c>
@@ -8598,10 +8614,10 @@
         <v>1.1254804180454987E-8</v>
       </c>
       <c r="L208" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" s="15" t="s">
         <v>110</v>
       </c>
@@ -8632,10 +8648,10 @@
         <v>1.1465792612242759E-8</v>
       </c>
       <c r="L209" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" s="15" t="s">
         <v>110</v>
       </c>
@@ -8666,10 +8682,10 @@
         <v>1.1337285321102111E-8</v>
       </c>
       <c r="L210" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" s="15" t="s">
         <v>110</v>
       </c>
@@ -8700,10 +8716,10 @@
         <v>9.3555366931340526E-9</v>
       </c>
       <c r="L211" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="15" t="s">
         <v>110</v>
       </c>
@@ -8734,10 +8750,10 @@
         <v>8.2839586205679468E-9</v>
       </c>
       <c r="L212" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="15" t="s">
         <v>110</v>
       </c>
@@ -8768,10 +8784,10 @@
         <v>6.7543120307208839E-9</v>
       </c>
       <c r="L213" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="15" t="s">
         <v>110</v>
       </c>
@@ -8802,10 +8818,10 @@
         <v>6.2830578837469086E-9</v>
       </c>
       <c r="L214" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="15" t="s">
         <v>110</v>
       </c>
@@ -8836,10 +8852,10 @@
         <v>5.3266482802985421E-9</v>
       </c>
       <c r="L215" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" s="15" t="s">
         <v>110</v>
       </c>
@@ -8870,10 +8886,10 @@
         <v>4.3397527436625145E-9</v>
       </c>
       <c r="L216" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" s="15" t="s">
         <v>110</v>
       </c>
@@ -8904,10 +8920,10 @@
         <v>3.6736427613513551E-9</v>
       </c>
       <c r="L217" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="15" t="s">
         <v>110</v>
       </c>
@@ -8938,10 +8954,10 @@
         <v>2.6857931058207825E-9</v>
       </c>
       <c r="L218" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="15" t="s">
         <v>110</v>
       </c>
@@ -8972,10 +8988,10 @@
         <v>2.4095793617634816E-9</v>
       </c>
       <c r="L219" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="15" t="s">
         <v>110</v>
       </c>
@@ -9006,10 +9022,10 @@
         <v>1.7420903307285709E-9</v>
       </c>
       <c r="L220" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="15" t="s">
         <v>110</v>
       </c>
@@ -9040,10 +9056,10 @@
         <v>1.486711004144262E-9</v>
       </c>
       <c r="L221" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="15" t="s">
         <v>110</v>
       </c>
@@ -9074,10 +9090,10 @@
         <v>8.2320631649556376E-10</v>
       </c>
       <c r="L222" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="15" t="s">
         <v>110</v>
       </c>
@@ -9108,10 +9124,10 @@
         <v>1.0239832219882873E-8</v>
       </c>
       <c r="L223" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" s="15" t="s">
         <v>110</v>
       </c>
@@ -9142,10 +9158,10 @@
         <v>9.0646678587588034E-9</v>
       </c>
       <c r="L224" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" s="15" t="s">
         <v>110</v>
       </c>
@@ -9176,10 +9192,10 @@
         <v>9.0363861503197521E-9</v>
       </c>
       <c r="L225" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" s="15" t="s">
         <v>110</v>
       </c>
@@ -9210,10 +9226,10 @@
         <v>9.6520112027050787E-9</v>
       </c>
       <c r="L226" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" s="15" t="s">
         <v>110</v>
       </c>
@@ -9244,10 +9260,10 @@
         <v>9.5222075352605795E-9</v>
       </c>
       <c r="L227" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" s="15" t="s">
         <v>110</v>
       </c>
@@ -9278,10 +9294,10 @@
         <v>8.5867004691429685E-9</v>
       </c>
       <c r="L228" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" s="15" t="s">
         <v>110</v>
       </c>
@@ -9312,10 +9328,10 @@
         <v>6.5584739917074511E-9</v>
       </c>
       <c r="L229" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" s="15" t="s">
         <v>110</v>
       </c>
@@ -9346,10 +9362,10 @@
         <v>5.5778094943989062E-9</v>
       </c>
       <c r="L230" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" s="15" t="s">
         <v>110</v>
       </c>
@@ -9380,10 +9396,10 @@
         <v>4.5983168336084311E-9</v>
       </c>
       <c r="L231" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" s="15" t="s">
         <v>110</v>
       </c>
@@ -9414,10 +9430,10 @@
         <v>4.2079331003297735E-9</v>
       </c>
       <c r="L232" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" s="15" t="s">
         <v>110</v>
       </c>
@@ -9448,10 +9464,10 @@
         <v>3.5835716651381008E-9</v>
       </c>
       <c r="L233" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" s="15" t="s">
         <v>110</v>
       </c>
@@ -9482,10 +9498,10 @@
         <v>3.0534277260250306E-9</v>
       </c>
       <c r="L234" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" s="15" t="s">
         <v>110</v>
       </c>
@@ -9516,10 +9532,10 @@
         <v>2.5587182519172453E-9</v>
       </c>
       <c r="L235" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" s="15" t="s">
         <v>110</v>
       </c>
@@ -9550,10 +9566,10 @@
         <v>1.6726966189359743E-9</v>
       </c>
       <c r="L236" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" s="15" t="s">
         <v>110</v>
       </c>
@@ -9584,10 +9600,10 @@
         <v>1.317258656228455E-9</v>
       </c>
       <c r="L237" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" s="15" t="s">
         <v>110</v>
       </c>
@@ -9618,10 +9634,10 @@
         <v>8.2981732619473843E-10</v>
       </c>
       <c r="L238" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" s="15" t="s">
         <v>110</v>
       </c>
@@ -9655,7 +9671,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" s="15" t="s">
         <v>110</v>
       </c>
@@ -9689,7 +9705,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" s="15" t="s">
         <v>110</v>
       </c>
@@ -9723,7 +9739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" s="15" t="s">
         <v>110</v>
       </c>
@@ -9757,7 +9773,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" s="15" t="s">
         <v>110</v>
       </c>
@@ -9791,7 +9807,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" s="15" t="s">
         <v>110</v>
       </c>
@@ -9825,7 +9841,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" s="15" t="s">
         <v>110</v>
       </c>
@@ -9859,7 +9875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" s="15" t="s">
         <v>110</v>
       </c>
@@ -9893,7 +9909,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" s="15" t="s">
         <v>110</v>
       </c>
@@ -9927,7 +9943,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" s="15" t="s">
         <v>110</v>
       </c>
@@ -9961,7 +9977,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" s="15" t="s">
         <v>110</v>
       </c>
@@ -9995,7 +10011,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" s="15" t="s">
         <v>110</v>
       </c>
@@ -10029,7 +10045,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" s="15" t="s">
         <v>110</v>
       </c>
@@ -10063,7 +10079,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" s="15" t="s">
         <v>110</v>
       </c>
@@ -10097,7 +10113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" s="15" t="s">
         <v>110</v>
       </c>
@@ -10131,7 +10147,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" s="15" t="s">
         <v>110</v>
       </c>
@@ -10165,7 +10181,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" s="15" t="s">
         <v>110</v>
       </c>
@@ -10196,10 +10212,10 @@
         <v>8.746230443946397E-9</v>
       </c>
       <c r="L255" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" s="15" t="s">
         <v>110</v>
       </c>
@@ -10230,10 +10246,10 @@
         <v>8.5325036283775244E-9</v>
       </c>
       <c r="L256" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257" s="15" t="s">
         <v>110</v>
       </c>
@@ -10264,10 +10280,10 @@
         <v>8.1486804979842301E-9</v>
       </c>
       <c r="L257" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" s="15" t="s">
         <v>110</v>
       </c>
@@ -10298,10 +10314,10 @@
         <v>7.1415808130567291E-9</v>
       </c>
       <c r="L258" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259" s="15" t="s">
         <v>110</v>
       </c>
@@ -10332,10 +10348,10 @@
         <v>7.3087275189236353E-9</v>
       </c>
       <c r="L259" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260" s="15" t="s">
         <v>110</v>
       </c>
@@ -10366,10 +10382,10 @@
         <v>7.6669440517637356E-9</v>
       </c>
       <c r="L260" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" s="15" t="s">
         <v>110</v>
       </c>
@@ -10400,10 +10416,10 @@
         <v>7.32536647890205E-9</v>
       </c>
       <c r="L261" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" s="15" t="s">
         <v>110</v>
       </c>
@@ -10434,10 +10450,10 @@
         <v>5.9664366185231072E-9</v>
       </c>
       <c r="L262" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263" s="15" t="s">
         <v>110</v>
       </c>
@@ -10468,10 +10484,10 @@
         <v>4.6255864816930365E-9</v>
       </c>
       <c r="L263" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264" s="15" t="s">
         <v>110</v>
       </c>
@@ -10502,10 +10518,10 @@
         <v>3.9365046578645785E-9</v>
       </c>
       <c r="L264" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265" s="15" t="s">
         <v>110</v>
       </c>
@@ -10536,10 +10552,10 @@
         <v>3.2558210093119662E-9</v>
       </c>
       <c r="L265" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266" s="15" t="s">
         <v>110</v>
       </c>
@@ -10570,10 +10586,10 @@
         <v>2.9045596649221447E-9</v>
       </c>
       <c r="L266" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A267" s="15" t="s">
         <v>110</v>
       </c>
@@ -10604,10 +10620,10 @@
         <v>2.3798250819066919E-9</v>
       </c>
       <c r="L267" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268" s="15" t="s">
         <v>110</v>
       </c>
@@ -10638,10 +10654,10 @@
         <v>1.9118400198620957E-9</v>
       </c>
       <c r="L268" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269" s="15" t="s">
         <v>110</v>
       </c>
@@ -10672,10 +10688,10 @@
         <v>1.404328611827309E-9</v>
       </c>
       <c r="L269" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270" s="15" t="s">
         <v>110</v>
       </c>
@@ -10706,8 +10722,66 @@
         <v>8.3893501875581897E-10</v>
       </c>
       <c r="L270" t="s">
-        <v>58</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A271" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B271" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C271" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D271">
+        <v>2001</v>
+      </c>
+      <c r="H271">
+        <v>9348178000</v>
+      </c>
+      <c r="I271">
+        <v>395000000</v>
+      </c>
+      <c r="L271" t="s">
+        <v>58</v>
+      </c>
+      <c r="M271" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A272" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B272" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C272" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D272">
+        <v>2011</v>
+      </c>
+      <c r="H272">
+        <v>10159121000</v>
+      </c>
+      <c r="I272">
+        <v>109994000</v>
+      </c>
+      <c r="L272" t="s">
+        <v>58</v>
+      </c>
+      <c r="M272" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C273" s="31"/>
+    </row>
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C274" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 2019 total population as a calib target
Previously only calibrating to total population in 2001 and 2011 because
the 2001 and 2011 census provide confidence intervals on their
population estimates. However, assuming that variance continues to
decrease as sampling techniques improve, using the 2011 variance for
2019. This will help calibrate the second fertility decrease from 2010
to 2020.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="117">
   <si>
     <t>N</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>Absolute error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution.</t>
+  </si>
+  <si>
+    <t>Using variance from 2011. Assumes that variance continues to decrease as sampling techniques improve and that this is therefore a conservative approximation.</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
   <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F279" sqref="F279"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I275" sqref="I275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10777,10 +10780,33 @@
         <v>115</v>
       </c>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C273" s="31"/>
-    </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A273" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B273" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C273" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D273">
+        <v>2019</v>
+      </c>
+      <c r="H273">
+        <v>11192662000</v>
+      </c>
+      <c r="I273">
+        <v>109994000</v>
+      </c>
+      <c r="L273" t="s">
+        <v>58</v>
+      </c>
+      <c r="M273" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C274" s="31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix total population variance for calibration
Absolute error was reported for the 2001 and 2011 Census. This is not
the same as variance. Can calculate standard error from the absolute
error, and then variance as the square of the standard error.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -410,13 +410,13 @@
     <t>Total population size</t>
   </si>
   <si>
-    <t>Absolute error for KZN from the Statistics South Africa Census 2001 Post-enumeration survey, Table 2.7: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution.</t>
-  </si>
-  <si>
-    <t>Absolute error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution.</t>
-  </si>
-  <si>
     <t>Using variance from 2011. Assumes that variance continues to decrease as sampling techniques improve and that this is therefore a conservative approximation.</t>
+  </si>
+  <si>
+    <t>Absolute error for KZN from the Statistics South Africa Census 2001 Post-enumeration survey, Table 2.7: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution. Calculate the standard error (SE) as (absolute error/1.96). Variance is then SE^2.</t>
+  </si>
+  <si>
+    <t>Absolute error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution. Calculate the standard error (SE) as (absolute error/1.96). Variance is then SE^2.</t>
   </si>
 </sst>
 </file>
@@ -867,8 +867,8 @@
   <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I275" sqref="I275"/>
+      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P271" sqref="P271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10728,7 +10728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="15" t="s">
         <v>113</v>
       </c>
@@ -10745,16 +10745,17 @@
         <v>9348178000</v>
       </c>
       <c r="I271">
-        <v>395000000</v>
+        <f>(395000000/1.96)^2</f>
+        <v>4.0614587671803416E+16</v>
       </c>
       <c r="L271" t="s">
         <v>58</v>
       </c>
       <c r="M271" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="272" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="15" t="s">
         <v>113</v>
       </c>
@@ -10771,13 +10772,14 @@
         <v>10159121000</v>
       </c>
       <c r="I272">
-        <v>109994000</v>
+        <f>(109994000/1.96)^2</f>
+        <v>3149385682007496.5</v>
       </c>
       <c r="L272" t="s">
         <v>58</v>
       </c>
       <c r="M272" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="273" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10797,13 +10799,14 @@
         <v>11192662000</v>
       </c>
       <c r="I273">
-        <v>109994000</v>
+        <f>(109994000/1.96)^2</f>
+        <v>3149385682007496.5</v>
       </c>
       <c r="L273" t="s">
         <v>58</v>
       </c>
       <c r="M273" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix total pop calibration mean/var & reload .mat
For calibrating to the total population size, used the wrong order of magnitude for the mean and
absolute/standard error (used to calculate variance). Both values were three orders of
magnitude too large. 2011 Census reported value is actually standard error, not
absolute error. Therefore redid calculation of 2011 variance. Had also
not re-saved the calibData.mat file after the recent update of the
variance. Noticed all these issues because the observed mean was >>
model population size, and this was causing a much larger magnitude of
the summed log-likelihood.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -416,7 +416,7 @@
     <t>Absolute error for KZN from the Statistics South Africa Census 2001 Post-enumeration survey, Table 2.7: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution. Calculate the standard error (SE) as (absolute error/1.96). Variance is then SE^2.</t>
   </si>
   <si>
-    <t>Absolute error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution. Calculate the standard error (SE) as (absolute error/1.96). Variance is then SE^2.</t>
+    <t>Standard error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution. Variance calculated as SE^2.</t>
   </si>
 </sst>
 </file>
@@ -867,8 +867,8 @@
   <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P271" sqref="P271"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E272" sqref="E272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10742,11 +10742,11 @@
         <v>2001</v>
       </c>
       <c r="H271">
-        <v>9348178000</v>
+        <v>9348178</v>
       </c>
       <c r="I271">
-        <f>(395000000/1.96)^2</f>
-        <v>4.0614587671803416E+16</v>
+        <f>(395000/1.96)^2</f>
+        <v>40614587671.803413</v>
       </c>
       <c r="L271" t="s">
         <v>58</v>
@@ -10769,11 +10769,11 @@
         <v>2011</v>
       </c>
       <c r="H272">
-        <v>10159121000</v>
+        <v>10159121</v>
       </c>
       <c r="I272">
-        <f>(109994000/1.96)^2</f>
-        <v>3149385682007496.5</v>
+        <f>(109994)^2</f>
+        <v>12098680036</v>
       </c>
       <c r="L272" t="s">
         <v>58</v>
@@ -10796,11 +10796,11 @@
         <v>2019</v>
       </c>
       <c r="H273">
-        <v>11192662000</v>
+        <v>11192662</v>
       </c>
       <c r="I273">
-        <f>(109994000/1.96)^2</f>
-        <v>3149385682007496.5</v>
+        <f>(109994)^2</f>
+        <v>12098680036</v>
       </c>
       <c r="L273" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Calibrate to 2011, 2019 KZN age distribution
In addition to years 1996 andn 2016, calibrate to the KZN age
distribution in 2011 and 2019. This will better capture changes
in the distribution, particularly after 2016.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -867,8 +867,8 @@
   <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E272" sqref="E272"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M259" sqref="M259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9127,7 +9127,7 @@
         <v>1.0239832219882873E-8</v>
       </c>
       <c r="L223" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.25">
@@ -9161,7 +9161,7 @@
         <v>9.0646678587588034E-9</v>
       </c>
       <c r="L224" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.25">
@@ -9195,7 +9195,7 @@
         <v>9.0363861503197521E-9</v>
       </c>
       <c r="L225" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.25">
@@ -9229,7 +9229,7 @@
         <v>9.6520112027050787E-9</v>
       </c>
       <c r="L226" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.25">
@@ -9263,7 +9263,7 @@
         <v>9.5222075352605795E-9</v>
       </c>
       <c r="L227" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.25">
@@ -9297,7 +9297,7 @@
         <v>8.5867004691429685E-9</v>
       </c>
       <c r="L228" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.25">
@@ -9331,7 +9331,7 @@
         <v>6.5584739917074511E-9</v>
       </c>
       <c r="L229" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
@@ -9365,7 +9365,7 @@
         <v>5.5778094943989062E-9</v>
       </c>
       <c r="L230" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
@@ -9399,7 +9399,7 @@
         <v>4.5983168336084311E-9</v>
       </c>
       <c r="L231" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
@@ -9433,7 +9433,7 @@
         <v>4.2079331003297735E-9</v>
       </c>
       <c r="L232" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
@@ -9467,7 +9467,7 @@
         <v>3.5835716651381008E-9</v>
       </c>
       <c r="L233" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
@@ -9501,7 +9501,7 @@
         <v>3.0534277260250306E-9</v>
       </c>
       <c r="L234" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
@@ -9535,7 +9535,7 @@
         <v>2.5587182519172453E-9</v>
       </c>
       <c r="L235" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
@@ -9569,7 +9569,7 @@
         <v>1.6726966189359743E-9</v>
       </c>
       <c r="L236" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
@@ -9603,7 +9603,7 @@
         <v>1.317258656228455E-9</v>
       </c>
       <c r="L237" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
@@ -9637,7 +9637,7 @@
         <v>8.2981732619473843E-10</v>
       </c>
       <c r="L238" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
@@ -10215,7 +10215,7 @@
         <v>8.746230443946397E-9</v>
       </c>
       <c r="L255" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
@@ -10249,7 +10249,7 @@
         <v>8.5325036283775244E-9</v>
       </c>
       <c r="L256" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
@@ -10283,7 +10283,7 @@
         <v>8.1486804979842301E-9</v>
       </c>
       <c r="L257" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.25">
@@ -10317,7 +10317,7 @@
         <v>7.1415808130567291E-9</v>
       </c>
       <c r="L258" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.25">
@@ -10351,7 +10351,7 @@
         <v>7.3087275189236353E-9</v>
       </c>
       <c r="L259" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.25">
@@ -10385,7 +10385,7 @@
         <v>7.6669440517637356E-9</v>
       </c>
       <c r="L260" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.25">
@@ -10419,7 +10419,7 @@
         <v>7.32536647890205E-9</v>
       </c>
       <c r="L261" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.25">
@@ -10453,7 +10453,7 @@
         <v>5.9664366185231072E-9</v>
       </c>
       <c r="L262" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.25">
@@ -10487,7 +10487,7 @@
         <v>4.6255864816930365E-9</v>
       </c>
       <c r="L263" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.25">
@@ -10521,7 +10521,7 @@
         <v>3.9365046578645785E-9</v>
       </c>
       <c r="L264" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.25">
@@ -10555,7 +10555,7 @@
         <v>3.2558210093119662E-9</v>
       </c>
       <c r="L265" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.25">
@@ -10589,7 +10589,7 @@
         <v>2.9045596649221447E-9</v>
       </c>
       <c r="L266" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.25">
@@ -10623,7 +10623,7 @@
         <v>2.3798250819066919E-9</v>
       </c>
       <c r="L267" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.25">
@@ -10657,7 +10657,7 @@
         <v>1.9118400198620957E-9</v>
       </c>
       <c r="L268" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.25">
@@ -10691,7 +10691,7 @@
         <v>1.404328611827309E-9</v>
       </c>
       <c r="L269" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.25">
@@ -10725,7 +10725,7 @@
         <v>8.3893501875581897E-10</v>
       </c>
       <c r="L270" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="271" spans="1:13" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove 2016 age distribution calibration target
I think I am over-weighting the importance of the age distribution
relative to other calibration targets because I fit to many data points
by age with low variance. Therefore, removing the age distribution in
2016 from the calibration targets.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -867,8 +867,8 @@
   <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M259" sqref="M259"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M249" sqref="M249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9671,7 +9671,7 @@
         <v>9.7684728703616492E-9</v>
       </c>
       <c r="L239" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
@@ -9705,7 +9705,7 @@
         <v>9.4420929480849662E-9</v>
       </c>
       <c r="L240" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
@@ -9739,7 +9739,7 @@
         <v>8.9434044692568144E-9</v>
       </c>
       <c r="L241" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
@@ -9773,7 +9773,7 @@
         <v>8.0620361646391683E-9</v>
       </c>
       <c r="L242" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
@@ -9807,7 +9807,7 @@
         <v>8.0129783165877258E-9</v>
       </c>
       <c r="L243" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
@@ -9841,7 +9841,7 @@
         <v>7.831677706074032E-9</v>
       </c>
       <c r="L244" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
@@ -9875,7 +9875,7 @@
         <v>6.5191632325615928E-9</v>
       </c>
       <c r="L245" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
@@ -9909,7 +9909,7 @@
         <v>5.1805951316295778E-9</v>
       </c>
       <c r="L246" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
@@ -9943,7 +9943,7 @@
         <v>4.2395325504596404E-9</v>
       </c>
       <c r="L247" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
@@ -9977,7 +9977,7 @@
         <v>3.5456466777438688E-9</v>
       </c>
       <c r="L248" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
@@ -10011,7 +10011,7 @@
         <v>3.0665317971936424E-9</v>
       </c>
       <c r="L249" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
@@ -10045,7 +10045,7 @@
         <v>2.6322117693620562E-9</v>
       </c>
       <c r="L250" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
@@ -10079,7 +10079,7 @@
         <v>2.2474344527822039E-9</v>
       </c>
       <c r="L251" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
@@ -10113,7 +10113,7 @@
         <v>1.7879942123676255E-9</v>
       </c>
       <c r="L252" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
@@ -10147,7 +10147,7 @@
         <v>1.1840882686502118E-9</v>
       </c>
       <c r="L253" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
@@ -10181,7 +10181,7 @@
         <v>6.9452231407165145E-10</v>
       </c>
       <c r="L254" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calibrate to Globocan 2012 CC inc. vs. 2011 NCR black women
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="119">
   <si>
     <t>N</t>
   </si>
@@ -417,6 +417,33 @@
   </si>
   <si>
     <t>Standard error for KZN from the Statistics South Africa Census 2011 Post-enumeration survey, Table 14: Adjusted total population- full universe. Note that the error is for the total KZN population while the mean is for only ages 0-79. This discrepancy shouldn't make too much of a difference because ages 80+ are a small portion of the population. Assume a normal distribution. Variance calculated as SE^2.</t>
+  </si>
+  <si>
+    <t>Globocan 2012</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Incidence rates per 100,000 women come from Globocan 2012. Monisha Sharma emailed a connection to get age-specific rates. A single rate was given for ages 15-39, and I believe Monisha estimated the rates for ages &lt;39 by 5-year age groups. Assume a normal approximation of the Poisson distribution where </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ=λ and variance=λ  and λ=CC incidence rate per year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -482,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -536,9 +563,15 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,11 +897,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X274"/>
+  <dimension ref="A1:X286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M249" sqref="M249"/>
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M275" sqref="M275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6819,7 +6852,7 @@
       <c r="J162" s="7"/>
       <c r="K162" s="7"/>
       <c r="L162" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="M162" s="14" t="s">
         <v>92</v>
@@ -6859,7 +6892,7 @@
       <c r="J163" s="7"/>
       <c r="K163" s="7"/>
       <c r="L163" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -6896,7 +6929,7 @@
       <c r="J164" s="7"/>
       <c r="K164" s="7"/>
       <c r="L164" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -6933,7 +6966,7 @@
       <c r="J165" s="7"/>
       <c r="K165" s="7"/>
       <c r="L165" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -6970,7 +7003,7 @@
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
       <c r="L166" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -7007,7 +7040,7 @@
       <c r="J167" s="7"/>
       <c r="K167" s="7"/>
       <c r="L167" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -7044,7 +7077,7 @@
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
       <c r="L168" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -7081,7 +7114,7 @@
       <c r="J169" s="7"/>
       <c r="K169" s="7"/>
       <c r="L169" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -7118,7 +7151,7 @@
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
       <c r="L170" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -7155,7 +7188,7 @@
       <c r="J171" s="7"/>
       <c r="K171" s="7"/>
       <c r="L171" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -7192,7 +7225,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
       <c r="L172" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -7229,7 +7262,7 @@
       <c r="J173" s="7"/>
       <c r="K173" s="7"/>
       <c r="L173" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -7266,7 +7299,7 @@
       <c r="J174" s="7"/>
       <c r="K174" s="7"/>
       <c r="L174" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -10735,7 +10768,7 @@
       <c r="B271" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C271" s="32" t="s">
+      <c r="C271" s="31" t="s">
         <v>112</v>
       </c>
       <c r="D271">
@@ -10762,7 +10795,7 @@
       <c r="B272" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C272" s="32" t="s">
+      <c r="C272" s="31" t="s">
         <v>112</v>
       </c>
       <c r="D272">
@@ -10789,7 +10822,7 @@
       <c r="B273" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C273" s="32" t="s">
+      <c r="C273" s="31" t="s">
         <v>112</v>
       </c>
       <c r="D273">
@@ -10809,8 +10842,424 @@
         <v>114</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C274" s="31"/>
+    <row r="274" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D274" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E274" s="1"/>
+      <c r="F274" s="10"/>
+      <c r="G274" s="34">
+        <v>0</v>
+      </c>
+      <c r="H274" s="33">
+        <f>G274</f>
+        <v>0</v>
+      </c>
+      <c r="I274" s="7">
+        <f>H274</f>
+        <v>0</v>
+      </c>
+      <c r="J274" s="7"/>
+      <c r="K274" s="7"/>
+      <c r="L274" t="s">
+        <v>58</v>
+      </c>
+      <c r="M274" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D275" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E275" s="1"/>
+      <c r="F275" s="10"/>
+      <c r="G275" s="32">
+        <v>2.646467153656904</v>
+      </c>
+      <c r="H275" s="33">
+        <f t="shared" ref="H275:H286" si="11">G275</f>
+        <v>2.646467153656904</v>
+      </c>
+      <c r="I275" s="7">
+        <f t="shared" ref="I275:I286" si="12">H275</f>
+        <v>2.646467153656904</v>
+      </c>
+      <c r="J275" s="7"/>
+      <c r="K275" s="7"/>
+      <c r="L275" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D276" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E276" s="1"/>
+      <c r="F276" s="10"/>
+      <c r="G276" s="32">
+        <v>8.848389035625793</v>
+      </c>
+      <c r="H276" s="33">
+        <f t="shared" si="11"/>
+        <v>8.848389035625793</v>
+      </c>
+      <c r="I276" s="7">
+        <f t="shared" si="12"/>
+        <v>8.848389035625793</v>
+      </c>
+      <c r="J276" s="7"/>
+      <c r="K276" s="7"/>
+      <c r="L276" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D277" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E277" s="12"/>
+      <c r="F277" s="10"/>
+      <c r="G277" s="32">
+        <v>45.193737900145855</v>
+      </c>
+      <c r="H277" s="33">
+        <f t="shared" si="11"/>
+        <v>45.193737900145855</v>
+      </c>
+      <c r="I277" s="7">
+        <f t="shared" si="12"/>
+        <v>45.193737900145855</v>
+      </c>
+      <c r="J277" s="7"/>
+      <c r="K277" s="7"/>
+      <c r="L277" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D278" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E278" s="12"/>
+      <c r="F278" s="10"/>
+      <c r="G278" s="32">
+        <v>53.40682333812245</v>
+      </c>
+      <c r="H278" s="33">
+        <f t="shared" si="11"/>
+        <v>53.40682333812245</v>
+      </c>
+      <c r="I278" s="7">
+        <f t="shared" si="12"/>
+        <v>53.40682333812245</v>
+      </c>
+      <c r="J278" s="7"/>
+      <c r="K278" s="7"/>
+      <c r="L278" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D279" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E279" s="12"/>
+      <c r="F279" s="10"/>
+      <c r="G279" s="32">
+        <v>63.4</v>
+      </c>
+      <c r="H279" s="33">
+        <f t="shared" si="11"/>
+        <v>63.4</v>
+      </c>
+      <c r="I279" s="7">
+        <f t="shared" si="12"/>
+        <v>63.4</v>
+      </c>
+      <c r="J279" s="7"/>
+      <c r="K279" s="7"/>
+      <c r="L279" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D280" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E280" s="12"/>
+      <c r="F280" s="10"/>
+      <c r="G280" s="32">
+        <v>68.3</v>
+      </c>
+      <c r="H280" s="33">
+        <f t="shared" si="11"/>
+        <v>68.3</v>
+      </c>
+      <c r="I280" s="7">
+        <f t="shared" si="12"/>
+        <v>68.3</v>
+      </c>
+      <c r="J280" s="7"/>
+      <c r="K280" s="7"/>
+      <c r="L280" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D281" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E281" s="12"/>
+      <c r="F281" s="10"/>
+      <c r="G281" s="32">
+        <v>70.7</v>
+      </c>
+      <c r="H281" s="33">
+        <f t="shared" si="11"/>
+        <v>70.7</v>
+      </c>
+      <c r="I281" s="7">
+        <f t="shared" si="12"/>
+        <v>70.7</v>
+      </c>
+      <c r="J281" s="7"/>
+      <c r="K281" s="7"/>
+      <c r="L281" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D282" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E282" s="12"/>
+      <c r="F282" s="10"/>
+      <c r="G282" s="32">
+        <v>73</v>
+      </c>
+      <c r="H282" s="33">
+        <f t="shared" si="11"/>
+        <v>73</v>
+      </c>
+      <c r="I282" s="7">
+        <f t="shared" si="12"/>
+        <v>73</v>
+      </c>
+      <c r="J282" s="7"/>
+      <c r="K282" s="7"/>
+      <c r="L282" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D283" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E283" s="12"/>
+      <c r="F283" s="10"/>
+      <c r="G283" s="32">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="H283" s="33">
+        <f t="shared" si="11"/>
+        <v>77.400000000000006</v>
+      </c>
+      <c r="I283" s="7">
+        <f t="shared" si="12"/>
+        <v>77.400000000000006</v>
+      </c>
+      <c r="J283" s="7"/>
+      <c r="K283" s="7"/>
+      <c r="L283" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D284" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E284" s="12"/>
+      <c r="F284" s="10"/>
+      <c r="G284" s="32">
+        <v>82.7</v>
+      </c>
+      <c r="H284" s="33">
+        <f t="shared" si="11"/>
+        <v>82.7</v>
+      </c>
+      <c r="I284" s="7">
+        <f t="shared" si="12"/>
+        <v>82.7</v>
+      </c>
+      <c r="J284" s="7"/>
+      <c r="K284" s="7"/>
+      <c r="L284" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D285" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E285" s="12"/>
+      <c r="F285" s="10"/>
+      <c r="G285" s="32">
+        <v>88.6</v>
+      </c>
+      <c r="H285" s="33">
+        <f t="shared" si="11"/>
+        <v>88.6</v>
+      </c>
+      <c r="I285" s="7">
+        <f t="shared" si="12"/>
+        <v>88.6</v>
+      </c>
+      <c r="J285" s="7"/>
+      <c r="K285" s="7"/>
+      <c r="L285" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D286" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E286" s="12"/>
+      <c r="F286" s="10"/>
+      <c r="G286" s="32">
+        <v>95.2</v>
+      </c>
+      <c r="H286" s="33">
+        <f t="shared" si="11"/>
+        <v>95.2</v>
+      </c>
+      <c r="I286" s="7">
+        <f t="shared" si="12"/>
+        <v>95.2</v>
+      </c>
+      <c r="J286" s="7"/>
+      <c r="K286" s="7"/>
+      <c r="L286" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change Globocan 0.0 value to avoid Nans
Changing Globocan 2012 15-19 observed incidence rate value from 0.0
to 0.1 to avoid division by zero resulting in Nan likelihood values.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -423,7 +423,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Incidence rates per 100,000 women come from Globocan 2012. Monisha Sharma emailed a connection to get age-specific rates. A single rate was given for ages 15-39, and I believe Monisha estimated the rates for ages &lt;39 by 5-year age groups. Assume a normal approximation of the Poisson distribution where </t>
+      <t xml:space="preserve">Incidence rates per 100,000 women come from Globocan 2012. Monisha Sharma emailed a connection to get age-specific rates. A single rate was given for ages 15-39, and I believe Monisha estimated the rates for ages &lt;39 by 5-year age groups. Changed 15-19 rate from 0.0 to 0.10 to avoid division by zero resulting in Nan likelihood values. Assume a normal approximation of the Poisson distribution where </t>
     </r>
     <r>
       <rPr>
@@ -899,9 +899,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X286"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M275" sqref="M275"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M277" sqref="M277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10842,7 +10842,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="274" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>70</v>
       </c>
@@ -10858,15 +10858,15 @@
       <c r="E274" s="1"/>
       <c r="F274" s="10"/>
       <c r="G274" s="34">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H274" s="33">
         <f>G274</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I274" s="7">
         <f>H274</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J274" s="7"/>
       <c r="K274" s="7"/>

</xml_diff>

<commit_message>
Calibrate to Globocan ages 15-39 incidence
Globocan 2012 provided an estimate of cervical cancer incidence for ages
15-39 combined. I believe Monisha estimated incidence disaggregated by
5-year age groups. However, I'm not sure this is the best shape.
Therefore, fitting to incidence for these ages combined.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B075D438-4463-4CC2-81AF-C216EA467F36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="120">
   <si>
     <t>N</t>
   </si>
@@ -445,11 +446,14 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>15-39 years</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
@@ -509,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -573,6 +577,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,28 +612,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M161" totalsRowShown="0">
-  <autoFilter ref="A1:M161"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M161" totalsRowShown="0">
+  <autoFilter ref="A1:M161" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Criteria"/>
-    <tableColumn id="9" name="Source"/>
-    <tableColumn id="2" name="Group"/>
-    <tableColumn id="7" name="Year"/>
-    <tableColumn id="10" name="Occurances"/>
-    <tableColumn id="3" name="N"/>
-    <tableColumn id="4" name="Prev/Inc Rate" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Criteria"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Source"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Group"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Year"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Occurances"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="N"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Prev/Inc Rate" dataDxfId="4">
       <calculatedColumnFormula>Table1[Occurances]/Table1[N]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Mean" dataDxfId="3">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Mean" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[Prev/Inc Rate]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Variance" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Variance" dataDxfId="2">
       <calculatedColumnFormula>(Table1[[#This Row],[Prev/Inc Rate]]*(1-Table1[[#This Row],[Prev/Inc Rate]]))/Table1[[#This Row],[N]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="LB" dataDxfId="1"/>
-    <tableColumn id="6" name="UB" dataDxfId="0"/>
-    <tableColumn id="8" name="Usage Status"/>
-    <tableColumn id="11" name="Comments"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="LB" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="UB" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Usage Status"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -896,12 +901,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X286"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X287"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M277" sqref="M277"/>
+      <selection pane="bottomLeft" activeCell="I279" sqref="I279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10871,7 +10876,7 @@
       <c r="J274" s="7"/>
       <c r="K274" s="7"/>
       <c r="L274" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="M274" s="14" t="s">
         <v>118</v>
@@ -10896,17 +10901,17 @@
         <v>2.646467153656904</v>
       </c>
       <c r="H275" s="33">
-        <f t="shared" ref="H275:H286" si="11">G275</f>
+        <f t="shared" ref="H275:H287" si="11">G275</f>
         <v>2.646467153656904</v>
       </c>
       <c r="I275" s="7">
-        <f t="shared" ref="I275:I286" si="12">H275</f>
+        <f t="shared" ref="I275:I287" si="12">H275</f>
         <v>2.646467153656904</v>
       </c>
       <c r="J275" s="7"/>
       <c r="K275" s="7"/>
       <c r="L275" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.25">
@@ -10938,7 +10943,7 @@
       <c r="J276" s="7"/>
       <c r="K276" s="7"/>
       <c r="L276" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.25">
@@ -10970,7 +10975,7 @@
       <c r="J277" s="7"/>
       <c r="K277" s="7"/>
       <c r="L277" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.25">
@@ -11002,34 +11007,34 @@
       <c r="J278" s="7"/>
       <c r="K278" s="7"/>
       <c r="L278" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="B279" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C279" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D279" s="1">
+      <c r="C279" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D279" s="12">
         <v>2012</v>
       </c>
       <c r="E279" s="12"/>
       <c r="F279" s="10"/>
       <c r="G279" s="32">
-        <v>63.4</v>
+        <v>21.9</v>
       </c>
       <c r="H279" s="33">
         <f t="shared" si="11"/>
-        <v>63.4</v>
+        <v>21.9</v>
       </c>
       <c r="I279" s="7">
         <f t="shared" si="12"/>
-        <v>63.4</v>
+        <v>21.9</v>
       </c>
       <c r="J279" s="7"/>
       <c r="K279" s="7"/>
@@ -11045,7 +11050,7 @@
         <v>117</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D280" s="1">
         <v>2012</v>
@@ -11053,15 +11058,15 @@
       <c r="E280" s="12"/>
       <c r="F280" s="10"/>
       <c r="G280" s="32">
-        <v>68.3</v>
+        <v>63.4</v>
       </c>
       <c r="H280" s="33">
         <f t="shared" si="11"/>
-        <v>68.3</v>
+        <v>63.4</v>
       </c>
       <c r="I280" s="7">
         <f t="shared" si="12"/>
-        <v>68.3</v>
+        <v>63.4</v>
       </c>
       <c r="J280" s="7"/>
       <c r="K280" s="7"/>
@@ -11077,7 +11082,7 @@
         <v>117</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D281" s="1">
         <v>2012</v>
@@ -11085,15 +11090,15 @@
       <c r="E281" s="12"/>
       <c r="F281" s="10"/>
       <c r="G281" s="32">
-        <v>70.7</v>
+        <v>68.3</v>
       </c>
       <c r="H281" s="33">
         <f t="shared" si="11"/>
-        <v>70.7</v>
+        <v>68.3</v>
       </c>
       <c r="I281" s="7">
         <f t="shared" si="12"/>
-        <v>70.7</v>
+        <v>68.3</v>
       </c>
       <c r="J281" s="7"/>
       <c r="K281" s="7"/>
@@ -11109,7 +11114,7 @@
         <v>117</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D282" s="1">
         <v>2012</v>
@@ -11117,15 +11122,15 @@
       <c r="E282" s="12"/>
       <c r="F282" s="10"/>
       <c r="G282" s="32">
-        <v>73</v>
+        <v>70.7</v>
       </c>
       <c r="H282" s="33">
         <f t="shared" si="11"/>
-        <v>73</v>
+        <v>70.7</v>
       </c>
       <c r="I282" s="7">
         <f t="shared" si="12"/>
-        <v>73</v>
+        <v>70.7</v>
       </c>
       <c r="J282" s="7"/>
       <c r="K282" s="7"/>
@@ -11141,7 +11146,7 @@
         <v>117</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="D283" s="1">
         <v>2012</v>
@@ -11149,15 +11154,15 @@
       <c r="E283" s="12"/>
       <c r="F283" s="10"/>
       <c r="G283" s="32">
-        <v>77.400000000000006</v>
+        <v>73</v>
       </c>
       <c r="H283" s="33">
         <f t="shared" si="11"/>
-        <v>77.400000000000006</v>
+        <v>73</v>
       </c>
       <c r="I283" s="7">
         <f t="shared" si="12"/>
-        <v>77.400000000000006</v>
+        <v>73</v>
       </c>
       <c r="J283" s="7"/>
       <c r="K283" s="7"/>
@@ -11172,8 +11177,8 @@
       <c r="B284" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C284" s="1" t="s">
-        <v>67</v>
+      <c r="C284" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D284" s="1">
         <v>2012</v>
@@ -11181,15 +11186,15 @@
       <c r="E284" s="12"/>
       <c r="F284" s="10"/>
       <c r="G284" s="32">
-        <v>82.7</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="H284" s="33">
         <f t="shared" si="11"/>
-        <v>82.7</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="I284" s="7">
         <f t="shared" si="12"/>
-        <v>82.7</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="J284" s="7"/>
       <c r="K284" s="7"/>
@@ -11205,7 +11210,7 @@
         <v>117</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D285" s="1">
         <v>2012</v>
@@ -11213,15 +11218,15 @@
       <c r="E285" s="12"/>
       <c r="F285" s="10"/>
       <c r="G285" s="32">
-        <v>88.6</v>
+        <v>82.7</v>
       </c>
       <c r="H285" s="33">
         <f t="shared" si="11"/>
-        <v>88.6</v>
+        <v>82.7</v>
       </c>
       <c r="I285" s="7">
         <f t="shared" si="12"/>
-        <v>88.6</v>
+        <v>82.7</v>
       </c>
       <c r="J285" s="7"/>
       <c r="K285" s="7"/>
@@ -11237,7 +11242,7 @@
         <v>117</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D286" s="1">
         <v>2012</v>
@@ -11245,19 +11250,51 @@
       <c r="E286" s="12"/>
       <c r="F286" s="10"/>
       <c r="G286" s="32">
-        <v>95.2</v>
+        <v>88.6</v>
       </c>
       <c r="H286" s="33">
         <f t="shared" si="11"/>
-        <v>95.2</v>
+        <v>88.6</v>
       </c>
       <c r="I286" s="7">
         <f t="shared" si="12"/>
-        <v>95.2</v>
+        <v>88.6</v>
       </c>
       <c r="J286" s="7"/>
       <c r="K286" s="7"/>
       <c r="L286" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D287" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E287" s="12"/>
+      <c r="F287" s="10"/>
+      <c r="G287" s="32">
+        <v>95.2</v>
+      </c>
+      <c r="H287" s="33">
+        <f t="shared" si="11"/>
+        <v>95.2</v>
+      </c>
+      <c r="I287" s="7">
+        <f t="shared" si="12"/>
+        <v>95.2</v>
+      </c>
+      <c r="J287" s="7"/>
+      <c r="K287" s="7"/>
+      <c r="L287" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add calibration to 2015 CIN1, CIN2, CIN3 prevalence
Add calibration to (Kuhn, 2020) 2015 CIN1, CIN2, CIN3 prevalence observed
data in women aged 30-65. Goal is for this to help raise CIN2/3 prevalence
and subsequent cervical cancer incidence. Update summed-log-likelihood
accordingly. Add plot of model outputs vs. observed data.

Modify CC incidence plot to show Globocan 2012 combined 15-39 incidence
now used for calibration.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B075D438-4463-4CC2-81AF-C216EA467F36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E4D072-CA80-4F1C-98C2-8940EB31AF88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="130">
   <si>
     <t>N</t>
   </si>
@@ -448,6 +448,36 @@
   </si>
   <si>
     <t>15-39 years</t>
+  </si>
+  <si>
+    <t>CIN1 Prevalence (HIV+)</t>
+  </si>
+  <si>
+    <t>CIN2 Prevalence (HIV+)</t>
+  </si>
+  <si>
+    <t>CIN3 Prevalence (HIV+)</t>
+  </si>
+  <si>
+    <t>Kuhn (2020) Lancet Glob Health. "Clinical evalulation of modifications to a human papillomavirus assay to optimise its utility for cervical cancer screening in low-resource settings: a diagnostic accuracy study"</t>
+  </si>
+  <si>
+    <t>30-65 years</t>
+  </si>
+  <si>
+    <t>CIN1 Prevalence (HIV-)</t>
+  </si>
+  <si>
+    <t>CIN2 Prevalence (HIV-)</t>
+  </si>
+  <si>
+    <t>CIN3 Prevalence (HIV-)</t>
+  </si>
+  <si>
+    <t>Kuhn (2020) Lancet Glob Health.</t>
+  </si>
+  <si>
+    <t>Data are from a cohort of women aged 30-65 recruited for screening from a primary care site from February 2015 to May 2016. Persons on ART were included as HIV-positive. Assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
   </si>
 </sst>
 </file>
@@ -902,11 +932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X287"/>
+  <dimension ref="A1:X293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I279" sqref="I279"/>
+      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11298,6 +11328,219 @@
         <v>58</v>
       </c>
     </row>
+    <row r="288" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>120</v>
+      </c>
+      <c r="B288" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C288" t="s">
+        <v>124</v>
+      </c>
+      <c r="D288">
+        <v>2015</v>
+      </c>
+      <c r="E288">
+        <v>45</v>
+      </c>
+      <c r="F288">
+        <v>333</v>
+      </c>
+      <c r="G288">
+        <f>E288/F288</f>
+        <v>0.13513513513513514</v>
+      </c>
+      <c r="H288">
+        <f>G288</f>
+        <v>0.13513513513513514</v>
+      </c>
+      <c r="I288">
+        <f>(H288*(1-H288))/F288</f>
+        <v>3.509718630244562E-4</v>
+      </c>
+      <c r="L288" t="s">
+        <v>58</v>
+      </c>
+      <c r="M288" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>121</v>
+      </c>
+      <c r="B289" t="s">
+        <v>128</v>
+      </c>
+      <c r="C289" t="s">
+        <v>124</v>
+      </c>
+      <c r="D289">
+        <v>2015</v>
+      </c>
+      <c r="E289">
+        <v>28</v>
+      </c>
+      <c r="F289">
+        <v>333</v>
+      </c>
+      <c r="G289">
+        <f t="shared" ref="G289:G293" si="13">E289/F289</f>
+        <v>8.408408408408409E-2</v>
+      </c>
+      <c r="H289">
+        <f t="shared" ref="H289:H293" si="14">G289</f>
+        <v>8.408408408408409E-2</v>
+      </c>
+      <c r="I289">
+        <f t="shared" ref="I289:I293" si="15">(H289*(1-H289))/F289</f>
+        <v>2.3127312578926357E-4</v>
+      </c>
+      <c r="L289" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>122</v>
+      </c>
+      <c r="B290" t="s">
+        <v>128</v>
+      </c>
+      <c r="C290" t="s">
+        <v>124</v>
+      </c>
+      <c r="D290">
+        <v>2015</v>
+      </c>
+      <c r="E290">
+        <v>23</v>
+      </c>
+      <c r="F290">
+        <v>333</v>
+      </c>
+      <c r="G290">
+        <f t="shared" si="13"/>
+        <v>6.9069069069069067E-2</v>
+      </c>
+      <c r="H290">
+        <f t="shared" si="14"/>
+        <v>6.9069069069069067E-2</v>
+      </c>
+      <c r="I290">
+        <f t="shared" si="15"/>
+        <v>1.930886869879917E-4</v>
+      </c>
+      <c r="L290" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>125</v>
+      </c>
+      <c r="B291" t="s">
+        <v>128</v>
+      </c>
+      <c r="C291" t="s">
+        <v>124</v>
+      </c>
+      <c r="D291">
+        <v>2015</v>
+      </c>
+      <c r="E291">
+        <v>28</v>
+      </c>
+      <c r="F291">
+        <v>382</v>
+      </c>
+      <c r="G291">
+        <f t="shared" si="13"/>
+        <v>7.3298429319371722E-2</v>
+      </c>
+      <c r="H291">
+        <f t="shared" si="14"/>
+        <v>7.3298429319371722E-2</v>
+      </c>
+      <c r="I291">
+        <f t="shared" si="15"/>
+        <v>1.7781615072954134E-4</v>
+      </c>
+      <c r="L291" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>126</v>
+      </c>
+      <c r="B292" t="s">
+        <v>128</v>
+      </c>
+      <c r="C292" t="s">
+        <v>124</v>
+      </c>
+      <c r="D292">
+        <v>2015</v>
+      </c>
+      <c r="E292">
+        <v>8</v>
+      </c>
+      <c r="F292">
+        <v>382</v>
+      </c>
+      <c r="G292">
+        <f t="shared" si="13"/>
+        <v>2.0942408376963352E-2</v>
+      </c>
+      <c r="H292">
+        <f t="shared" si="14"/>
+        <v>2.0942408376963352E-2</v>
+      </c>
+      <c r="I292">
+        <f t="shared" si="15"/>
+        <v>5.367493169721426E-5</v>
+      </c>
+      <c r="L292" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>127</v>
+      </c>
+      <c r="B293" t="s">
+        <v>128</v>
+      </c>
+      <c r="C293" t="s">
+        <v>124</v>
+      </c>
+      <c r="D293">
+        <v>2015</v>
+      </c>
+      <c r="E293">
+        <v>10</v>
+      </c>
+      <c r="F293">
+        <v>382</v>
+      </c>
+      <c r="G293">
+        <f t="shared" si="13"/>
+        <v>2.6178010471204188E-2</v>
+      </c>
+      <c r="H293">
+        <f t="shared" si="14"/>
+        <v>2.6178010471204188E-2</v>
+      </c>
+      <c r="I293">
+        <f t="shared" si="15"/>
+        <v>6.6734874971135369E-5</v>
+      </c>
+      <c r="L293" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Calibrate to Globocan ages 15-39 incidence"
This reverts commit 71f9aef671b8a241f1a6e9bb3ba72c497aabbbd8.

Kept Globocan 2012 15-39 cervical cancer incidence target in
Excel sheet. Therefore, with switch back to 5-year age group
targets needed to update sheet indices in loadUp2 accordingly.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E4D072-CA80-4F1C-98C2-8940EB31AF88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31AF21C-D13C-487C-BA59-0B3F7788080E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -935,8 +935,8 @@
   <dimension ref="A1:X293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M284" sqref="M284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10881,27 +10881,27 @@
       <c r="A274" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B274" s="1" t="s">
+      <c r="B274" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C274" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D274" s="1">
+      <c r="C274" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D274" s="12">
         <v>2012</v>
       </c>
-      <c r="E274" s="1"/>
+      <c r="E274" s="12"/>
       <c r="F274" s="10"/>
       <c r="G274" s="34">
-        <v>0.1</v>
+        <v>21.9</v>
       </c>
       <c r="H274" s="33">
         <f>G274</f>
-        <v>0.1</v>
+        <v>21.9</v>
       </c>
       <c r="I274" s="7">
         <f>H274</f>
-        <v>0.1</v>
+        <v>21.9</v>
       </c>
       <c r="J274" s="7"/>
       <c r="K274" s="7"/>
@@ -10920,29 +10920,30 @@
         <v>117</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D275" s="1">
         <v>2012</v>
       </c>
       <c r="E275" s="1"/>
       <c r="F275" s="10"/>
-      <c r="G275" s="32">
-        <v>2.646467153656904</v>
+      <c r="G275" s="34">
+        <v>0.1</v>
       </c>
       <c r="H275" s="33">
-        <f t="shared" ref="H275:H287" si="11">G275</f>
-        <v>2.646467153656904</v>
+        <f>G275</f>
+        <v>0.1</v>
       </c>
       <c r="I275" s="7">
-        <f t="shared" ref="I275:I287" si="12">H275</f>
-        <v>2.646467153656904</v>
+        <f>H275</f>
+        <v>0.1</v>
       </c>
       <c r="J275" s="7"/>
       <c r="K275" s="7"/>
       <c r="L275" t="s">
-        <v>0</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="M275" s="14"/>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
@@ -10952,7 +10953,7 @@
         <v>117</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D276" s="1">
         <v>2012</v>
@@ -10960,20 +10961,20 @@
       <c r="E276" s="1"/>
       <c r="F276" s="10"/>
       <c r="G276" s="32">
-        <v>8.848389035625793</v>
+        <v>2.646467153656904</v>
       </c>
       <c r="H276" s="33">
-        <f t="shared" si="11"/>
-        <v>8.848389035625793</v>
+        <f t="shared" ref="H276:H287" si="11">G276</f>
+        <v>2.646467153656904</v>
       </c>
       <c r="I276" s="7">
-        <f t="shared" si="12"/>
-        <v>8.848389035625793</v>
+        <f t="shared" ref="I276:I287" si="12">H276</f>
+        <v>2.646467153656904</v>
       </c>
       <c r="J276" s="7"/>
       <c r="K276" s="7"/>
       <c r="L276" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.25">
@@ -10984,28 +10985,28 @@
         <v>117</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D277" s="1">
         <v>2012</v>
       </c>
-      <c r="E277" s="12"/>
+      <c r="E277" s="1"/>
       <c r="F277" s="10"/>
       <c r="G277" s="32">
-        <v>45.193737900145855</v>
+        <v>8.848389035625793</v>
       </c>
       <c r="H277" s="33">
         <f t="shared" si="11"/>
-        <v>45.193737900145855</v>
+        <v>8.848389035625793</v>
       </c>
       <c r="I277" s="7">
         <f t="shared" si="12"/>
-        <v>45.193737900145855</v>
+        <v>8.848389035625793</v>
       </c>
       <c r="J277" s="7"/>
       <c r="K277" s="7"/>
       <c r="L277" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.25">
@@ -11016,7 +11017,7 @@
         <v>117</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D278" s="1">
         <v>2012</v>
@@ -11024,47 +11025,47 @@
       <c r="E278" s="12"/>
       <c r="F278" s="10"/>
       <c r="G278" s="32">
-        <v>53.40682333812245</v>
+        <v>45.193737900145855</v>
       </c>
       <c r="H278" s="33">
         <f t="shared" si="11"/>
-        <v>53.40682333812245</v>
+        <v>45.193737900145855</v>
       </c>
       <c r="I278" s="7">
         <f t="shared" si="12"/>
-        <v>53.40682333812245</v>
+        <v>45.193737900145855</v>
       </c>
       <c r="J278" s="7"/>
       <c r="K278" s="7"/>
       <c r="L278" t="s">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B279" s="12" t="s">
+      <c r="B279" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C279" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D279" s="12">
+      <c r="C279" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D279" s="1">
         <v>2012</v>
       </c>
       <c r="E279" s="12"/>
       <c r="F279" s="10"/>
       <c r="G279" s="32">
-        <v>21.9</v>
+        <v>53.40682333812245</v>
       </c>
       <c r="H279" s="33">
         <f t="shared" si="11"/>
-        <v>21.9</v>
+        <v>53.40682333812245</v>
       </c>
       <c r="I279" s="7">
         <f t="shared" si="12"/>
-        <v>21.9</v>
+        <v>53.40682333812245</v>
       </c>
       <c r="J279" s="7"/>
       <c r="K279" s="7"/>

</xml_diff>

<commit_message>
Increase estimated Globocan aged 15-19 incidence target
Globocan 2012 provided an estimate of cervical cancer incidence for
ages 15-39 combined. I believe Monisha estimated incidence
disaggregated by 5-year age groups. I originally changed estimated
incidence in the 15-19 age group from 0.0 to 0.01 to avoid division
by 0 issues. Now changing incidence in this age group to 1.0 to make
estimated variance in the likelihood more similar to that of the other
age groups.
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31AF21C-D13C-487C-BA59-0B3F7788080E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C2CEB1-3C3B-48FB-A4EC-AA378E9A3F61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,8 +423,41 @@
     <t>Globocan 2012</t>
   </si>
   <si>
+    <t>15-39 years</t>
+  </si>
+  <si>
+    <t>CIN1 Prevalence (HIV+)</t>
+  </si>
+  <si>
+    <t>CIN2 Prevalence (HIV+)</t>
+  </si>
+  <si>
+    <t>CIN3 Prevalence (HIV+)</t>
+  </si>
+  <si>
+    <t>Kuhn (2020) Lancet Glob Health. "Clinical evalulation of modifications to a human papillomavirus assay to optimise its utility for cervical cancer screening in low-resource settings: a diagnostic accuracy study"</t>
+  </si>
+  <si>
+    <t>30-65 years</t>
+  </si>
+  <si>
+    <t>CIN1 Prevalence (HIV-)</t>
+  </si>
+  <si>
+    <t>CIN2 Prevalence (HIV-)</t>
+  </si>
+  <si>
+    <t>CIN3 Prevalence (HIV-)</t>
+  </si>
+  <si>
+    <t>Kuhn (2020) Lancet Glob Health.</t>
+  </si>
+  <si>
+    <t>Data are from a cohort of women aged 30-65 recruited for screening from a primary care site from February 2015 to May 2016. Persons on ART were included as HIV-positive. Assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Incidence rates per 100,000 women come from Globocan 2012. Monisha Sharma emailed a connection to get age-specific rates. A single rate was given for ages 15-39, and I believe Monisha estimated the rates for ages &lt;39 by 5-year age groups. Changed 15-19 rate from 0.0 to 0.10 to avoid division by zero resulting in Nan likelihood values. Assume a normal approximation of the Poisson distribution where </t>
+      <t xml:space="preserve">Incidence rates per 100,000 women come from Globocan 2012. Monisha Sharma emailed a connection to get age-specific rates. A single rate was given for ages 15-39, and I believe Monisha estimated the rates for ages &lt;39 by 5-year age groups. Changed 15-19 rate from 0.0 to 1.0 to avoid division by zero resulting in Nan likelihood values. Assume a normal approximation of the Poisson distribution where </t>
     </r>
     <r>
       <rPr>
@@ -445,39 +478,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>15-39 years</t>
-  </si>
-  <si>
-    <t>CIN1 Prevalence (HIV+)</t>
-  </si>
-  <si>
-    <t>CIN2 Prevalence (HIV+)</t>
-  </si>
-  <si>
-    <t>CIN3 Prevalence (HIV+)</t>
-  </si>
-  <si>
-    <t>Kuhn (2020) Lancet Glob Health. "Clinical evalulation of modifications to a human papillomavirus assay to optimise its utility for cervical cancer screening in low-resource settings: a diagnostic accuracy study"</t>
-  </si>
-  <si>
-    <t>30-65 years</t>
-  </si>
-  <si>
-    <t>CIN1 Prevalence (HIV-)</t>
-  </si>
-  <si>
-    <t>CIN2 Prevalence (HIV-)</t>
-  </si>
-  <si>
-    <t>CIN3 Prevalence (HIV-)</t>
-  </si>
-  <si>
-    <t>Kuhn (2020) Lancet Glob Health.</t>
-  </si>
-  <si>
-    <t>Data are from a cohort of women aged 30-65 recruited for screening from a primary care site from February 2015 to May 2016. Persons on ART were included as HIV-positive. Assuming a normal approximation of the binomial distribution where µ=prevalence proportion (p) and variance=(p(1-p))/n.</t>
   </si>
 </sst>
 </file>
@@ -936,7 +936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M284" sqref="M284"/>
+      <selection pane="bottomLeft" activeCell="M281" sqref="M281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10885,7 +10885,7 @@
         <v>117</v>
       </c>
       <c r="C274" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D274" s="12">
         <v>2012</v>
@@ -10909,7 +10909,7 @@
         <v>0</v>
       </c>
       <c r="M274" s="14" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.25">
@@ -10928,15 +10928,15 @@
       <c r="E275" s="1"/>
       <c r="F275" s="10"/>
       <c r="G275" s="34">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H275" s="33">
         <f>G275</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I275" s="7">
         <f>H275</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J275" s="7"/>
       <c r="K275" s="7"/>
@@ -11331,13 +11331,13 @@
     </row>
     <row r="288" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B288" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C288" t="s">
         <v>123</v>
-      </c>
-      <c r="C288" t="s">
-        <v>124</v>
       </c>
       <c r="D288">
         <v>2015</v>
@@ -11364,18 +11364,18 @@
         <v>58</v>
       </c>
       <c r="M288" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B289" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C289" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D289">
         <v>2015</v>
@@ -11404,13 +11404,13 @@
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B290" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C290" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D290">
         <v>2015</v>
@@ -11439,13 +11439,13 @@
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B291" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C291" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D291">
         <v>2015</v>
@@ -11474,13 +11474,13 @@
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B292" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C292" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D292">
         <v>2015</v>
@@ -11509,13 +11509,13 @@
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
+        <v>126</v>
+      </c>
+      <c r="B293" t="s">
         <v>127</v>
       </c>
-      <c r="B293" t="s">
-        <v>128</v>
-      </c>
       <c r="C293" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D293">
         <v>2015</v>

</xml_diff>

<commit_message>
Calibrate to Globocan 2018 CC inc by age
-Stop calibrating to Globocan 2012 cervical cancer incidence data by age
and remove variance adjustment in older ages accordingly
-Switch to calibrating to Globocan 2018 cervical cancer incidence data
by age
-Load and save Globocan 2018 data
</commit_message>
<xml_diff>
--- a/Config/Calibration_targets.xlsx
+++ b/Config/Calibration_targets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C2CEB1-3C3B-48FB-A4EC-AA378E9A3F61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D2BAB3-1CCF-459A-B2DA-6AACB4B17BDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="132">
   <si>
     <t>N</t>
   </si>
@@ -479,16 +479,44 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>Globocan 2018</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Incidence rates per 100,000 women come from Globocan 2018 from Minttu. Assume a normal approximation of the Poisson distribution where </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ=λ and variance=λ  and λ=CC incidence rate per year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,6 +550,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -540,10 +582,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -608,9 +652,20 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -932,11 +987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X293"/>
+  <dimension ref="A1:X310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M281" sqref="M281"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E310" sqref="E310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10941,7 +10996,7 @@
       <c r="J275" s="7"/>
       <c r="K275" s="7"/>
       <c r="L275" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="M275" s="14"/>
     </row>
@@ -10974,7 +11029,7 @@
       <c r="J276" s="7"/>
       <c r="K276" s="7"/>
       <c r="L276" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.25">
@@ -11006,7 +11061,7 @@
       <c r="J277" s="7"/>
       <c r="K277" s="7"/>
       <c r="L277" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.25">
@@ -11038,7 +11093,7 @@
       <c r="J278" s="7"/>
       <c r="K278" s="7"/>
       <c r="L278" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.25">
@@ -11070,7 +11125,7 @@
       <c r="J279" s="7"/>
       <c r="K279" s="7"/>
       <c r="L279" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:13" x14ac:dyDescent="0.25">
@@ -11102,7 +11157,7 @@
       <c r="J280" s="7"/>
       <c r="K280" s="7"/>
       <c r="L280" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.25">
@@ -11134,7 +11189,7 @@
       <c r="J281" s="7"/>
       <c r="K281" s="7"/>
       <c r="L281" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.25">
@@ -11166,7 +11221,7 @@
       <c r="J282" s="7"/>
       <c r="K282" s="7"/>
       <c r="L282" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.25">
@@ -11198,7 +11253,7 @@
       <c r="J283" s="7"/>
       <c r="K283" s="7"/>
       <c r="L283" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.25">
@@ -11230,7 +11285,7 @@
       <c r="J284" s="7"/>
       <c r="K284" s="7"/>
       <c r="L284" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.25">
@@ -11262,7 +11317,7 @@
       <c r="J285" s="7"/>
       <c r="K285" s="7"/>
       <c r="L285" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.25">
@@ -11294,7 +11349,7 @@
       <c r="J286" s="7"/>
       <c r="K286" s="7"/>
       <c r="L286" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.25">
@@ -11326,7 +11381,7 @@
       <c r="J287" s="7"/>
       <c r="K287" s="7"/>
       <c r="L287" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -11367,7 +11422,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>120</v>
       </c>
@@ -11402,7 +11457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>121</v>
       </c>
@@ -11437,7 +11492,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>124</v>
       </c>
@@ -11472,7 +11527,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>125</v>
       </c>
@@ -11507,7 +11562,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>126</v>
       </c>
@@ -11541,6 +11596,421 @@
       <c r="L293" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="294" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B294" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D294" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E294" s="1"/>
+      <c r="F294" s="10"/>
+      <c r="G294" s="37">
+        <v>3.9070527772503256</v>
+      </c>
+      <c r="H294" s="33">
+        <f>G294</f>
+        <v>3.9070527772503256</v>
+      </c>
+      <c r="I294" s="7">
+        <f>H294</f>
+        <v>3.9070527772503256</v>
+      </c>
+      <c r="J294" s="7"/>
+      <c r="K294" s="7"/>
+      <c r="L294" t="s">
+        <v>58</v>
+      </c>
+      <c r="M294" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B295" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D295" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E295" s="1"/>
+      <c r="F295" s="10"/>
+      <c r="G295" s="37">
+        <v>19.718592555074853</v>
+      </c>
+      <c r="H295" s="33">
+        <f t="shared" ref="H295:H305" si="16">G295</f>
+        <v>19.718592555074853</v>
+      </c>
+      <c r="I295" s="7">
+        <f t="shared" ref="I295:I305" si="17">H295</f>
+        <v>19.718592555074853</v>
+      </c>
+      <c r="J295" s="7"/>
+      <c r="K295" s="7"/>
+      <c r="L295" t="s">
+        <v>58</v>
+      </c>
+      <c r="M295" s="14"/>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B296" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D296" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E296" s="1"/>
+      <c r="F296" s="10"/>
+      <c r="G296" s="37">
+        <v>35.815396540774046</v>
+      </c>
+      <c r="H296" s="33">
+        <f t="shared" si="16"/>
+        <v>35.815396540774046</v>
+      </c>
+      <c r="I296" s="7">
+        <f t="shared" si="17"/>
+        <v>35.815396540774046</v>
+      </c>
+      <c r="J296" s="7"/>
+      <c r="K296" s="7"/>
+      <c r="L296" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B297" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D297" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E297" s="12"/>
+      <c r="F297" s="10"/>
+      <c r="G297" s="37">
+        <v>53.753954608683522</v>
+      </c>
+      <c r="H297" s="33">
+        <f t="shared" si="16"/>
+        <v>53.753954608683522</v>
+      </c>
+      <c r="I297" s="7">
+        <f t="shared" si="17"/>
+        <v>53.753954608683522</v>
+      </c>
+      <c r="J297" s="7"/>
+      <c r="K297" s="7"/>
+      <c r="L297" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B298" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D298" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E298" s="12"/>
+      <c r="F298" s="10"/>
+      <c r="G298" s="37">
+        <v>71.181262777416052</v>
+      </c>
+      <c r="H298" s="33">
+        <f t="shared" si="16"/>
+        <v>71.181262777416052</v>
+      </c>
+      <c r="I298" s="7">
+        <f t="shared" si="17"/>
+        <v>71.181262777416052</v>
+      </c>
+      <c r="J298" s="7"/>
+      <c r="K298" s="7"/>
+      <c r="L298" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B299" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D299" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E299" s="12"/>
+      <c r="F299" s="10"/>
+      <c r="G299" s="37">
+        <v>85.090519192952186</v>
+      </c>
+      <c r="H299" s="33">
+        <f t="shared" si="16"/>
+        <v>85.090519192952186</v>
+      </c>
+      <c r="I299" s="7">
+        <f t="shared" si="17"/>
+        <v>85.090519192952186</v>
+      </c>
+      <c r="J299" s="7"/>
+      <c r="K299" s="7"/>
+      <c r="L299" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B300" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D300" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E300" s="12"/>
+      <c r="F300" s="10"/>
+      <c r="G300" s="37">
+        <v>95.443618498222065</v>
+      </c>
+      <c r="H300" s="33">
+        <f t="shared" si="16"/>
+        <v>95.443618498222065</v>
+      </c>
+      <c r="I300" s="7">
+        <f t="shared" si="17"/>
+        <v>95.443618498222065</v>
+      </c>
+      <c r="J300" s="7"/>
+      <c r="K300" s="7"/>
+      <c r="L300" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B301" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D301" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E301" s="12"/>
+      <c r="F301" s="10"/>
+      <c r="G301" s="37">
+        <v>96.099524161750054</v>
+      </c>
+      <c r="H301" s="33">
+        <f t="shared" si="16"/>
+        <v>96.099524161750054</v>
+      </c>
+      <c r="I301" s="7">
+        <f t="shared" si="17"/>
+        <v>96.099524161750054</v>
+      </c>
+      <c r="J301" s="7"/>
+      <c r="K301" s="7"/>
+      <c r="L301" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B302" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D302" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E302" s="12"/>
+      <c r="F302" s="10"/>
+      <c r="G302" s="37">
+        <v>94.851577973825016</v>
+      </c>
+      <c r="H302" s="33">
+        <f t="shared" si="16"/>
+        <v>94.851577973825016</v>
+      </c>
+      <c r="I302" s="7">
+        <f t="shared" si="17"/>
+        <v>94.851577973825016</v>
+      </c>
+      <c r="J302" s="7"/>
+      <c r="K302" s="7"/>
+      <c r="L302" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B303" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D303" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E303" s="12"/>
+      <c r="F303" s="10"/>
+      <c r="G303" s="37">
+        <v>97.48752644071628</v>
+      </c>
+      <c r="H303" s="33">
+        <f t="shared" si="16"/>
+        <v>97.48752644071628</v>
+      </c>
+      <c r="I303" s="7">
+        <f t="shared" si="17"/>
+        <v>97.48752644071628</v>
+      </c>
+      <c r="J303" s="7"/>
+      <c r="K303" s="7"/>
+      <c r="L303" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B304" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D304" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E304" s="12"/>
+      <c r="F304" s="10"/>
+      <c r="G304" s="37">
+        <v>101.98823806664386</v>
+      </c>
+      <c r="H304" s="33">
+        <f t="shared" si="16"/>
+        <v>101.98823806664386</v>
+      </c>
+      <c r="I304" s="7">
+        <f t="shared" si="17"/>
+        <v>101.98823806664386</v>
+      </c>
+      <c r="J304" s="7"/>
+      <c r="K304" s="7"/>
+      <c r="L304" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B305" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D305" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E305" s="12"/>
+      <c r="F305" s="10"/>
+      <c r="G305" s="37">
+        <v>110.42515650113373</v>
+      </c>
+      <c r="H305" s="33">
+        <f t="shared" si="16"/>
+        <v>110.42515650113373</v>
+      </c>
+      <c r="I305" s="7">
+        <f t="shared" si="17"/>
+        <v>110.42515650113373</v>
+      </c>
+      <c r="J305" s="7"/>
+      <c r="K305" s="7"/>
+      <c r="L305" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A306" s="1"/>
+      <c r="B306" s="12"/>
+      <c r="C306" s="1"/>
+      <c r="D306" s="1"/>
+      <c r="E306" s="12"/>
+      <c r="F306" s="10"/>
+      <c r="G306" s="38"/>
+      <c r="H306" s="33"/>
+      <c r="I306" s="7"/>
+      <c r="J306" s="7"/>
+      <c r="K306" s="7"/>
+    </row>
+    <row r="310" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C310" s="36"/>
+      <c r="D310" s="36"/>
+      <c r="E310" s="36"/>
+      <c r="F310" s="36"/>
+      <c r="G310" s="36"/>
+      <c r="H310" s="36"/>
+      <c r="I310" s="36"/>
+      <c r="J310" s="36"/>
+      <c r="K310" s="36"/>
+      <c r="L310" s="36"/>
+      <c r="M310" s="36"/>
+      <c r="N310" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>